<commit_message>
江南百草园 8个席克氏 老品种编号清单 Signed-off-by: twtcom001 <twtcom001@sina.com>
</commit_message>
<xml_diff>
--- a/统计清单/2017国内编号清单.xlsx
+++ b/统计清单/2017国内编号清单.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\git\fall\统计清单\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\fall\统计清单\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1851" uniqueCount="960">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1908" uniqueCount="962">
   <si>
     <t>本地编号</t>
   </si>
@@ -3354,10 +3354,6 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>引进尺寸</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
     <t>引进尺寸2</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
@@ -3575,6 +3571,17 @@
   </si>
   <si>
     <t>Echinocereus reichenbachii - v bergamannii</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>引进价格</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Echinopsis</t>
+  </si>
+  <si>
+    <t>Echinopsis</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -3811,7 +3818,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3920,12 +3927,204 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
-  <dxfs count="19">
+  <dxfs count="18">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="10"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="4"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -4125,224 +4324,6 @@
         <horizontal/>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="10"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="4"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
@@ -4357,19 +4338,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:L178" totalsRowShown="0">
-  <autoFilter ref="A1:L178"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:L186" totalsRowShown="0">
+  <autoFilter ref="A1:L186"/>
   <tableColumns count="12">
     <tableColumn id="1" name="145"/>
     <tableColumn id="2" name="属"/>
-    <tableColumn id="3" name="属内编号" dataDxfId="18"/>
-    <tableColumn id="4" name="拉丁名" dataDxfId="17"/>
-    <tableColumn id="5" name="中文" dataDxfId="16"/>
-    <tableColumn id="7" name="来源编号" dataDxfId="15"/>
-    <tableColumn id="6" name="来源" dataDxfId="14"/>
-    <tableColumn id="8" name="参考链接" dataDxfId="13" dataCellStyle="超链接"/>
-    <tableColumn id="9" name="引进尺寸" dataDxfId="12"/>
-    <tableColumn id="10" name="引进尺寸2" dataDxfId="11"/>
+    <tableColumn id="3" name="属内编号" dataDxfId="6"/>
+    <tableColumn id="4" name="拉丁名" dataDxfId="5"/>
+    <tableColumn id="5" name="中文" dataDxfId="4"/>
+    <tableColumn id="7" name="来源编号" dataDxfId="3"/>
+    <tableColumn id="12" name="引进价格"/>
+    <tableColumn id="6" name="来源" dataDxfId="2"/>
+    <tableColumn id="8" name="参考链接" dataDxfId="1" dataCellStyle="超链接"/>
+    <tableColumn id="10" name="引进尺寸2" dataDxfId="0"/>
     <tableColumn id="11" name="引进日期"/>
     <tableColumn id="13" name="备注"/>
   </tableColumns>
@@ -4382,9 +4363,9 @@
   <autoFilter ref="A1:E162"/>
   <tableColumns count="5">
     <tableColumn id="1" name="145"/>
-    <tableColumn id="3" name="编号" dataDxfId="10"/>
-    <tableColumn id="5" name="中文" dataDxfId="9"/>
-    <tableColumn id="7" name="来源编号" dataDxfId="8"/>
+    <tableColumn id="3" name="编号" dataDxfId="17"/>
+    <tableColumn id="5" name="中文" dataDxfId="16"/>
+    <tableColumn id="7" name="来源编号" dataDxfId="15"/>
     <tableColumn id="2" name="数量"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -4392,20 +4373,20 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A1:G129" totalsRowShown="0" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A1:G129" totalsRowShown="0" dataDxfId="14">
   <autoFilter ref="A1:G129">
     <filterColumn colId="6">
       <filters blank="1"/>
     </filterColumn>
   </autoFilter>
   <tableColumns count="7">
-    <tableColumn id="1" name="本地编号" dataDxfId="6"/>
-    <tableColumn id="2" name="编号" dataDxfId="5"/>
-    <tableColumn id="5" name="中文名" dataDxfId="4"/>
-    <tableColumn id="6" name="购买目标" dataDxfId="3"/>
-    <tableColumn id="7" name="来源编号" dataDxfId="2"/>
-    <tableColumn id="4" name="链接" dataDxfId="1"/>
-    <tableColumn id="3" name="购买数量" dataDxfId="0"/>
+    <tableColumn id="1" name="本地编号" dataDxfId="13"/>
+    <tableColumn id="2" name="编号" dataDxfId="12"/>
+    <tableColumn id="5" name="中文名" dataDxfId="11"/>
+    <tableColumn id="6" name="购买目标" dataDxfId="10"/>
+    <tableColumn id="7" name="来源编号" dataDxfId="9"/>
+    <tableColumn id="4" name="链接" dataDxfId="8"/>
+    <tableColumn id="3" name="购买数量" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4698,10 +4679,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L178"/>
+  <dimension ref="A1:L186"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
-      <selection activeCell="D175" sqref="D175:D176"/>
+    <sheetView tabSelected="1" topLeftCell="C172" workbookViewId="0">
+      <selection activeCell="H179" sqref="H179:H186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -4711,12 +4692,13 @@
     <col min="4" max="4" width="64.125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="26.125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.25" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="47.125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12" customWidth="1"/>
-    <col min="10" max="10" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.75" customWidth="1"/>
+    <col min="8" max="8" width="16.25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="47.125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" customWidth="1"/>
+    <col min="11" max="11" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -4739,16 +4721,16 @@
         <v>738</v>
       </c>
       <c r="G1" s="14" t="s">
+        <v>959</v>
+      </c>
+      <c r="H1" s="14" t="s">
         <v>737</v>
       </c>
-      <c r="H1" s="65" t="s">
+      <c r="I1" s="65" t="s">
         <v>739</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="J1" s="14" t="s">
         <v>904</v>
-      </c>
-      <c r="J1" s="14" t="s">
-        <v>905</v>
       </c>
       <c r="K1" s="27" t="s">
         <v>902</v>
@@ -4774,14 +4756,14 @@
         <v>330</v>
       </c>
       <c r="F2" s="40"/>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="9">
+        <v>15</v>
+      </c>
+      <c r="H2" s="14" t="s">
         <v>337</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="I2" s="11" t="s">
         <v>339</v>
-      </c>
-      <c r="I2" s="9">
-        <v>15</v>
       </c>
       <c r="J2" s="14" t="s">
         <v>355</v>
@@ -4807,14 +4789,14 @@
         <v>468</v>
       </c>
       <c r="F3" s="40"/>
-      <c r="G3" s="14" t="s">
+      <c r="G3" s="9">
+        <v>30</v>
+      </c>
+      <c r="H3" s="14" t="s">
         <v>482</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="I3" s="11" t="s">
         <v>469</v>
-      </c>
-      <c r="I3" s="9">
-        <v>30</v>
       </c>
       <c r="J3" s="14" t="s">
         <v>357</v>
@@ -4840,14 +4822,14 @@
         <v>415</v>
       </c>
       <c r="F4" s="40"/>
-      <c r="G4" s="14" t="s">
+      <c r="G4" s="9">
+        <v>30</v>
+      </c>
+      <c r="H4" s="14" t="s">
         <v>482</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="I4" s="11" t="s">
         <v>481</v>
-      </c>
-      <c r="I4" s="9">
-        <v>30</v>
       </c>
       <c r="J4" s="14" t="s">
         <v>357</v>
@@ -4875,14 +4857,14 @@
       <c r="F5" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G5" s="9">
+        <v>30</v>
+      </c>
+      <c r="H5" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="H5" s="11" t="s">
+      <c r="I5" s="11" t="s">
         <v>5</v>
-      </c>
-      <c r="I5" s="9">
-        <v>30</v>
       </c>
       <c r="J5" s="9" t="s">
         <v>2</v>
@@ -4910,14 +4892,14 @@
       <c r="F6" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="G6" s="9">
+        <v>30</v>
+      </c>
+      <c r="H6" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="I6" s="11" t="s">
         <v>8</v>
-      </c>
-      <c r="I6" s="9">
-        <v>30</v>
       </c>
       <c r="J6" s="9" t="s">
         <v>2</v>
@@ -4945,14 +4927,14 @@
       <c r="F7" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="G7" s="9">
+        <v>30</v>
+      </c>
+      <c r="H7" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="H7" s="11" t="s">
+      <c r="I7" s="11" t="s">
         <v>11</v>
-      </c>
-      <c r="I7" s="9">
-        <v>30</v>
       </c>
       <c r="J7" s="9" t="s">
         <v>2</v>
@@ -4980,14 +4962,14 @@
       <c r="F8" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="G8" s="9">
+        <v>30</v>
+      </c>
+      <c r="H8" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="H8" s="11" t="s">
+      <c r="I8" s="11" t="s">
         <v>14</v>
-      </c>
-      <c r="I8" s="9">
-        <v>30</v>
       </c>
       <c r="J8" s="9" t="s">
         <v>2</v>
@@ -5015,14 +4997,14 @@
       <c r="F9" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="G9" s="9" t="s">
+      <c r="G9" s="9">
+        <v>30</v>
+      </c>
+      <c r="H9" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="H9" s="11" t="s">
+      <c r="I9" s="11" t="s">
         <v>17</v>
-      </c>
-      <c r="I9" s="9">
-        <v>30</v>
       </c>
       <c r="J9" s="9" t="s">
         <v>2</v>
@@ -5050,14 +5032,14 @@
       <c r="F10" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="G10" s="9" t="s">
+      <c r="G10" s="9">
+        <v>30</v>
+      </c>
+      <c r="H10" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="H10" s="11" t="s">
+      <c r="I10" s="11" t="s">
         <v>20</v>
-      </c>
-      <c r="I10" s="9">
-        <v>30</v>
       </c>
       <c r="J10" s="9" t="s">
         <v>2</v>
@@ -5085,11 +5067,11 @@
       <c r="F11" s="44" t="s">
         <v>629</v>
       </c>
-      <c r="G11" s="23" t="s">
+      <c r="G11" s="9"/>
+      <c r="H11" s="23" t="s">
         <v>590</v>
       </c>
-      <c r="H11" s="11"/>
-      <c r="I11" s="9"/>
+      <c r="I11" s="11"/>
       <c r="J11" s="14"/>
       <c r="K11" s="10">
         <v>42941</v>
@@ -5114,11 +5096,11 @@
       <c r="F12" s="44" t="s">
         <v>615</v>
       </c>
-      <c r="G12" s="20" t="s">
+      <c r="G12" s="9"/>
+      <c r="H12" s="20" t="s">
         <v>590</v>
       </c>
-      <c r="H12" s="11"/>
-      <c r="I12" s="9"/>
+      <c r="I12" s="11"/>
       <c r="J12" s="14"/>
       <c r="K12" s="10">
         <v>42941</v>
@@ -5141,14 +5123,14 @@
         <v>429</v>
       </c>
       <c r="F13" s="40"/>
-      <c r="G13" s="14" t="s">
+      <c r="G13" s="9">
+        <v>30</v>
+      </c>
+      <c r="H13" s="14" t="s">
         <v>482</v>
       </c>
-      <c r="H13" s="11" t="s">
+      <c r="I13" s="11" t="s">
         <v>430</v>
-      </c>
-      <c r="I13" s="9">
-        <v>30</v>
       </c>
       <c r="J13" s="14" t="s">
         <v>357</v>
@@ -5174,14 +5156,14 @@
         <v>437</v>
       </c>
       <c r="F14" s="40"/>
-      <c r="G14" s="14" t="s">
+      <c r="G14" s="9">
+        <v>30</v>
+      </c>
+      <c r="H14" s="14" t="s">
         <v>482</v>
       </c>
-      <c r="H14" s="11" t="s">
+      <c r="I14" s="11" t="s">
         <v>438</v>
-      </c>
-      <c r="I14" s="9">
-        <v>30</v>
       </c>
       <c r="J14" s="14" t="s">
         <v>357</v>
@@ -5207,14 +5189,14 @@
         <v>411</v>
       </c>
       <c r="F15" s="40"/>
-      <c r="G15" s="14" t="s">
+      <c r="G15" s="9">
+        <v>30</v>
+      </c>
+      <c r="H15" s="14" t="s">
         <v>482</v>
       </c>
-      <c r="H15" s="11" t="s">
+      <c r="I15" s="11" t="s">
         <v>412</v>
-      </c>
-      <c r="I15" s="9">
-        <v>30</v>
       </c>
       <c r="J15" s="14" t="s">
         <v>357</v>
@@ -5242,14 +5224,14 @@
       <c r="F16" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="G16" s="9" t="s">
+      <c r="G16" s="9">
+        <v>30</v>
+      </c>
+      <c r="H16" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="H16" s="11" t="s">
+      <c r="I16" s="11" t="s">
         <v>25</v>
-      </c>
-      <c r="I16" s="9">
-        <v>30</v>
       </c>
       <c r="J16" s="9" t="s">
         <v>2</v>
@@ -5275,14 +5257,14 @@
         <v>361</v>
       </c>
       <c r="F17" s="40"/>
-      <c r="G17" s="14" t="s">
+      <c r="G17" s="9">
+        <v>30</v>
+      </c>
+      <c r="H17" s="14" t="s">
         <v>482</v>
       </c>
-      <c r="H17" s="11" t="s">
+      <c r="I17" s="11" t="s">
         <v>362</v>
-      </c>
-      <c r="I17" s="9">
-        <v>30</v>
       </c>
       <c r="J17" s="14" t="s">
         <v>357</v>
@@ -5308,14 +5290,14 @@
         <v>449</v>
       </c>
       <c r="F18" s="40"/>
-      <c r="G18" s="14" t="s">
+      <c r="G18" s="9">
+        <v>30</v>
+      </c>
+      <c r="H18" s="14" t="s">
         <v>482</v>
       </c>
-      <c r="H18" s="11" t="s">
+      <c r="I18" s="11" t="s">
         <v>450</v>
-      </c>
-      <c r="I18" s="9">
-        <v>30</v>
       </c>
       <c r="J18" s="14" t="s">
         <v>357</v>
@@ -5343,11 +5325,11 @@
       <c r="F19" s="44" t="s">
         <v>623</v>
       </c>
-      <c r="G19" s="20" t="s">
+      <c r="G19" s="9"/>
+      <c r="H19" s="20" t="s">
         <v>590</v>
       </c>
-      <c r="H19" s="11"/>
-      <c r="I19" s="9"/>
+      <c r="I19" s="11"/>
       <c r="J19" s="14"/>
       <c r="K19" s="10">
         <v>42941</v>
@@ -5370,14 +5352,14 @@
         <v>413</v>
       </c>
       <c r="F20" s="40"/>
-      <c r="G20" s="14" t="s">
+      <c r="G20" s="9">
+        <v>30</v>
+      </c>
+      <c r="H20" s="14" t="s">
         <v>482</v>
       </c>
-      <c r="H20" s="11" t="s">
+      <c r="I20" s="11" t="s">
         <v>414</v>
-      </c>
-      <c r="I20" s="9">
-        <v>30</v>
       </c>
       <c r="J20" s="14" t="s">
         <v>357</v>
@@ -5403,13 +5385,13 @@
         <v>484</v>
       </c>
       <c r="F21" s="40"/>
-      <c r="G21" s="14" t="s">
+      <c r="G21" s="9"/>
+      <c r="H21" s="14" t="s">
         <v>492</v>
       </c>
-      <c r="H21" s="11" t="s">
+      <c r="I21" s="11" t="s">
         <v>483</v>
       </c>
-      <c r="I21" s="9"/>
       <c r="J21" s="9"/>
       <c r="K21" s="10">
         <v>42912</v>
@@ -5434,11 +5416,11 @@
       <c r="F22" s="44" t="s">
         <v>644</v>
       </c>
-      <c r="G22" s="20" t="s">
+      <c r="G22" s="9"/>
+      <c r="H22" s="20" t="s">
         <v>590</v>
       </c>
-      <c r="H22" s="11"/>
-      <c r="I22" s="9"/>
+      <c r="I22" s="11"/>
       <c r="J22" s="14"/>
       <c r="K22" s="10">
         <v>42941</v>
@@ -5463,13 +5445,13 @@
       <c r="F23" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="G23" s="9" t="s">
+      <c r="G23" s="9">
+        <v>30</v>
+      </c>
+      <c r="H23" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="H23" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="I23" s="9">
+      <c r="I23" s="11" t="s">
         <v>30</v>
       </c>
       <c r="J23" s="9" t="s">
@@ -5496,14 +5478,14 @@
         <v>456</v>
       </c>
       <c r="F24" s="40"/>
-      <c r="G24" s="14" t="s">
+      <c r="G24" s="9">
+        <v>30</v>
+      </c>
+      <c r="H24" s="14" t="s">
         <v>482</v>
       </c>
-      <c r="H24" s="11" t="s">
+      <c r="I24" s="11" t="s">
         <v>455</v>
-      </c>
-      <c r="I24" s="9">
-        <v>30</v>
       </c>
       <c r="J24" s="14" t="s">
         <v>357</v>
@@ -5531,11 +5513,11 @@
       <c r="F25" s="44" t="s">
         <v>631</v>
       </c>
-      <c r="G25" s="20" t="s">
+      <c r="G25" s="9"/>
+      <c r="H25" s="20" t="s">
         <v>590</v>
       </c>
-      <c r="H25" s="11"/>
-      <c r="I25" s="9"/>
+      <c r="I25" s="11"/>
       <c r="J25" s="14"/>
       <c r="K25" s="10">
         <v>42941</v>
@@ -5560,11 +5542,11 @@
       <c r="F26" s="44" t="s">
         <v>606</v>
       </c>
-      <c r="G26" s="20" t="s">
+      <c r="G26" s="9"/>
+      <c r="H26" s="20" t="s">
         <v>590</v>
       </c>
-      <c r="H26" s="11"/>
-      <c r="I26" s="9"/>
+      <c r="I26" s="11"/>
       <c r="J26" s="14"/>
       <c r="K26" s="10">
         <v>42941</v>
@@ -5587,14 +5569,14 @@
         <v>354</v>
       </c>
       <c r="F27" s="40"/>
-      <c r="G27" s="14" t="s">
+      <c r="G27" s="9">
+        <v>30</v>
+      </c>
+      <c r="H27" s="14" t="s">
         <v>482</v>
       </c>
-      <c r="H27" s="11" t="s">
+      <c r="I27" s="11" t="s">
         <v>359</v>
-      </c>
-      <c r="I27" s="9">
-        <v>30</v>
       </c>
       <c r="J27" s="14" t="s">
         <v>357</v>
@@ -5622,14 +5604,14 @@
       <c r="F28" s="40" t="s">
         <v>75</v>
       </c>
-      <c r="G28" s="9" t="s">
+      <c r="G28" s="9">
+        <v>30</v>
+      </c>
+      <c r="H28" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="H28" s="21" t="s">
+      <c r="I28" s="21" t="s">
         <v>76</v>
-      </c>
-      <c r="I28" s="9">
-        <v>30</v>
       </c>
       <c r="J28" s="9" t="s">
         <v>2</v>
@@ -5657,11 +5639,11 @@
       <c r="F29" s="44" t="s">
         <v>639</v>
       </c>
-      <c r="G29" s="20" t="s">
+      <c r="G29" s="9"/>
+      <c r="H29" s="20" t="s">
         <v>590</v>
       </c>
-      <c r="H29" s="11"/>
-      <c r="I29" s="9"/>
+      <c r="I29" s="11"/>
       <c r="J29" s="14"/>
       <c r="K29" s="10">
         <v>42941</v>
@@ -5686,11 +5668,11 @@
       <c r="F30" s="44" t="s">
         <v>634</v>
       </c>
-      <c r="G30" s="20" t="s">
+      <c r="G30" s="9"/>
+      <c r="H30" s="20" t="s">
         <v>590</v>
       </c>
-      <c r="H30" s="11"/>
-      <c r="I30" s="9"/>
+      <c r="I30" s="11"/>
       <c r="J30" s="14"/>
       <c r="K30" s="10">
         <v>42941</v>
@@ -5713,14 +5695,14 @@
         <v>394</v>
       </c>
       <c r="F31" s="40"/>
-      <c r="G31" s="14" t="s">
+      <c r="G31" s="9">
+        <v>30</v>
+      </c>
+      <c r="H31" s="14" t="s">
         <v>482</v>
       </c>
-      <c r="H31" s="11" t="s">
+      <c r="I31" s="11" t="s">
         <v>393</v>
-      </c>
-      <c r="I31" s="9">
-        <v>30</v>
       </c>
       <c r="J31" s="14" t="s">
         <v>357</v>
@@ -5748,14 +5730,14 @@
       <c r="F32" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="G32" s="9" t="s">
+      <c r="G32" s="9">
+        <v>30</v>
+      </c>
+      <c r="H32" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="H32" s="11" t="s">
+      <c r="I32" s="11" t="s">
         <v>34</v>
-      </c>
-      <c r="I32" s="9">
-        <v>30</v>
       </c>
       <c r="J32" s="9" t="s">
         <v>2</v>
@@ -5781,14 +5763,14 @@
         <v>459</v>
       </c>
       <c r="F33" s="40"/>
-      <c r="G33" s="14" t="s">
+      <c r="G33" s="9">
+        <v>30</v>
+      </c>
+      <c r="H33" s="14" t="s">
         <v>482</v>
       </c>
-      <c r="H33" s="11" t="s">
+      <c r="I33" s="11" t="s">
         <v>460</v>
-      </c>
-      <c r="I33" s="9">
-        <v>30</v>
       </c>
       <c r="J33" s="14" t="s">
         <v>357</v>
@@ -5814,14 +5796,14 @@
         <v>453</v>
       </c>
       <c r="F34" s="40"/>
-      <c r="G34" s="14" t="s">
+      <c r="G34" s="9">
+        <v>30</v>
+      </c>
+      <c r="H34" s="14" t="s">
         <v>482</v>
       </c>
-      <c r="H34" s="11" t="s">
+      <c r="I34" s="11" t="s">
         <v>454</v>
-      </c>
-      <c r="I34" s="9">
-        <v>30</v>
       </c>
       <c r="J34" s="14" t="s">
         <v>357</v>
@@ -5849,11 +5831,11 @@
       <c r="F35" s="44" t="s">
         <v>647</v>
       </c>
-      <c r="G35" s="20" t="s">
+      <c r="G35" s="9"/>
+      <c r="H35" s="20" t="s">
         <v>590</v>
       </c>
-      <c r="H35" s="11"/>
-      <c r="I35" s="9"/>
+      <c r="I35" s="11"/>
       <c r="J35" s="14"/>
       <c r="K35" s="10">
         <v>42941</v>
@@ -5876,14 +5858,14 @@
         <v>391</v>
       </c>
       <c r="F36" s="40"/>
-      <c r="G36" s="14" t="s">
+      <c r="G36" s="9">
+        <v>30</v>
+      </c>
+      <c r="H36" s="14" t="s">
         <v>482</v>
       </c>
-      <c r="H36" s="9" t="s">
+      <c r="I36" s="9" t="s">
         <v>390</v>
-      </c>
-      <c r="I36" s="9">
-        <v>30</v>
       </c>
       <c r="J36" s="14" t="s">
         <v>357</v>
@@ -5911,11 +5893,11 @@
       <c r="F37" s="44" t="s">
         <v>591</v>
       </c>
-      <c r="G37" s="20" t="s">
+      <c r="G37" s="9"/>
+      <c r="H37" s="20" t="s">
         <v>590</v>
       </c>
-      <c r="H37" s="11"/>
-      <c r="I37" s="9"/>
+      <c r="I37" s="11"/>
       <c r="J37" s="14"/>
       <c r="K37" s="10">
         <v>42941</v>
@@ -5938,14 +5920,14 @@
         <v>458</v>
       </c>
       <c r="F38" s="40"/>
-      <c r="G38" s="14" t="s">
+      <c r="G38" s="9">
+        <v>30</v>
+      </c>
+      <c r="H38" s="14" t="s">
         <v>482</v>
       </c>
-      <c r="H38" s="11" t="s">
+      <c r="I38" s="11" t="s">
         <v>457</v>
-      </c>
-      <c r="I38" s="9">
-        <v>30</v>
       </c>
       <c r="J38" s="14" t="s">
         <v>357</v>
@@ -5973,14 +5955,14 @@
       <c r="F39" s="40" t="s">
         <v>80</v>
       </c>
-      <c r="G39" s="9" t="s">
+      <c r="G39" s="9">
+        <v>30</v>
+      </c>
+      <c r="H39" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="H39" s="11" t="s">
+      <c r="I39" s="11" t="s">
         <v>81</v>
-      </c>
-      <c r="I39" s="9">
-        <v>30</v>
       </c>
       <c r="J39" s="9" t="s">
         <v>2</v>
@@ -6008,14 +5990,14 @@
       <c r="F40" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="G40" s="9" t="s">
+      <c r="G40" s="9">
+        <v>30</v>
+      </c>
+      <c r="H40" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="H40" s="11" t="s">
+      <c r="I40" s="11" t="s">
         <v>39</v>
-      </c>
-      <c r="I40" s="9">
-        <v>30</v>
       </c>
       <c r="J40" s="9" t="s">
         <v>2</v>
@@ -6043,11 +6025,11 @@
       <c r="F41" s="44" t="s">
         <v>605</v>
       </c>
-      <c r="G41" s="20" t="s">
+      <c r="G41" s="9"/>
+      <c r="H41" s="20" t="s">
         <v>590</v>
       </c>
-      <c r="H41" s="11"/>
-      <c r="I41" s="9"/>
+      <c r="I41" s="11"/>
       <c r="J41" s="14"/>
       <c r="K41" s="10">
         <v>42941</v>
@@ -6070,14 +6052,14 @@
         <v>407</v>
       </c>
       <c r="F42" s="40"/>
-      <c r="G42" s="14" t="s">
+      <c r="G42" s="9">
+        <v>30</v>
+      </c>
+      <c r="H42" s="14" t="s">
         <v>482</v>
       </c>
-      <c r="H42" s="11" t="s">
+      <c r="I42" s="11" t="s">
         <v>408</v>
-      </c>
-      <c r="I42" s="9">
-        <v>30</v>
       </c>
       <c r="J42" s="14" t="s">
         <v>357</v>
@@ -6105,14 +6087,14 @@
       <c r="F43" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="G43" s="9" t="s">
+      <c r="G43" s="9">
+        <v>30</v>
+      </c>
+      <c r="H43" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="H43" s="11" t="s">
+      <c r="I43" s="11" t="s">
         <v>44</v>
-      </c>
-      <c r="I43" s="9">
-        <v>30</v>
       </c>
       <c r="J43" s="9" t="s">
         <v>2</v>
@@ -6140,11 +6122,11 @@
       <c r="F44" s="44" t="s">
         <v>598</v>
       </c>
-      <c r="G44" s="20" t="s">
+      <c r="G44" s="9"/>
+      <c r="H44" s="20" t="s">
         <v>590</v>
       </c>
-      <c r="H44" s="11"/>
-      <c r="I44" s="9"/>
+      <c r="I44" s="11"/>
       <c r="J44" s="14"/>
       <c r="K44" s="10">
         <v>42941</v>
@@ -6169,14 +6151,14 @@
       <c r="F45" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="G45" s="9" t="s">
+      <c r="G45" s="9">
+        <v>30</v>
+      </c>
+      <c r="H45" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="H45" s="11" t="s">
+      <c r="I45" s="11" t="s">
         <v>49</v>
-      </c>
-      <c r="I45" s="9">
-        <v>30</v>
       </c>
       <c r="J45" s="9" t="s">
         <v>2</v>
@@ -6202,14 +6184,14 @@
         <v>366</v>
       </c>
       <c r="F46" s="40"/>
-      <c r="G46" s="14" t="s">
+      <c r="G46" s="9">
+        <v>30</v>
+      </c>
+      <c r="H46" s="14" t="s">
         <v>482</v>
       </c>
-      <c r="H46" s="11" t="s">
+      <c r="I46" s="11" t="s">
         <v>367</v>
-      </c>
-      <c r="I46" s="9">
-        <v>30</v>
       </c>
       <c r="J46" s="14" t="s">
         <v>357</v>
@@ -6235,14 +6217,14 @@
         <v>451</v>
       </c>
       <c r="F47" s="40"/>
-      <c r="G47" s="14" t="s">
+      <c r="G47" s="9">
+        <v>30</v>
+      </c>
+      <c r="H47" s="14" t="s">
         <v>482</v>
       </c>
-      <c r="H47" s="11" t="s">
+      <c r="I47" s="11" t="s">
         <v>452</v>
-      </c>
-      <c r="I47" s="9">
-        <v>30</v>
       </c>
       <c r="J47" s="14" t="s">
         <v>357</v>
@@ -6268,14 +6250,14 @@
         <v>440</v>
       </c>
       <c r="F48" s="40"/>
-      <c r="G48" s="14" t="s">
+      <c r="G48" s="9">
+        <v>30</v>
+      </c>
+      <c r="H48" s="14" t="s">
         <v>482</v>
       </c>
-      <c r="H48" s="11" t="s">
+      <c r="I48" s="11" t="s">
         <v>441</v>
-      </c>
-      <c r="I48" s="9">
-        <v>30</v>
       </c>
       <c r="J48" s="14" t="s">
         <v>357</v>
@@ -6303,14 +6285,14 @@
       <c r="F49" s="40" t="s">
         <v>53</v>
       </c>
-      <c r="G49" s="9" t="s">
+      <c r="G49" s="9">
+        <v>30</v>
+      </c>
+      <c r="H49" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="H49" s="11" t="s">
+      <c r="I49" s="11" t="s">
         <v>54</v>
-      </c>
-      <c r="I49" s="9">
-        <v>30</v>
       </c>
       <c r="J49" s="9" t="s">
         <v>2</v>
@@ -6336,14 +6318,14 @@
         <v>375</v>
       </c>
       <c r="F50" s="40"/>
-      <c r="G50" s="14" t="s">
+      <c r="G50" s="9">
+        <v>30</v>
+      </c>
+      <c r="H50" s="14" t="s">
         <v>482</v>
       </c>
-      <c r="H50" s="11" t="s">
+      <c r="I50" s="11" t="s">
         <v>376</v>
-      </c>
-      <c r="I50" s="9">
-        <v>30</v>
       </c>
       <c r="J50" s="14" t="s">
         <v>357</v>
@@ -6369,14 +6351,14 @@
         <v>399</v>
       </c>
       <c r="F51" s="40"/>
-      <c r="G51" s="14" t="s">
+      <c r="G51" s="9">
+        <v>30</v>
+      </c>
+      <c r="H51" s="14" t="s">
         <v>482</v>
       </c>
-      <c r="H51" s="11" t="s">
+      <c r="I51" s="11" t="s">
         <v>400</v>
-      </c>
-      <c r="I51" s="9">
-        <v>30</v>
       </c>
       <c r="J51" s="14" t="s">
         <v>357</v>
@@ -6404,11 +6386,11 @@
       <c r="F52" s="44" t="s">
         <v>655</v>
       </c>
-      <c r="G52" s="20" t="s">
+      <c r="G52" s="9"/>
+      <c r="H52" s="20" t="s">
         <v>590</v>
       </c>
-      <c r="H52" s="11"/>
-      <c r="I52" s="9"/>
+      <c r="I52" s="11"/>
       <c r="J52" s="14"/>
       <c r="K52" s="10">
         <v>42941</v>
@@ -6433,11 +6415,11 @@
       <c r="F53" s="44" t="s">
         <v>632</v>
       </c>
-      <c r="G53" s="20" t="s">
+      <c r="G53" s="9"/>
+      <c r="H53" s="20" t="s">
         <v>590</v>
       </c>
-      <c r="H53" s="11"/>
-      <c r="I53" s="9"/>
+      <c r="I53" s="11"/>
       <c r="J53" s="14"/>
       <c r="K53" s="10">
         <v>42941</v>
@@ -6460,14 +6442,14 @@
         <v>332</v>
       </c>
       <c r="F54" s="40"/>
-      <c r="G54" s="14" t="s">
+      <c r="G54" s="9">
+        <v>25</v>
+      </c>
+      <c r="H54" s="14" t="s">
         <v>337</v>
       </c>
-      <c r="H54" s="11" t="s">
+      <c r="I54" s="11" t="s">
         <v>340</v>
-      </c>
-      <c r="I54" s="9">
-        <v>25</v>
       </c>
       <c r="J54" s="14" t="s">
         <v>356</v>
@@ -6495,11 +6477,11 @@
       <c r="F55" s="44" t="s">
         <v>594</v>
       </c>
-      <c r="G55" s="20" t="s">
+      <c r="G55" s="9"/>
+      <c r="H55" s="20" t="s">
         <v>590</v>
       </c>
-      <c r="H55" s="11"/>
-      <c r="I55" s="9"/>
+      <c r="I55" s="11"/>
       <c r="J55" s="14"/>
       <c r="K55" s="10">
         <v>42941</v>
@@ -6524,14 +6506,14 @@
       <c r="F56" s="40" t="s">
         <v>85</v>
       </c>
-      <c r="G56" s="9" t="s">
+      <c r="G56" s="9">
+        <v>30</v>
+      </c>
+      <c r="H56" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="H56" s="21" t="s">
+      <c r="I56" s="21" t="s">
         <v>86</v>
-      </c>
-      <c r="I56" s="9">
-        <v>30</v>
       </c>
       <c r="J56" s="9" t="s">
         <v>2</v>
@@ -6559,11 +6541,11 @@
       <c r="F57" s="44" t="s">
         <v>600</v>
       </c>
-      <c r="G57" s="20" t="s">
+      <c r="G57" s="9"/>
+      <c r="H57" s="20" t="s">
         <v>590</v>
       </c>
-      <c r="H57" s="11"/>
-      <c r="I57" s="9"/>
+      <c r="I57" s="11"/>
       <c r="J57" s="14"/>
       <c r="K57" s="10">
         <v>42941</v>
@@ -6588,11 +6570,11 @@
       <c r="F58" s="44" t="s">
         <v>637</v>
       </c>
-      <c r="G58" s="20" t="s">
+      <c r="G58" s="9"/>
+      <c r="H58" s="20" t="s">
         <v>590</v>
       </c>
-      <c r="H58" s="11"/>
-      <c r="I58" s="9"/>
+      <c r="I58" s="11"/>
       <c r="J58" s="14"/>
       <c r="K58" s="10">
         <v>42941</v>
@@ -6615,14 +6597,14 @@
         <v>341</v>
       </c>
       <c r="F59" s="40"/>
-      <c r="G59" s="14" t="s">
+      <c r="G59" s="9">
+        <v>30</v>
+      </c>
+      <c r="H59" s="14" t="s">
         <v>482</v>
       </c>
-      <c r="H59" s="11" t="s">
+      <c r="I59" s="11" t="s">
         <v>347</v>
-      </c>
-      <c r="I59" s="9">
-        <v>30</v>
       </c>
       <c r="J59" s="14" t="s">
         <v>358</v>
@@ -6648,14 +6630,14 @@
         <v>395</v>
       </c>
       <c r="F60" s="40"/>
-      <c r="G60" s="14" t="s">
+      <c r="G60" s="9">
+        <v>30</v>
+      </c>
+      <c r="H60" s="14" t="s">
         <v>482</v>
       </c>
-      <c r="H60" s="11" t="s">
+      <c r="I60" s="11" t="s">
         <v>397</v>
-      </c>
-      <c r="I60" s="9">
-        <v>30</v>
       </c>
       <c r="J60" s="14" t="s">
         <v>357</v>
@@ -6681,14 +6663,14 @@
         <v>382</v>
       </c>
       <c r="F61" s="40"/>
-      <c r="G61" s="14" t="s">
+      <c r="G61" s="9">
+        <v>30</v>
+      </c>
+      <c r="H61" s="14" t="s">
         <v>482</v>
       </c>
-      <c r="H61" s="11" t="s">
+      <c r="I61" s="11" t="s">
         <v>383</v>
-      </c>
-      <c r="I61" s="9">
-        <v>30</v>
       </c>
       <c r="J61" s="14" t="s">
         <v>357</v>
@@ -6716,11 +6698,11 @@
       <c r="F62" s="44" t="s">
         <v>603</v>
       </c>
-      <c r="G62" s="20" t="s">
+      <c r="G62" s="9"/>
+      <c r="H62" s="20" t="s">
         <v>590</v>
       </c>
-      <c r="H62" s="11"/>
-      <c r="I62" s="9"/>
+      <c r="I62" s="11"/>
       <c r="J62" s="14"/>
       <c r="K62" s="10">
         <v>42941</v>
@@ -6743,14 +6725,14 @@
         <v>402</v>
       </c>
       <c r="F63" s="40"/>
-      <c r="G63" s="14" t="s">
+      <c r="G63" s="9">
+        <v>30</v>
+      </c>
+      <c r="H63" s="14" t="s">
         <v>482</v>
       </c>
-      <c r="H63" s="11" t="s">
+      <c r="I63" s="11" t="s">
         <v>401</v>
-      </c>
-      <c r="I63" s="9">
-        <v>30</v>
       </c>
       <c r="J63" s="14" t="s">
         <v>357</v>
@@ -6778,14 +6760,14 @@
       <c r="F64" s="40" t="s">
         <v>90</v>
       </c>
-      <c r="G64" s="9" t="s">
+      <c r="G64" s="9">
+        <v>30</v>
+      </c>
+      <c r="H64" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="H64" s="11" t="s">
+      <c r="I64" s="11" t="s">
         <v>91</v>
-      </c>
-      <c r="I64" s="9">
-        <v>30</v>
       </c>
       <c r="J64" s="9" t="s">
         <v>2</v>
@@ -6813,14 +6795,14 @@
       <c r="F65" s="40" t="s">
         <v>58</v>
       </c>
-      <c r="G65" s="9" t="s">
+      <c r="G65" s="9">
+        <v>30</v>
+      </c>
+      <c r="H65" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="H65" s="11" t="s">
+      <c r="I65" s="11" t="s">
         <v>59</v>
-      </c>
-      <c r="I65" s="9">
-        <v>30</v>
       </c>
       <c r="J65" s="9" t="s">
         <v>2</v>
@@ -6848,11 +6830,11 @@
       <c r="F66" s="44" t="s">
         <v>649</v>
       </c>
-      <c r="G66" s="20" t="s">
+      <c r="G66" s="9"/>
+      <c r="H66" s="20" t="s">
         <v>590</v>
       </c>
-      <c r="H66" s="11"/>
-      <c r="I66" s="9"/>
+      <c r="I66" s="11"/>
       <c r="J66" s="14"/>
       <c r="K66" s="10">
         <v>42941</v>
@@ -6875,13 +6857,13 @@
         <v>491</v>
       </c>
       <c r="F67" s="40"/>
-      <c r="G67" s="14" t="s">
+      <c r="G67" s="9"/>
+      <c r="H67" s="14" t="s">
         <v>493</v>
       </c>
-      <c r="H67" s="11" t="s">
+      <c r="I67" s="11" t="s">
         <v>490</v>
       </c>
-      <c r="I67" s="9"/>
       <c r="J67" s="9"/>
       <c r="K67" s="10">
         <v>42912</v>
@@ -6906,11 +6888,11 @@
       <c r="F68" s="44" t="s">
         <v>687</v>
       </c>
-      <c r="G68" s="20" t="s">
+      <c r="G68" s="9"/>
+      <c r="H68" s="20" t="s">
         <v>590</v>
       </c>
-      <c r="H68" s="11"/>
-      <c r="I68" s="9"/>
+      <c r="I68" s="11"/>
       <c r="J68" s="14"/>
       <c r="K68" s="10">
         <v>42941</v>
@@ -6933,14 +6915,14 @@
         <v>447</v>
       </c>
       <c r="F69" s="40"/>
-      <c r="G69" s="14" t="s">
+      <c r="G69" s="9">
+        <v>30</v>
+      </c>
+      <c r="H69" s="14" t="s">
         <v>482</v>
       </c>
-      <c r="H69" s="11" t="s">
+      <c r="I69" s="11" t="s">
         <v>448</v>
-      </c>
-      <c r="I69" s="9">
-        <v>30</v>
       </c>
       <c r="J69" s="14" t="s">
         <v>357</v>
@@ -6966,14 +6948,14 @@
         <v>342</v>
       </c>
       <c r="F70" s="40"/>
-      <c r="G70" s="14" t="s">
+      <c r="G70" s="9">
+        <v>30</v>
+      </c>
+      <c r="H70" s="14" t="s">
         <v>482</v>
       </c>
-      <c r="H70" s="11" t="s">
+      <c r="I70" s="11" t="s">
         <v>345</v>
-      </c>
-      <c r="I70" s="9">
-        <v>30</v>
       </c>
       <c r="J70" s="14" t="s">
         <v>358</v>
@@ -7001,11 +6983,11 @@
       <c r="F71" s="44" t="s">
         <v>641</v>
       </c>
-      <c r="G71" s="20" t="s">
+      <c r="G71" s="9"/>
+      <c r="H71" s="20" t="s">
         <v>590</v>
       </c>
-      <c r="H71" s="11"/>
-      <c r="I71" s="9"/>
+      <c r="I71" s="11"/>
       <c r="J71" s="14"/>
       <c r="K71" s="10">
         <v>42941</v>
@@ -7028,14 +7010,14 @@
         <v>409</v>
       </c>
       <c r="F72" s="40"/>
-      <c r="G72" s="14" t="s">
+      <c r="G72" s="9">
+        <v>30</v>
+      </c>
+      <c r="H72" s="14" t="s">
         <v>482</v>
       </c>
-      <c r="H72" s="11" t="s">
+      <c r="I72" s="11" t="s">
         <v>410</v>
-      </c>
-      <c r="I72" s="9">
-        <v>30</v>
       </c>
       <c r="J72" s="14" t="s">
         <v>357</v>
@@ -7063,11 +7045,11 @@
       <c r="F73" s="44" t="s">
         <v>652</v>
       </c>
-      <c r="G73" s="20" t="s">
+      <c r="G73" s="9"/>
+      <c r="H73" s="20" t="s">
         <v>590</v>
       </c>
-      <c r="H73" s="11"/>
-      <c r="I73" s="9"/>
+      <c r="I73" s="11"/>
       <c r="J73" s="14"/>
       <c r="K73" s="10">
         <v>42941</v>
@@ -7090,14 +7072,14 @@
         <v>389</v>
       </c>
       <c r="F74" s="40"/>
-      <c r="G74" s="14" t="s">
+      <c r="G74" s="9">
+        <v>30</v>
+      </c>
+      <c r="H74" s="14" t="s">
         <v>482</v>
       </c>
-      <c r="H74" s="11" t="s">
+      <c r="I74" s="11" t="s">
         <v>388</v>
-      </c>
-      <c r="I74" s="9">
-        <v>30</v>
       </c>
       <c r="J74" s="14" t="s">
         <v>357</v>
@@ -7123,14 +7105,14 @@
         <v>368</v>
       </c>
       <c r="F75" s="40"/>
-      <c r="G75" s="14" t="s">
+      <c r="G75" s="9">
+        <v>30</v>
+      </c>
+      <c r="H75" s="14" t="s">
         <v>482</v>
       </c>
-      <c r="H75" s="11" t="s">
+      <c r="I75" s="11" t="s">
         <v>369</v>
-      </c>
-      <c r="I75" s="9">
-        <v>30</v>
       </c>
       <c r="J75" s="14" t="s">
         <v>357</v>
@@ -7156,14 +7138,14 @@
         <v>380</v>
       </c>
       <c r="F76" s="40"/>
-      <c r="G76" s="14" t="s">
+      <c r="G76" s="9">
+        <v>30</v>
+      </c>
+      <c r="H76" s="14" t="s">
         <v>482</v>
       </c>
-      <c r="H76" s="11" t="s">
+      <c r="I76" s="11" t="s">
         <v>379</v>
-      </c>
-      <c r="I76" s="9">
-        <v>30</v>
       </c>
       <c r="J76" s="14" t="s">
         <v>357</v>
@@ -7189,14 +7171,14 @@
         <v>432</v>
       </c>
       <c r="F77" s="40"/>
-      <c r="G77" s="14" t="s">
+      <c r="G77" s="9">
+        <v>30</v>
+      </c>
+      <c r="H77" s="14" t="s">
         <v>482</v>
       </c>
-      <c r="H77" s="11" t="s">
+      <c r="I77" s="11" t="s">
         <v>431</v>
-      </c>
-      <c r="I77" s="9">
-        <v>30</v>
       </c>
       <c r="J77" s="14" t="s">
         <v>357</v>
@@ -7224,14 +7206,14 @@
       <c r="F78" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="G78" s="30" t="s">
+      <c r="G78" s="30">
+        <v>30</v>
+      </c>
+      <c r="H78" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="H78" s="31" t="s">
+      <c r="I78" s="31" t="s">
         <v>351</v>
-      </c>
-      <c r="I78" s="30">
-        <v>30</v>
       </c>
       <c r="J78" s="30" t="s">
         <v>2</v>
@@ -7257,14 +7239,14 @@
         <v>343</v>
       </c>
       <c r="F79" s="48"/>
-      <c r="G79" s="29" t="s">
+      <c r="G79" s="30">
+        <v>30</v>
+      </c>
+      <c r="H79" s="29" t="s">
         <v>482</v>
       </c>
-      <c r="H79" s="31" t="s">
+      <c r="I79" s="31" t="s">
         <v>351</v>
-      </c>
-      <c r="I79" s="30">
-        <v>30</v>
       </c>
       <c r="J79" s="29" t="s">
         <v>357</v>
@@ -7290,14 +7272,14 @@
         <v>463</v>
       </c>
       <c r="F80" s="40"/>
-      <c r="G80" s="14" t="s">
+      <c r="G80" s="9">
+        <v>30</v>
+      </c>
+      <c r="H80" s="14" t="s">
         <v>482</v>
       </c>
-      <c r="H80" s="11" t="s">
+      <c r="I80" s="11" t="s">
         <v>462</v>
-      </c>
-      <c r="I80" s="9">
-        <v>30</v>
       </c>
       <c r="J80" s="14" t="s">
         <v>357</v>
@@ -7325,11 +7307,11 @@
       <c r="F81" s="44" t="s">
         <v>625</v>
       </c>
-      <c r="G81" s="20" t="s">
+      <c r="G81" s="9"/>
+      <c r="H81" s="20" t="s">
         <v>590</v>
       </c>
-      <c r="H81" s="11"/>
-      <c r="I81" s="9"/>
+      <c r="I81" s="11"/>
       <c r="J81" s="14"/>
       <c r="K81" s="10">
         <v>42941</v>
@@ -7354,11 +7336,11 @@
       <c r="F82" s="44" t="s">
         <v>651</v>
       </c>
-      <c r="G82" s="20" t="s">
+      <c r="G82" s="9"/>
+      <c r="H82" s="20" t="s">
         <v>590</v>
       </c>
-      <c r="H82" s="11"/>
-      <c r="I82" s="9"/>
+      <c r="I82" s="11"/>
       <c r="J82" s="14"/>
       <c r="K82" s="10">
         <v>42941</v>
@@ -7383,14 +7365,14 @@
       <c r="F83" s="40" t="s">
         <v>95</v>
       </c>
-      <c r="G83" s="9" t="s">
+      <c r="G83" s="9">
+        <v>30</v>
+      </c>
+      <c r="H83" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="H83" s="11" t="s">
+      <c r="I83" s="11" t="s">
         <v>96</v>
-      </c>
-      <c r="I83" s="9">
-        <v>30</v>
       </c>
       <c r="J83" s="9" t="s">
         <v>2</v>
@@ -7416,14 +7398,14 @@
         <v>466</v>
       </c>
       <c r="F84" s="40"/>
-      <c r="G84" s="14" t="s">
+      <c r="G84" s="9">
+        <v>30</v>
+      </c>
+      <c r="H84" s="14" t="s">
         <v>482</v>
       </c>
-      <c r="H84" s="11" t="s">
+      <c r="I84" s="11" t="s">
         <v>467</v>
-      </c>
-      <c r="I84" s="9">
-        <v>30</v>
       </c>
       <c r="J84" s="14" t="s">
         <v>357</v>
@@ -7449,14 +7431,14 @@
         <v>465</v>
       </c>
       <c r="F85" s="40"/>
-      <c r="G85" s="14" t="s">
+      <c r="G85" s="9">
+        <v>30</v>
+      </c>
+      <c r="H85" s="14" t="s">
         <v>482</v>
       </c>
-      <c r="H85" s="11" t="s">
+      <c r="I85" s="11" t="s">
         <v>464</v>
-      </c>
-      <c r="I85" s="9">
-        <v>30</v>
       </c>
       <c r="J85" s="14" t="s">
         <v>357</v>
@@ -7484,14 +7466,14 @@
       <c r="F86" s="40" t="s">
         <v>65</v>
       </c>
-      <c r="G86" s="9" t="s">
+      <c r="G86" s="9">
+        <v>30</v>
+      </c>
+      <c r="H86" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="H86" s="11" t="s">
+      <c r="I86" s="11" t="s">
         <v>66</v>
-      </c>
-      <c r="I86" s="9">
-        <v>30</v>
       </c>
       <c r="J86" s="9" t="s">
         <v>2</v>
@@ -7519,14 +7501,14 @@
       <c r="F87" s="40" t="s">
         <v>99</v>
       </c>
-      <c r="G87" s="9" t="s">
+      <c r="G87" s="9">
+        <v>30</v>
+      </c>
+      <c r="H87" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="H87" s="21" t="s">
+      <c r="I87" s="21" t="s">
         <v>100</v>
-      </c>
-      <c r="I87" s="9">
-        <v>30</v>
       </c>
       <c r="J87" s="9" t="s">
         <v>2</v>
@@ -7552,14 +7534,14 @@
         <v>404</v>
       </c>
       <c r="F88" s="40"/>
-      <c r="G88" s="14" t="s">
+      <c r="G88" s="9">
+        <v>30</v>
+      </c>
+      <c r="H88" s="14" t="s">
         <v>482</v>
       </c>
-      <c r="H88" s="11" t="s">
+      <c r="I88" s="11" t="s">
         <v>403</v>
-      </c>
-      <c r="I88" s="9">
-        <v>30</v>
       </c>
       <c r="J88" s="14" t="s">
         <v>357</v>
@@ -7587,11 +7569,11 @@
       <c r="F89" s="44" t="s">
         <v>596</v>
       </c>
-      <c r="G89" s="20" t="s">
+      <c r="G89" s="9"/>
+      <c r="H89" s="20" t="s">
         <v>590</v>
       </c>
-      <c r="H89" s="11"/>
-      <c r="I89" s="9"/>
+      <c r="I89" s="11"/>
       <c r="J89" s="14"/>
       <c r="K89" s="10">
         <v>42941</v>
@@ -7616,11 +7598,11 @@
       <c r="F90" s="44" t="s">
         <v>686</v>
       </c>
-      <c r="G90" s="20" t="s">
+      <c r="G90" s="9"/>
+      <c r="H90" s="20" t="s">
         <v>590</v>
       </c>
-      <c r="H90" s="11"/>
-      <c r="I90" s="9"/>
+      <c r="I90" s="11"/>
       <c r="J90" s="14"/>
       <c r="K90" s="10">
         <v>42941</v>
@@ -7643,14 +7625,14 @@
         <v>433</v>
       </c>
       <c r="F91" s="40"/>
-      <c r="G91" s="14" t="s">
+      <c r="G91" s="9">
+        <v>30</v>
+      </c>
+      <c r="H91" s="14" t="s">
         <v>482</v>
       </c>
-      <c r="H91" s="11" t="s">
+      <c r="I91" s="11" t="s">
         <v>434</v>
-      </c>
-      <c r="I91" s="9">
-        <v>30</v>
       </c>
       <c r="J91" s="14" t="s">
         <v>357</v>
@@ -7676,14 +7658,14 @@
         <v>385</v>
       </c>
       <c r="F92" s="40"/>
-      <c r="G92" s="14" t="s">
+      <c r="G92" s="9">
+        <v>30</v>
+      </c>
+      <c r="H92" s="14" t="s">
         <v>482</v>
       </c>
-      <c r="H92" s="11" t="s">
+      <c r="I92" s="11" t="s">
         <v>386</v>
-      </c>
-      <c r="I92" s="9">
-        <v>30</v>
       </c>
       <c r="J92" s="14" t="s">
         <v>357</v>
@@ -7709,14 +7691,14 @@
         <v>405</v>
       </c>
       <c r="F93" s="40"/>
-      <c r="G93" s="14" t="s">
+      <c r="G93" s="9">
+        <v>30</v>
+      </c>
+      <c r="H93" s="14" t="s">
         <v>482</v>
       </c>
-      <c r="H93" s="11" t="s">
+      <c r="I93" s="11" t="s">
         <v>406</v>
-      </c>
-      <c r="I93" s="9">
-        <v>30</v>
       </c>
       <c r="J93" s="14" t="s">
         <v>357</v>
@@ -7742,14 +7724,14 @@
         <v>436</v>
       </c>
       <c r="F94" s="40"/>
-      <c r="G94" s="14" t="s">
+      <c r="G94" s="9">
+        <v>30</v>
+      </c>
+      <c r="H94" s="14" t="s">
         <v>482</v>
       </c>
-      <c r="H94" s="11" t="s">
+      <c r="I94" s="11" t="s">
         <v>435</v>
-      </c>
-      <c r="I94" s="9">
-        <v>30</v>
       </c>
       <c r="J94" s="14" t="s">
         <v>357</v>
@@ -7777,14 +7759,14 @@
       <c r="F95" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="G95" s="9" t="s">
+      <c r="G95" s="9">
+        <v>30</v>
+      </c>
+      <c r="H95" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="H95" s="11" t="s">
+      <c r="I95" s="11" t="s">
         <v>69</v>
-      </c>
-      <c r="I95" s="9">
-        <v>30</v>
       </c>
       <c r="J95" s="9" t="s">
         <v>2</v>
@@ -7812,13 +7794,13 @@
       <c r="F96" s="9" t="s">
         <v>692</v>
       </c>
-      <c r="G96" s="9" t="s">
+      <c r="G96" s="9"/>
+      <c r="H96" s="9" t="s">
         <v>691</v>
       </c>
-      <c r="H96" s="11" t="s">
+      <c r="I96" s="11" t="s">
         <v>694</v>
       </c>
-      <c r="I96" s="9"/>
       <c r="J96" s="9"/>
       <c r="K96" s="10"/>
     </row>
@@ -7842,10 +7824,10 @@
         <v>709</v>
       </c>
       <c r="G97" s="17"/>
-      <c r="H97" s="18" t="s">
+      <c r="H97" s="17"/>
+      <c r="I97" s="18" t="s">
         <v>710</v>
       </c>
-      <c r="I97" s="17"/>
       <c r="J97" s="17"/>
       <c r="K97" s="22"/>
     </row>
@@ -7866,13 +7848,13 @@
         <v>293</v>
       </c>
       <c r="F98" s="9"/>
-      <c r="G98" s="14" t="s">
+      <c r="G98" s="9">
+        <v>8</v>
+      </c>
+      <c r="H98" s="14" t="s">
         <v>297</v>
       </c>
-      <c r="H98" s="14"/>
-      <c r="I98" s="9">
-        <v>8</v>
-      </c>
+      <c r="I98" s="14"/>
       <c r="J98" s="14" t="s">
         <v>286</v>
       </c>
@@ -7898,13 +7880,13 @@
         <v>219</v>
       </c>
       <c r="F99" s="9"/>
-      <c r="G99" s="14" t="s">
+      <c r="G99" s="9">
+        <v>10</v>
+      </c>
+      <c r="H99" s="14" t="s">
         <v>252</v>
       </c>
-      <c r="H99" s="14"/>
-      <c r="I99" s="9">
-        <v>10</v>
-      </c>
+      <c r="I99" s="14"/>
       <c r="J99" s="14" t="s">
         <v>221</v>
       </c>
@@ -7930,13 +7912,13 @@
         <v>227</v>
       </c>
       <c r="F100" s="9"/>
-      <c r="G100" s="14" t="s">
+      <c r="G100" s="9">
+        <v>15</v>
+      </c>
+      <c r="H100" s="14" t="s">
         <v>252</v>
       </c>
-      <c r="H100" s="14"/>
-      <c r="I100" s="9">
-        <v>15</v>
-      </c>
+      <c r="I100" s="14"/>
       <c r="J100" s="14" t="s">
         <v>221</v>
       </c>
@@ -7962,13 +7944,13 @@
         <v>218</v>
       </c>
       <c r="F101" s="30"/>
-      <c r="G101" s="29" t="s">
+      <c r="G101" s="30">
+        <v>10</v>
+      </c>
+      <c r="H101" s="29" t="s">
         <v>252</v>
       </c>
-      <c r="H101" s="29"/>
-      <c r="I101" s="30">
-        <v>10</v>
-      </c>
+      <c r="I101" s="29"/>
       <c r="J101" s="29" t="s">
         <v>221</v>
       </c>
@@ -7994,13 +7976,13 @@
         <v>279</v>
       </c>
       <c r="F102" s="30"/>
-      <c r="G102" s="29" t="s">
+      <c r="G102" s="30">
+        <v>8</v>
+      </c>
+      <c r="H102" s="29" t="s">
         <v>297</v>
       </c>
-      <c r="H102" s="29"/>
-      <c r="I102" s="30">
-        <v>8</v>
-      </c>
+      <c r="I102" s="29"/>
       <c r="J102" s="29" t="s">
         <v>286</v>
       </c>
@@ -8026,11 +8008,11 @@
         <v>265</v>
       </c>
       <c r="F103" s="9"/>
-      <c r="G103" s="9"/>
+      <c r="G103" s="9">
+        <v>0</v>
+      </c>
       <c r="H103" s="9"/>
-      <c r="I103" s="9">
-        <v>0</v>
-      </c>
+      <c r="I103" s="9"/>
       <c r="J103" s="9">
         <v>0</v>
       </c>
@@ -8054,13 +8036,13 @@
         <v>244</v>
       </c>
       <c r="F104" s="14"/>
-      <c r="G104" s="14" t="s">
+      <c r="G104" s="14">
+        <v>0</v>
+      </c>
+      <c r="H104" s="14" t="s">
         <v>252</v>
       </c>
-      <c r="H104" s="14"/>
-      <c r="I104" s="14">
-        <v>0</v>
-      </c>
+      <c r="I104" s="14"/>
       <c r="J104" s="14" t="s">
         <v>221</v>
       </c>
@@ -8086,13 +8068,13 @@
         <v>292</v>
       </c>
       <c r="F105" s="9"/>
-      <c r="G105" s="14" t="s">
+      <c r="G105" s="9">
+        <v>7</v>
+      </c>
+      <c r="H105" s="14" t="s">
         <v>252</v>
       </c>
-      <c r="H105" s="14"/>
-      <c r="I105" s="9">
-        <v>7</v>
-      </c>
+      <c r="I105" s="14"/>
       <c r="J105" s="14" t="s">
         <v>221</v>
       </c>
@@ -8118,13 +8100,13 @@
         <v>282</v>
       </c>
       <c r="F106" s="9"/>
-      <c r="G106" s="14" t="s">
+      <c r="G106" s="9">
+        <v>8</v>
+      </c>
+      <c r="H106" s="14" t="s">
         <v>297</v>
       </c>
-      <c r="H106" s="14"/>
-      <c r="I106" s="9">
-        <v>8</v>
-      </c>
+      <c r="I106" s="14"/>
       <c r="J106" s="14" t="s">
         <v>286</v>
       </c>
@@ -8150,13 +8132,13 @@
         <v>259</v>
       </c>
       <c r="F107" s="9"/>
-      <c r="G107" s="14" t="s">
+      <c r="G107" s="9">
+        <v>3</v>
+      </c>
+      <c r="H107" s="14" t="s">
         <v>251</v>
       </c>
-      <c r="H107" s="14"/>
-      <c r="I107" s="9">
-        <v>3</v>
-      </c>
+      <c r="I107" s="14"/>
       <c r="J107" s="14" t="s">
         <v>249</v>
       </c>
@@ -8182,13 +8164,13 @@
         <v>283</v>
       </c>
       <c r="F108" s="9"/>
-      <c r="G108" s="14" t="s">
+      <c r="G108" s="9">
+        <v>8</v>
+      </c>
+      <c r="H108" s="14" t="s">
         <v>297</v>
       </c>
-      <c r="H108" s="14"/>
-      <c r="I108" s="9">
-        <v>8</v>
-      </c>
+      <c r="I108" s="14"/>
       <c r="J108" s="14" t="s">
         <v>286</v>
       </c>
@@ -8214,13 +8196,13 @@
         <v>213</v>
       </c>
       <c r="F109" s="14"/>
-      <c r="G109" s="14" t="s">
+      <c r="G109" s="14">
+        <v>6</v>
+      </c>
+      <c r="H109" s="14" t="s">
         <v>252</v>
       </c>
-      <c r="H109" s="14"/>
-      <c r="I109" s="14">
-        <v>6</v>
-      </c>
+      <c r="I109" s="14"/>
       <c r="J109" s="14" t="s">
         <v>222</v>
       </c>
@@ -8246,13 +8228,13 @@
         <v>277</v>
       </c>
       <c r="F110" s="9"/>
-      <c r="G110" s="14" t="s">
+      <c r="G110" s="9">
+        <v>8</v>
+      </c>
+      <c r="H110" s="14" t="s">
         <v>297</v>
       </c>
-      <c r="H110" s="14"/>
-      <c r="I110" s="9">
-        <v>8</v>
-      </c>
+      <c r="I110" s="14"/>
       <c r="J110" s="14" t="s">
         <v>286</v>
       </c>
@@ -8278,13 +8260,13 @@
         <v>263</v>
       </c>
       <c r="F111" s="9"/>
-      <c r="G111" s="14" t="s">
+      <c r="G111" s="9">
+        <v>3</v>
+      </c>
+      <c r="H111" s="14" t="s">
         <v>251</v>
       </c>
-      <c r="H111" s="14"/>
-      <c r="I111" s="9">
-        <v>3</v>
-      </c>
+      <c r="I111" s="14"/>
       <c r="J111" s="14" t="s">
         <v>249</v>
       </c>
@@ -8310,13 +8292,13 @@
         <v>232</v>
       </c>
       <c r="F112" s="9"/>
-      <c r="G112" s="14" t="s">
+      <c r="G112" s="9">
+        <v>15</v>
+      </c>
+      <c r="H112" s="14" t="s">
         <v>252</v>
       </c>
-      <c r="H112" s="14"/>
-      <c r="I112" s="9">
-        <v>15</v>
-      </c>
+      <c r="I112" s="14"/>
       <c r="J112" s="14" t="s">
         <v>221</v>
       </c>
@@ -8342,13 +8324,13 @@
         <v>242</v>
       </c>
       <c r="F113" s="9"/>
-      <c r="G113" s="14" t="s">
+      <c r="G113" s="9">
+        <v>20</v>
+      </c>
+      <c r="H113" s="14" t="s">
         <v>252</v>
       </c>
-      <c r="H113" s="14"/>
-      <c r="I113" s="9">
-        <v>20</v>
-      </c>
+      <c r="I113" s="14"/>
       <c r="J113" s="14" t="s">
         <v>221</v>
       </c>
@@ -8374,13 +8356,13 @@
         <v>233</v>
       </c>
       <c r="F114" s="9"/>
-      <c r="G114" s="14" t="s">
+      <c r="G114" s="9">
+        <v>15</v>
+      </c>
+      <c r="H114" s="14" t="s">
         <v>252</v>
       </c>
-      <c r="H114" s="14"/>
-      <c r="I114" s="9">
-        <v>15</v>
-      </c>
+      <c r="I114" s="14"/>
       <c r="J114" s="14" t="s">
         <v>221</v>
       </c>
@@ -8406,13 +8388,13 @@
         <v>239</v>
       </c>
       <c r="F115" s="9"/>
-      <c r="G115" s="14" t="s">
+      <c r="G115" s="9">
+        <v>20</v>
+      </c>
+      <c r="H115" s="14" t="s">
         <v>252</v>
       </c>
-      <c r="H115" s="14"/>
-      <c r="I115" s="9">
-        <v>20</v>
-      </c>
+      <c r="I115" s="14"/>
       <c r="J115" s="14" t="s">
         <v>221</v>
       </c>
@@ -8438,13 +8420,13 @@
         <v>243</v>
       </c>
       <c r="F116" s="30"/>
-      <c r="G116" s="29" t="s">
+      <c r="G116" s="30">
+        <v>7</v>
+      </c>
+      <c r="H116" s="29" t="s">
         <v>252</v>
       </c>
-      <c r="H116" s="29"/>
-      <c r="I116" s="30">
-        <v>7</v>
-      </c>
+      <c r="I116" s="29"/>
       <c r="J116" s="29" t="s">
         <v>221</v>
       </c>
@@ -8470,13 +8452,13 @@
         <v>215</v>
       </c>
       <c r="F117" s="30"/>
-      <c r="G117" s="29" t="s">
+      <c r="G117" s="30">
+        <v>8</v>
+      </c>
+      <c r="H117" s="29" t="s">
         <v>252</v>
       </c>
-      <c r="H117" s="29"/>
-      <c r="I117" s="30">
-        <v>8</v>
-      </c>
+      <c r="I117" s="29"/>
       <c r="J117" s="29" t="s">
         <v>221</v>
       </c>
@@ -8502,13 +8484,13 @@
         <v>275</v>
       </c>
       <c r="F118" s="30"/>
-      <c r="G118" s="29" t="s">
+      <c r="G118" s="30">
+        <v>8</v>
+      </c>
+      <c r="H118" s="29" t="s">
         <v>297</v>
       </c>
-      <c r="H118" s="29"/>
-      <c r="I118" s="30">
-        <v>8</v>
-      </c>
+      <c r="I118" s="29"/>
       <c r="J118" s="29" t="s">
         <v>287</v>
       </c>
@@ -8534,13 +8516,13 @@
         <v>284</v>
       </c>
       <c r="F119" s="30"/>
-      <c r="G119" s="29" t="s">
+      <c r="G119" s="30">
+        <v>8</v>
+      </c>
+      <c r="H119" s="29" t="s">
         <v>297</v>
       </c>
-      <c r="H119" s="29"/>
-      <c r="I119" s="30">
-        <v>8</v>
-      </c>
+      <c r="I119" s="29"/>
       <c r="J119" s="29" t="s">
         <v>286</v>
       </c>
@@ -8566,13 +8548,13 @@
         <v>274</v>
       </c>
       <c r="F120" s="30"/>
-      <c r="G120" s="29" t="s">
+      <c r="G120" s="30">
+        <v>8</v>
+      </c>
+      <c r="H120" s="29" t="s">
         <v>251</v>
       </c>
-      <c r="H120" s="29"/>
-      <c r="I120" s="30">
-        <v>8</v>
-      </c>
+      <c r="I120" s="29"/>
       <c r="J120" s="29" t="s">
         <v>246</v>
       </c>
@@ -8598,13 +8580,13 @@
         <v>278</v>
       </c>
       <c r="F121" s="30"/>
-      <c r="G121" s="29" t="s">
+      <c r="G121" s="30">
+        <v>8</v>
+      </c>
+      <c r="H121" s="29" t="s">
         <v>297</v>
       </c>
-      <c r="H121" s="29"/>
-      <c r="I121" s="30">
-        <v>8</v>
-      </c>
+      <c r="I121" s="29"/>
       <c r="J121" s="29" t="s">
         <v>286</v>
       </c>
@@ -8630,13 +8612,13 @@
         <v>266</v>
       </c>
       <c r="F122" s="9"/>
-      <c r="G122" s="14" t="s">
+      <c r="G122" s="9">
+        <v>25</v>
+      </c>
+      <c r="H122" s="14" t="s">
         <v>252</v>
       </c>
-      <c r="H122" s="14"/>
-      <c r="I122" s="9">
-        <v>25</v>
-      </c>
+      <c r="I122" s="14"/>
       <c r="J122" s="14" t="s">
         <v>221</v>
       </c>
@@ -8662,13 +8644,13 @@
         <v>229</v>
       </c>
       <c r="F123" s="9"/>
-      <c r="G123" s="14" t="s">
+      <c r="G123" s="9">
+        <v>15</v>
+      </c>
+      <c r="H123" s="14" t="s">
         <v>252</v>
       </c>
-      <c r="H123" s="14"/>
-      <c r="I123" s="9">
-        <v>15</v>
-      </c>
+      <c r="I123" s="14"/>
       <c r="J123" s="14" t="s">
         <v>221</v>
       </c>
@@ -8694,13 +8676,13 @@
         <v>248</v>
       </c>
       <c r="F124" s="9"/>
-      <c r="G124" s="14" t="s">
+      <c r="G124" s="9">
+        <v>8</v>
+      </c>
+      <c r="H124" s="14" t="s">
         <v>251</v>
       </c>
-      <c r="H124" s="14"/>
-      <c r="I124" s="9">
-        <v>8</v>
-      </c>
+      <c r="I124" s="14"/>
       <c r="J124" s="14" t="s">
         <v>245</v>
       </c>
@@ -8726,13 +8708,13 @@
         <v>248</v>
       </c>
       <c r="F125" s="9"/>
-      <c r="G125" s="14" t="s">
+      <c r="G125" s="9">
+        <v>3</v>
+      </c>
+      <c r="H125" s="14" t="s">
         <v>251</v>
       </c>
-      <c r="H125" s="14"/>
-      <c r="I125" s="9">
-        <v>3</v>
-      </c>
+      <c r="I125" s="14"/>
       <c r="J125" s="14" t="s">
         <v>250</v>
       </c>
@@ -8758,13 +8740,13 @@
         <v>261</v>
       </c>
       <c r="F126" s="9"/>
-      <c r="G126" s="14" t="s">
+      <c r="G126" s="9">
+        <v>10</v>
+      </c>
+      <c r="H126" s="14" t="s">
         <v>252</v>
       </c>
-      <c r="H126" s="14"/>
-      <c r="I126" s="9">
-        <v>10</v>
-      </c>
+      <c r="I126" s="14"/>
       <c r="J126" s="14" t="s">
         <v>221</v>
       </c>
@@ -8790,13 +8772,13 @@
         <v>224</v>
       </c>
       <c r="F127" s="14"/>
-      <c r="G127" s="14" t="s">
+      <c r="G127" s="14">
+        <v>5.3</v>
+      </c>
+      <c r="H127" s="14" t="s">
         <v>252</v>
       </c>
-      <c r="H127" s="14"/>
-      <c r="I127" s="14">
-        <v>5.3</v>
-      </c>
+      <c r="I127" s="14"/>
       <c r="J127" s="14" t="s">
         <v>222</v>
       </c>
@@ -8818,19 +8800,19 @@
         <v>320</v>
       </c>
       <c r="D128" s="14" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="E128" s="14" t="s">
         <v>272</v>
       </c>
       <c r="F128" s="9"/>
-      <c r="G128" s="14" t="s">
+      <c r="G128" s="9">
+        <v>5</v>
+      </c>
+      <c r="H128" s="14" t="s">
         <v>252</v>
       </c>
-      <c r="H128" s="14"/>
-      <c r="I128" s="9">
-        <v>5</v>
-      </c>
+      <c r="I128" s="14"/>
       <c r="J128" s="14" t="s">
         <v>221</v>
       </c>
@@ -8858,13 +8840,13 @@
         <v>276</v>
       </c>
       <c r="F129" s="30"/>
-      <c r="G129" s="29" t="s">
+      <c r="G129" s="30">
+        <v>8</v>
+      </c>
+      <c r="H129" s="29" t="s">
         <v>297</v>
       </c>
-      <c r="H129" s="29"/>
-      <c r="I129" s="30">
-        <v>8</v>
-      </c>
+      <c r="I129" s="29"/>
       <c r="J129" s="29" t="s">
         <v>286</v>
       </c>
@@ -8890,13 +8872,13 @@
         <v>273</v>
       </c>
       <c r="F130" s="30"/>
-      <c r="G130" s="29" t="s">
+      <c r="G130" s="30">
+        <v>10</v>
+      </c>
+      <c r="H130" s="29" t="s">
         <v>252</v>
       </c>
-      <c r="H130" s="29"/>
-      <c r="I130" s="30">
-        <v>10</v>
-      </c>
+      <c r="I130" s="29"/>
       <c r="J130" s="29" t="s">
         <v>221</v>
       </c>
@@ -8922,13 +8904,13 @@
         <v>247</v>
       </c>
       <c r="F131" s="30"/>
-      <c r="G131" s="29" t="s">
+      <c r="G131" s="30">
+        <v>4</v>
+      </c>
+      <c r="H131" s="29" t="s">
         <v>251</v>
       </c>
-      <c r="H131" s="29"/>
-      <c r="I131" s="30">
-        <v>4</v>
-      </c>
+      <c r="I131" s="29"/>
       <c r="J131" s="29" t="s">
         <v>250</v>
       </c>
@@ -8954,13 +8936,13 @@
         <v>231</v>
       </c>
       <c r="F132" s="30"/>
-      <c r="G132" s="29" t="s">
+      <c r="G132" s="30">
+        <v>15</v>
+      </c>
+      <c r="H132" s="29" t="s">
         <v>252</v>
       </c>
-      <c r="H132" s="29"/>
-      <c r="I132" s="30">
-        <v>15</v>
-      </c>
+      <c r="I132" s="29"/>
       <c r="J132" s="29" t="s">
         <v>221</v>
       </c>
@@ -8986,13 +8968,13 @@
         <v>231</v>
       </c>
       <c r="F133" s="30"/>
-      <c r="G133" s="29" t="s">
+      <c r="G133" s="30">
+        <v>8</v>
+      </c>
+      <c r="H133" s="29" t="s">
         <v>297</v>
       </c>
-      <c r="H133" s="29"/>
-      <c r="I133" s="30">
-        <v>8</v>
-      </c>
+      <c r="I133" s="29"/>
       <c r="J133" s="29" t="s">
         <v>286</v>
       </c>
@@ -9018,13 +9000,13 @@
         <v>216</v>
       </c>
       <c r="F134" s="9"/>
-      <c r="G134" s="14" t="s">
+      <c r="G134" s="9">
+        <v>8</v>
+      </c>
+      <c r="H134" s="14" t="s">
         <v>252</v>
       </c>
-      <c r="H134" s="14"/>
-      <c r="I134" s="9">
-        <v>8</v>
-      </c>
+      <c r="I134" s="14"/>
       <c r="J134" s="14" t="s">
         <v>221</v>
       </c>
@@ -9050,13 +9032,13 @@
         <v>256</v>
       </c>
       <c r="F135" s="9"/>
-      <c r="G135" s="14" t="s">
+      <c r="G135" s="9">
+        <v>8</v>
+      </c>
+      <c r="H135" s="14" t="s">
         <v>251</v>
       </c>
-      <c r="H135" s="14"/>
-      <c r="I135" s="9">
-        <v>8</v>
-      </c>
+      <c r="I135" s="14"/>
       <c r="J135" s="14" t="s">
         <v>246</v>
       </c>
@@ -9082,13 +9064,13 @@
         <v>225</v>
       </c>
       <c r="F136" s="9"/>
-      <c r="G136" s="14" t="s">
+      <c r="G136" s="9">
+        <v>10</v>
+      </c>
+      <c r="H136" s="14" t="s">
         <v>252</v>
       </c>
-      <c r="H136" s="14"/>
-      <c r="I136" s="9">
-        <v>10</v>
-      </c>
+      <c r="I136" s="14"/>
       <c r="J136" s="14" t="s">
         <v>221</v>
       </c>
@@ -9112,13 +9094,13 @@
       </c>
       <c r="E137" s="9"/>
       <c r="F137" s="9"/>
-      <c r="G137" s="14" t="s">
+      <c r="G137" s="9">
+        <v>10</v>
+      </c>
+      <c r="H137" s="14" t="s">
         <v>252</v>
       </c>
-      <c r="H137" s="14"/>
-      <c r="I137" s="9">
-        <v>10</v>
-      </c>
+      <c r="I137" s="14"/>
       <c r="J137" s="14" t="s">
         <v>221</v>
       </c>
@@ -9142,13 +9124,13 @@
       </c>
       <c r="E138" s="9"/>
       <c r="F138" s="9"/>
-      <c r="G138" s="14" t="s">
+      <c r="G138" s="9">
+        <v>8</v>
+      </c>
+      <c r="H138" s="14" t="s">
         <v>297</v>
       </c>
-      <c r="H138" s="14"/>
-      <c r="I138" s="9">
-        <v>8</v>
-      </c>
+      <c r="I138" s="14"/>
       <c r="J138" s="14" t="s">
         <v>286</v>
       </c>
@@ -9174,13 +9156,13 @@
         <v>236</v>
       </c>
       <c r="F139" s="9"/>
-      <c r="G139" s="14" t="s">
+      <c r="G139" s="9">
+        <v>30</v>
+      </c>
+      <c r="H139" s="14" t="s">
         <v>252</v>
       </c>
-      <c r="H139" s="14"/>
-      <c r="I139" s="9">
-        <v>30</v>
-      </c>
+      <c r="I139" s="14"/>
       <c r="J139" s="14" t="s">
         <v>221</v>
       </c>
@@ -9206,13 +9188,13 @@
         <v>296</v>
       </c>
       <c r="F140" s="17"/>
-      <c r="G140" s="25" t="s">
+      <c r="G140" s="17">
+        <v>8</v>
+      </c>
+      <c r="H140" s="25" t="s">
         <v>297</v>
       </c>
-      <c r="H140" s="25"/>
-      <c r="I140" s="17">
-        <v>8</v>
-      </c>
+      <c r="I140" s="25"/>
       <c r="J140" s="25" t="s">
         <v>287</v>
       </c>
@@ -9238,7 +9220,7 @@
       <c r="F141" s="9">
         <v>3</v>
       </c>
-      <c r="G141" s="14" t="s">
+      <c r="H141" s="14" t="s">
         <v>511</v>
       </c>
       <c r="J141" s="9">
@@ -9265,7 +9247,7 @@
       <c r="F142" s="9">
         <v>4</v>
       </c>
-      <c r="G142" s="14" t="s">
+      <c r="H142" s="14" t="s">
         <v>511</v>
       </c>
       <c r="J142" s="9">
@@ -9292,7 +9274,7 @@
       <c r="F143" s="9">
         <v>6</v>
       </c>
-      <c r="G143" s="14" t="s">
+      <c r="H143" s="14" t="s">
         <v>511</v>
       </c>
       <c r="J143" s="9">
@@ -9319,8 +9301,8 @@
         <v>698</v>
       </c>
       <c r="F144" s="9"/>
-      <c r="H144" s="10"/>
-      <c r="I144" s="14"/>
+      <c r="G144" s="14"/>
+      <c r="I144" s="10"/>
       <c r="J144" s="9">
         <v>80</v>
       </c>
@@ -9391,10 +9373,10 @@
       <c r="F147" s="14" t="s">
         <v>731</v>
       </c>
-      <c r="G147" s="14" t="s">
+      <c r="H147" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="H147" s="11" t="s">
+      <c r="I147" s="11" t="s">
         <v>71</v>
       </c>
       <c r="J147" s="14"/>
@@ -9419,10 +9401,10 @@
         <v>488</v>
       </c>
       <c r="F148" s="14"/>
-      <c r="G148" s="14" t="s">
+      <c r="H148" s="14" t="s">
         <v>492</v>
       </c>
-      <c r="H148" s="11" t="s">
+      <c r="I148" s="11" t="s">
         <v>487</v>
       </c>
       <c r="J148" s="14"/>
@@ -9447,10 +9429,10 @@
         <v>333</v>
       </c>
       <c r="F149" s="14"/>
-      <c r="G149" s="14" t="s">
+      <c r="H149" s="14" t="s">
         <v>337</v>
       </c>
-      <c r="H149" s="11" t="s">
+      <c r="I149" s="11" t="s">
         <v>338</v>
       </c>
       <c r="J149" s="14"/>
@@ -9475,10 +9457,10 @@
         <v>485</v>
       </c>
       <c r="F150" s="14"/>
-      <c r="G150" s="14" t="s">
+      <c r="H150" s="14" t="s">
         <v>492</v>
       </c>
-      <c r="H150" s="11" t="s">
+      <c r="I150" s="11" t="s">
         <v>486</v>
       </c>
       <c r="J150" s="14"/>
@@ -9504,10 +9486,10 @@
       </c>
       <c r="F151" s="14"/>
       <c r="G151" s="14"/>
-      <c r="H151" s="11" t="s">
+      <c r="H151" s="14"/>
+      <c r="I151" s="11" t="s">
         <v>715</v>
       </c>
-      <c r="I151" s="14"/>
       <c r="J151" s="14"/>
     </row>
     <row r="152" spans="1:11">
@@ -9528,10 +9510,10 @@
       </c>
       <c r="F152" s="14"/>
       <c r="G152" s="14"/>
-      <c r="H152" s="11" t="s">
+      <c r="H152" s="14"/>
+      <c r="I152" s="11" t="s">
         <v>718</v>
       </c>
-      <c r="I152" s="14"/>
       <c r="J152" s="14"/>
     </row>
     <row r="153" spans="1:11">
@@ -9552,10 +9534,10 @@
       </c>
       <c r="F153" s="14"/>
       <c r="G153" s="14"/>
-      <c r="H153" s="11" t="s">
+      <c r="H153" s="14"/>
+      <c r="I153" s="11" t="s">
         <v>723</v>
       </c>
-      <c r="I153" s="14"/>
       <c r="J153" s="14"/>
     </row>
     <row r="154" spans="1:11">
@@ -9576,10 +9558,10 @@
       </c>
       <c r="F154" s="14"/>
       <c r="G154" s="14"/>
-      <c r="H154" s="11" t="s">
+      <c r="H154" s="14"/>
+      <c r="I154" s="11" t="s">
         <v>725</v>
       </c>
-      <c r="I154" s="14"/>
       <c r="J154" s="14"/>
     </row>
     <row r="155" spans="1:11">
@@ -9600,10 +9582,10 @@
       </c>
       <c r="F155" s="25"/>
       <c r="G155" s="25"/>
-      <c r="H155" s="18" t="s">
+      <c r="H155" s="25"/>
+      <c r="I155" s="18" t="s">
         <v>727</v>
       </c>
-      <c r="I155" s="25"/>
       <c r="J155" s="25"/>
     </row>
     <row r="156" spans="1:11">
@@ -9611,7 +9593,7 @@
         <v>143</v>
       </c>
       <c r="B156" s="52" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="C156" s="53" t="s">
         <v>754</v>
@@ -9624,8 +9606,8 @@
       </c>
       <c r="F156" s="9"/>
       <c r="G156" s="9"/>
-      <c r="H156" s="36"/>
-      <c r="I156" s="9"/>
+      <c r="H156" s="9"/>
+      <c r="I156" s="36"/>
       <c r="J156" s="9"/>
     </row>
     <row r="157" spans="1:11">
@@ -9645,13 +9627,13 @@
         <v>761</v>
       </c>
       <c r="F157" s="9"/>
-      <c r="G157" s="9" t="s">
+      <c r="G157" s="9"/>
+      <c r="H157" s="9" t="s">
         <v>762</v>
       </c>
-      <c r="H157" s="37" t="s">
+      <c r="I157" s="37" t="s">
         <v>757</v>
       </c>
-      <c r="I157" s="9"/>
       <c r="J157" s="9"/>
     </row>
     <row r="158" spans="1:11">
@@ -9671,13 +9653,13 @@
         <v>763</v>
       </c>
       <c r="F158" s="9"/>
-      <c r="G158" s="9" t="s">
+      <c r="G158" s="9"/>
+      <c r="H158" s="9" t="s">
         <v>762</v>
       </c>
-      <c r="H158" s="37" t="s">
+      <c r="I158" s="37" t="s">
         <v>765</v>
       </c>
-      <c r="I158" s="9"/>
       <c r="J158" s="9"/>
     </row>
     <row r="159" spans="1:11">
@@ -9699,11 +9681,11 @@
       <c r="F159" s="9" t="s">
         <v>776</v>
       </c>
-      <c r="G159" s="9" t="s">
+      <c r="G159" s="9"/>
+      <c r="H159" s="9" t="s">
         <v>775</v>
       </c>
-      <c r="H159" s="36"/>
-      <c r="I159" s="9"/>
+      <c r="I159" s="36"/>
       <c r="J159" s="9"/>
     </row>
     <row r="160" spans="1:11">
@@ -9725,11 +9707,11 @@
       <c r="F160" s="9" t="s">
         <v>777</v>
       </c>
-      <c r="G160" s="9" t="s">
+      <c r="G160" s="9"/>
+      <c r="H160" s="9" t="s">
         <v>775</v>
       </c>
-      <c r="H160" s="36"/>
-      <c r="I160" s="9"/>
+      <c r="I160" s="36"/>
       <c r="J160" s="9"/>
     </row>
     <row r="161" spans="1:11">
@@ -9748,8 +9730,8 @@
       </c>
       <c r="F161" s="14"/>
       <c r="G161" s="14"/>
-      <c r="H161" s="11"/>
-      <c r="I161" s="14"/>
+      <c r="H161" s="14"/>
+      <c r="I161" s="11"/>
       <c r="J161" s="14"/>
     </row>
     <row r="162" spans="1:11">
@@ -9768,8 +9750,8 @@
       </c>
       <c r="F162" s="14"/>
       <c r="G162" s="14"/>
-      <c r="H162" s="11"/>
-      <c r="I162" s="14"/>
+      <c r="H162" s="14"/>
+      <c r="I162" s="11"/>
       <c r="J162" s="14"/>
     </row>
     <row r="163" spans="1:11">
@@ -9788,8 +9770,8 @@
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
-      <c r="H163" s="11"/>
-      <c r="I163" s="14"/>
+      <c r="H163" s="14"/>
+      <c r="I163" s="11"/>
       <c r="J163" s="14"/>
     </row>
     <row r="164" spans="1:11">
@@ -9808,8 +9790,8 @@
       </c>
       <c r="F164" s="14"/>
       <c r="G164" s="14"/>
-      <c r="H164" s="11"/>
-      <c r="I164" s="14"/>
+      <c r="H164" s="14"/>
+      <c r="I164" s="11"/>
       <c r="J164" s="14"/>
     </row>
     <row r="165" spans="1:11">
@@ -9828,8 +9810,8 @@
       </c>
       <c r="F165" s="14"/>
       <c r="G165" s="14"/>
-      <c r="H165" s="11"/>
-      <c r="I165" s="14"/>
+      <c r="H165" s="14"/>
+      <c r="I165" s="11"/>
       <c r="J165" s="14"/>
     </row>
     <row r="166" spans="1:11">
@@ -9848,8 +9830,8 @@
       </c>
       <c r="F166" s="14"/>
       <c r="G166" s="14"/>
-      <c r="H166" s="11"/>
-      <c r="I166" s="14"/>
+      <c r="H166" s="14"/>
+      <c r="I166" s="11"/>
       <c r="J166" s="14"/>
     </row>
     <row r="167" spans="1:11">
@@ -9868,8 +9850,8 @@
       </c>
       <c r="F167" s="14"/>
       <c r="G167" s="14"/>
-      <c r="H167" s="11"/>
-      <c r="I167" s="14"/>
+      <c r="H167" s="14"/>
+      <c r="I167" s="11"/>
       <c r="J167" s="14"/>
     </row>
     <row r="168" spans="1:11">
@@ -9889,14 +9871,14 @@
         <v>672</v>
       </c>
       <c r="F168" s="9"/>
-      <c r="G168" s="9" t="s">
+      <c r="G168" s="9">
+        <v>50</v>
+      </c>
+      <c r="H168" s="9" t="s">
         <v>898</v>
       </c>
-      <c r="H168" s="58" t="s">
+      <c r="I168" s="58" t="s">
         <v>681</v>
-      </c>
-      <c r="I168" s="9">
-        <v>50</v>
       </c>
       <c r="J168" s="9"/>
       <c r="K168" s="66">
@@ -9920,14 +9902,14 @@
         <v>863</v>
       </c>
       <c r="F169" s="14"/>
-      <c r="G169" s="14" t="s">
+      <c r="G169" s="14">
+        <v>30</v>
+      </c>
+      <c r="H169" s="14" t="s">
         <v>482</v>
       </c>
-      <c r="H169" s="55" t="s">
+      <c r="I169" s="55" t="s">
         <v>864</v>
-      </c>
-      <c r="I169" s="14">
-        <v>30</v>
       </c>
       <c r="J169" s="14"/>
       <c r="K169" s="66">
@@ -9951,14 +9933,14 @@
         <v>881</v>
       </c>
       <c r="F170" s="14"/>
-      <c r="G170" s="14" t="s">
+      <c r="G170" s="14">
+        <v>50</v>
+      </c>
+      <c r="H170" s="14" t="s">
         <v>482</v>
       </c>
-      <c r="H170" s="55" t="s">
+      <c r="I170" s="55" t="s">
         <v>882</v>
-      </c>
-      <c r="I170" s="14">
-        <v>50</v>
       </c>
       <c r="J170" s="14"/>
       <c r="K170" s="66">
@@ -9982,13 +9964,13 @@
         <v>588</v>
       </c>
       <c r="F171" s="63"/>
-      <c r="G171" s="63" t="s">
+      <c r="G171" s="63">
+        <v>50</v>
+      </c>
+      <c r="H171" s="63" t="s">
         <v>482</v>
       </c>
-      <c r="H171" s="64"/>
-      <c r="I171" s="63">
-        <v>50</v>
-      </c>
+      <c r="I171" s="64"/>
       <c r="J171" s="63"/>
       <c r="K171" s="66">
         <v>42984</v>
@@ -9999,7 +9981,7 @@
         <v>159</v>
       </c>
       <c r="B172" s="3" t="s">
-        <v>900</v>
+        <v>961</v>
       </c>
       <c r="C172" s="59" t="s">
         <v>202</v>
@@ -10011,13 +9993,13 @@
         <v>608</v>
       </c>
       <c r="F172" s="14"/>
-      <c r="G172" s="14" t="s">
+      <c r="G172" s="14">
+        <v>30</v>
+      </c>
+      <c r="H172" s="14" t="s">
         <v>482</v>
       </c>
-      <c r="H172" s="55"/>
-      <c r="I172" s="14">
-        <v>30</v>
-      </c>
+      <c r="I172" s="55"/>
       <c r="J172" s="14"/>
       <c r="K172" s="66">
         <v>42984</v>
@@ -10028,23 +10010,23 @@
         <v>160</v>
       </c>
       <c r="B173" s="3" t="s">
+        <v>906</v>
+      </c>
+      <c r="C173" s="13" t="s">
+        <v>905</v>
+      </c>
+      <c r="D173" s="14" t="s">
         <v>907</v>
       </c>
-      <c r="C173" s="13" t="s">
-        <v>906</v>
-      </c>
-      <c r="D173" s="14" t="s">
+      <c r="E173" s="14" t="s">
         <v>908</v>
       </c>
-      <c r="E173" s="14" t="s">
-        <v>909</v>
-      </c>
       <c r="F173" s="14"/>
-      <c r="G173" s="14" t="s">
+      <c r="G173" s="14"/>
+      <c r="H173" s="14" t="s">
         <v>482</v>
       </c>
-      <c r="H173" s="11"/>
-      <c r="I173" s="14"/>
+      <c r="I173" s="11"/>
       <c r="J173" s="14"/>
     </row>
     <row r="174" spans="1:11">
@@ -10052,21 +10034,21 @@
         <v>161</v>
       </c>
       <c r="B174" s="3" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="C174" s="13"/>
       <c r="D174" s="14" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="E174" s="14" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="F174" s="14"/>
-      <c r="G174" s="14" t="s">
+      <c r="G174" s="14"/>
+      <c r="H174" s="14" t="s">
         <v>482</v>
       </c>
-      <c r="H174" s="11"/>
-      <c r="I174" s="14"/>
+      <c r="I174" s="11"/>
       <c r="J174" s="14"/>
     </row>
     <row r="175" spans="1:11">
@@ -10074,17 +10056,17 @@
         <v>162</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="C175" s="13"/>
       <c r="D175" s="14"/>
       <c r="E175" s="14" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="F175" s="14"/>
       <c r="G175" s="14"/>
-      <c r="H175" s="11"/>
-      <c r="I175" s="14"/>
+      <c r="H175" s="14"/>
+      <c r="I175" s="11"/>
       <c r="J175" s="14"/>
     </row>
     <row r="176" spans="1:11">
@@ -10092,21 +10074,21 @@
         <v>163</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="C176" s="13"/>
       <c r="D176" s="14" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="E176" s="14" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="F176" s="14"/>
       <c r="G176" s="14"/>
-      <c r="H176" s="37" t="s">
-        <v>913</v>
-      </c>
-      <c r="I176" s="14"/>
+      <c r="H176" s="14"/>
+      <c r="I176" s="37" t="s">
+        <v>912</v>
+      </c>
       <c r="J176" s="14"/>
     </row>
     <row r="177" spans="1:10">
@@ -10114,19 +10096,19 @@
         <v>164</v>
       </c>
       <c r="B177" s="3" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="C177" s="13"/>
       <c r="D177" s="14" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="E177" s="14" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="F177" s="14"/>
       <c r="G177" s="14"/>
-      <c r="H177" s="11"/>
-      <c r="I177" s="14"/>
+      <c r="H177" s="14"/>
+      <c r="I177" s="11"/>
       <c r="J177" s="14"/>
     </row>
     <row r="178" spans="1:10">
@@ -10139,99 +10121,307 @@
       <c r="C178" s="15"/>
       <c r="D178" s="9"/>
       <c r="E178" s="9" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="F178" s="9"/>
       <c r="G178" s="9"/>
-      <c r="H178" s="69"/>
-      <c r="I178" s="9"/>
+      <c r="H178" s="9"/>
+      <c r="I178" s="69"/>
       <c r="J178" s="9"/>
+    </row>
+    <row r="179" spans="1:10">
+      <c r="A179">
+        <v>166</v>
+      </c>
+      <c r="B179" t="s">
+        <v>960</v>
+      </c>
+      <c r="C179" s="56" t="s">
+        <v>105</v>
+      </c>
+      <c r="D179" s="57" t="s">
+        <v>514</v>
+      </c>
+      <c r="E179" s="57" t="s">
+        <v>585</v>
+      </c>
+      <c r="F179" s="9"/>
+      <c r="G179" s="9">
+        <v>100</v>
+      </c>
+      <c r="H179" s="14" t="s">
+        <v>482</v>
+      </c>
+      <c r="I179" s="69"/>
+      <c r="J179" s="9"/>
+    </row>
+    <row r="180" spans="1:10">
+      <c r="A180">
+        <v>167</v>
+      </c>
+      <c r="B180" t="s">
+        <v>960</v>
+      </c>
+      <c r="C180" s="59" t="s">
+        <v>138</v>
+      </c>
+      <c r="D180" s="60" t="s">
+        <v>675</v>
+      </c>
+      <c r="E180" s="60" t="s">
+        <v>676</v>
+      </c>
+      <c r="F180" s="14"/>
+      <c r="G180" s="14">
+        <v>50</v>
+      </c>
+      <c r="H180" s="14" t="s">
+        <v>482</v>
+      </c>
+      <c r="I180" s="11"/>
+      <c r="J180" s="14"/>
+    </row>
+    <row r="181" spans="1:10">
+      <c r="A181">
+        <v>168</v>
+      </c>
+      <c r="B181" t="s">
+        <v>960</v>
+      </c>
+      <c r="C181" s="61" t="s">
+        <v>140</v>
+      </c>
+      <c r="D181" s="62" t="s">
+        <v>682</v>
+      </c>
+      <c r="E181" s="62" t="s">
+        <v>683</v>
+      </c>
+      <c r="F181" s="63"/>
+      <c r="G181" s="63">
+        <v>50</v>
+      </c>
+      <c r="H181" s="14" t="s">
+        <v>482</v>
+      </c>
+      <c r="I181" s="70"/>
+      <c r="J181" s="63"/>
+    </row>
+    <row r="182" spans="1:10">
+      <c r="A182">
+        <v>169</v>
+      </c>
+      <c r="B182" t="s">
+        <v>960</v>
+      </c>
+      <c r="C182" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="D182" s="4" t="s">
+        <v>705</v>
+      </c>
+      <c r="E182" s="4" t="s">
+        <v>701</v>
+      </c>
+      <c r="F182" s="14"/>
+      <c r="G182">
+        <v>30</v>
+      </c>
+      <c r="H182" s="14" t="s">
+        <v>482</v>
+      </c>
+      <c r="I182" s="11"/>
+      <c r="J182" s="14"/>
+    </row>
+    <row r="183" spans="1:10">
+      <c r="A183">
+        <v>170</v>
+      </c>
+      <c r="B183" t="s">
+        <v>960</v>
+      </c>
+      <c r="C183" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="D183" s="4" t="s">
+        <v>823</v>
+      </c>
+      <c r="E183" s="4" t="s">
+        <v>825</v>
+      </c>
+      <c r="F183" s="14"/>
+      <c r="G183">
+        <v>30</v>
+      </c>
+      <c r="H183" s="14" t="s">
+        <v>482</v>
+      </c>
+      <c r="I183" s="11"/>
+      <c r="J183" s="14"/>
+    </row>
+    <row r="184" spans="1:10">
+      <c r="A184">
+        <v>171</v>
+      </c>
+      <c r="B184" t="s">
+        <v>960</v>
+      </c>
+      <c r="C184" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="D184" s="4" t="s">
+        <v>670</v>
+      </c>
+      <c r="E184" s="4" t="s">
+        <v>859</v>
+      </c>
+      <c r="F184" s="14"/>
+      <c r="G184">
+        <v>30</v>
+      </c>
+      <c r="H184" s="14" t="s">
+        <v>482</v>
+      </c>
+      <c r="I184" s="11"/>
+      <c r="J184" s="14"/>
+    </row>
+    <row r="185" spans="1:10">
+      <c r="A185">
+        <v>172</v>
+      </c>
+      <c r="B185" t="s">
+        <v>960</v>
+      </c>
+      <c r="C185" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="D185" s="4" t="s">
+        <v>868</v>
+      </c>
+      <c r="E185" s="4" t="s">
+        <v>869</v>
+      </c>
+      <c r="F185" s="14"/>
+      <c r="G185">
+        <v>30</v>
+      </c>
+      <c r="H185" s="14" t="s">
+        <v>482</v>
+      </c>
+      <c r="I185" s="11"/>
+      <c r="J185" s="14"/>
+    </row>
+    <row r="186" spans="1:10">
+      <c r="A186">
+        <v>173</v>
+      </c>
+      <c r="B186" t="s">
+        <v>960</v>
+      </c>
+      <c r="C186" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="D186" s="4" t="s">
+        <v>872</v>
+      </c>
+      <c r="E186" s="4" t="s">
+        <v>871</v>
+      </c>
+      <c r="F186" s="14"/>
+      <c r="G186">
+        <v>30</v>
+      </c>
+      <c r="H186" s="14" t="s">
+        <v>482</v>
+      </c>
+      <c r="I186" s="11"/>
+      <c r="J186" s="14"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="H40" r:id="rId1"/>
-    <hyperlink ref="H23" r:id="rId2"/>
-    <hyperlink ref="H78" r:id="rId3"/>
-    <hyperlink ref="H65" r:id="rId4"/>
-    <hyperlink ref="H16" r:id="rId5"/>
-    <hyperlink ref="H86" r:id="rId6"/>
-    <hyperlink ref="H45" r:id="rId7"/>
-    <hyperlink ref="H49" r:id="rId8"/>
-    <hyperlink ref="H32" r:id="rId9"/>
-    <hyperlink ref="H43" r:id="rId10"/>
-    <hyperlink ref="H6" r:id="rId11"/>
-    <hyperlink ref="H5" r:id="rId12"/>
-    <hyperlink ref="H10" r:id="rId13"/>
-    <hyperlink ref="H8" r:id="rId14"/>
-    <hyperlink ref="H7" r:id="rId15"/>
-    <hyperlink ref="H9" r:id="rId16"/>
-    <hyperlink ref="H83" r:id="rId17"/>
-    <hyperlink ref="H28" r:id="rId18"/>
-    <hyperlink ref="H64" r:id="rId19"/>
-    <hyperlink ref="H39" r:id="rId20"/>
-    <hyperlink ref="H56" r:id="rId21"/>
-    <hyperlink ref="H87" r:id="rId22"/>
-    <hyperlink ref="H2" r:id="rId23"/>
-    <hyperlink ref="H54" r:id="rId24"/>
-    <hyperlink ref="H70" r:id="rId25"/>
-    <hyperlink ref="H79" r:id="rId26"/>
-    <hyperlink ref="H27" r:id="rId27"/>
-    <hyperlink ref="H17" r:id="rId28"/>
-    <hyperlink ref="H46" r:id="rId29"/>
-    <hyperlink ref="H75" r:id="rId30"/>
-    <hyperlink ref="H50" r:id="rId31"/>
-    <hyperlink ref="H76" r:id="rId32"/>
-    <hyperlink ref="H61" r:id="rId33"/>
-    <hyperlink ref="H92" r:id="rId34"/>
-    <hyperlink ref="H74" r:id="rId35"/>
-    <hyperlink ref="H31" r:id="rId36"/>
-    <hyperlink ref="H60" r:id="rId37"/>
-    <hyperlink ref="H51" r:id="rId38"/>
-    <hyperlink ref="H63" r:id="rId39"/>
-    <hyperlink ref="H88" r:id="rId40"/>
-    <hyperlink ref="H93" r:id="rId41"/>
-    <hyperlink ref="H42" r:id="rId42"/>
-    <hyperlink ref="H72" r:id="rId43"/>
-    <hyperlink ref="H15" r:id="rId44"/>
-    <hyperlink ref="H20" r:id="rId45"/>
-    <hyperlink ref="H4" r:id="rId46"/>
-    <hyperlink ref="H13" r:id="rId47"/>
-    <hyperlink ref="H77" r:id="rId48"/>
-    <hyperlink ref="H91" r:id="rId49"/>
-    <hyperlink ref="H94" r:id="rId50"/>
-    <hyperlink ref="H14" r:id="rId51"/>
-    <hyperlink ref="H48" r:id="rId52"/>
-    <hyperlink ref="H69" r:id="rId53"/>
-    <hyperlink ref="H18" r:id="rId54"/>
-    <hyperlink ref="H47" r:id="rId55"/>
-    <hyperlink ref="H34" r:id="rId56"/>
-    <hyperlink ref="H24" r:id="rId57"/>
-    <hyperlink ref="H38" r:id="rId58"/>
-    <hyperlink ref="H33" r:id="rId59"/>
-    <hyperlink ref="H80" r:id="rId60"/>
-    <hyperlink ref="H85" r:id="rId61"/>
-    <hyperlink ref="H84" r:id="rId62"/>
-    <hyperlink ref="H3" r:id="rId63"/>
-    <hyperlink ref="H21" r:id="rId64"/>
-    <hyperlink ref="H67" r:id="rId65"/>
-    <hyperlink ref="H96" r:id="rId66"/>
-    <hyperlink ref="H97" r:id="rId67"/>
-    <hyperlink ref="H147" r:id="rId68"/>
-    <hyperlink ref="H149" r:id="rId69"/>
-    <hyperlink ref="H150" r:id="rId70"/>
-    <hyperlink ref="H148" r:id="rId71"/>
-    <hyperlink ref="H151" r:id="rId72"/>
-    <hyperlink ref="H152" r:id="rId73"/>
-    <hyperlink ref="H153" r:id="rId74"/>
-    <hyperlink ref="H154" r:id="rId75"/>
-    <hyperlink ref="H155" r:id="rId76"/>
-    <hyperlink ref="H157" r:id="rId77"/>
-    <hyperlink ref="H158" r:id="rId78"/>
-    <hyperlink ref="H168" r:id="rId79"/>
-    <hyperlink ref="H169" r:id="rId80"/>
-    <hyperlink ref="H170" r:id="rId81"/>
-    <hyperlink ref="H176" r:id="rId82"/>
+    <hyperlink ref="I40" r:id="rId1"/>
+    <hyperlink ref="I23" r:id="rId2"/>
+    <hyperlink ref="I78" r:id="rId3"/>
+    <hyperlink ref="I65" r:id="rId4"/>
+    <hyperlink ref="I16" r:id="rId5"/>
+    <hyperlink ref="I86" r:id="rId6"/>
+    <hyperlink ref="I45" r:id="rId7"/>
+    <hyperlink ref="I49" r:id="rId8"/>
+    <hyperlink ref="I32" r:id="rId9"/>
+    <hyperlink ref="I43" r:id="rId10"/>
+    <hyperlink ref="I6" r:id="rId11"/>
+    <hyperlink ref="I5" r:id="rId12"/>
+    <hyperlink ref="I10" r:id="rId13"/>
+    <hyperlink ref="I8" r:id="rId14"/>
+    <hyperlink ref="I7" r:id="rId15"/>
+    <hyperlink ref="I9" r:id="rId16"/>
+    <hyperlink ref="I83" r:id="rId17"/>
+    <hyperlink ref="I28" r:id="rId18"/>
+    <hyperlink ref="I64" r:id="rId19"/>
+    <hyperlink ref="I39" r:id="rId20"/>
+    <hyperlink ref="I56" r:id="rId21"/>
+    <hyperlink ref="I87" r:id="rId22"/>
+    <hyperlink ref="I2" r:id="rId23"/>
+    <hyperlink ref="I54" r:id="rId24"/>
+    <hyperlink ref="I70" r:id="rId25"/>
+    <hyperlink ref="I79" r:id="rId26"/>
+    <hyperlink ref="I27" r:id="rId27"/>
+    <hyperlink ref="I17" r:id="rId28"/>
+    <hyperlink ref="I46" r:id="rId29"/>
+    <hyperlink ref="I75" r:id="rId30"/>
+    <hyperlink ref="I50" r:id="rId31"/>
+    <hyperlink ref="I76" r:id="rId32"/>
+    <hyperlink ref="I61" r:id="rId33"/>
+    <hyperlink ref="I92" r:id="rId34"/>
+    <hyperlink ref="I74" r:id="rId35"/>
+    <hyperlink ref="I31" r:id="rId36"/>
+    <hyperlink ref="I60" r:id="rId37"/>
+    <hyperlink ref="I51" r:id="rId38"/>
+    <hyperlink ref="I63" r:id="rId39"/>
+    <hyperlink ref="I88" r:id="rId40"/>
+    <hyperlink ref="I93" r:id="rId41"/>
+    <hyperlink ref="I42" r:id="rId42"/>
+    <hyperlink ref="I72" r:id="rId43"/>
+    <hyperlink ref="I15" r:id="rId44"/>
+    <hyperlink ref="I20" r:id="rId45"/>
+    <hyperlink ref="I4" r:id="rId46"/>
+    <hyperlink ref="I13" r:id="rId47"/>
+    <hyperlink ref="I77" r:id="rId48"/>
+    <hyperlink ref="I91" r:id="rId49"/>
+    <hyperlink ref="I94" r:id="rId50"/>
+    <hyperlink ref="I14" r:id="rId51"/>
+    <hyperlink ref="I48" r:id="rId52"/>
+    <hyperlink ref="I69" r:id="rId53"/>
+    <hyperlink ref="I18" r:id="rId54"/>
+    <hyperlink ref="I47" r:id="rId55"/>
+    <hyperlink ref="I34" r:id="rId56"/>
+    <hyperlink ref="I24" r:id="rId57"/>
+    <hyperlink ref="I38" r:id="rId58"/>
+    <hyperlink ref="I33" r:id="rId59"/>
+    <hyperlink ref="I80" r:id="rId60"/>
+    <hyperlink ref="I85" r:id="rId61"/>
+    <hyperlink ref="I84" r:id="rId62"/>
+    <hyperlink ref="I3" r:id="rId63"/>
+    <hyperlink ref="I21" r:id="rId64"/>
+    <hyperlink ref="I67" r:id="rId65"/>
+    <hyperlink ref="I96" r:id="rId66"/>
+    <hyperlink ref="I97" r:id="rId67"/>
+    <hyperlink ref="I147" r:id="rId68"/>
+    <hyperlink ref="I149" r:id="rId69"/>
+    <hyperlink ref="I150" r:id="rId70"/>
+    <hyperlink ref="I148" r:id="rId71"/>
+    <hyperlink ref="I151" r:id="rId72"/>
+    <hyperlink ref="I152" r:id="rId73"/>
+    <hyperlink ref="I153" r:id="rId74"/>
+    <hyperlink ref="I154" r:id="rId75"/>
+    <hyperlink ref="I155" r:id="rId76"/>
+    <hyperlink ref="I157" r:id="rId77"/>
+    <hyperlink ref="I158" r:id="rId78"/>
+    <hyperlink ref="I168" r:id="rId79"/>
+    <hyperlink ref="I169" r:id="rId80"/>
+    <hyperlink ref="I170" r:id="rId81"/>
+    <hyperlink ref="I176" r:id="rId82"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId83"/>
@@ -10245,8 +10435,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E378"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="F162" sqref="A1:F162"/>
+    <sheetView topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="C134" sqref="C134:C142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -10263,7 +10453,7 @@
         <v>767</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="C1" s="14" t="s">
         <v>736</v>
@@ -10272,7 +10462,7 @@
         <v>645</v>
       </c>
       <c r="E1" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -10322,7 +10512,7 @@
         <v>1</v>
       </c>
       <c r="D5" s="40" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -10336,7 +10526,7 @@
         <v>6</v>
       </c>
       <c r="D6" s="40" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -10350,7 +10540,7 @@
         <v>9</v>
       </c>
       <c r="D7" s="40" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -10364,7 +10554,7 @@
         <v>12</v>
       </c>
       <c r="D8" s="40" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -10378,7 +10568,7 @@
         <v>15</v>
       </c>
       <c r="D9" s="40" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -10392,7 +10582,7 @@
         <v>18</v>
       </c>
       <c r="D10" s="40" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -10470,7 +10660,7 @@
         <v>23</v>
       </c>
       <c r="D16" s="40" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -10546,7 +10736,7 @@
         <v>643</v>
       </c>
       <c r="D22" s="44" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -10560,7 +10750,7 @@
         <v>28</v>
       </c>
       <c r="D23" s="40" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -10626,7 +10816,7 @@
         <v>74</v>
       </c>
       <c r="D28" s="40" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -10680,7 +10870,7 @@
         <v>32</v>
       </c>
       <c r="D32" s="40" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -10718,7 +10908,7 @@
         <v>646</v>
       </c>
       <c r="D35" s="44" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -10770,7 +10960,7 @@
         <v>79</v>
       </c>
       <c r="D39" s="40" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -10784,7 +10974,7 @@
         <v>37</v>
       </c>
       <c r="D40" s="40" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -10824,7 +11014,7 @@
         <v>42</v>
       </c>
       <c r="D43" s="40" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -10852,7 +11042,7 @@
         <v>47</v>
       </c>
       <c r="D45" s="40" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -10902,7 +11092,7 @@
         <v>52</v>
       </c>
       <c r="D49" s="40" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -10940,7 +11130,7 @@
         <v>654</v>
       </c>
       <c r="D52" s="44" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -10994,7 +11184,7 @@
         <v>84</v>
       </c>
       <c r="D56" s="40" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -11098,7 +11288,7 @@
         <v>89</v>
       </c>
       <c r="D64" s="40" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -11112,7 +11302,7 @@
         <v>57</v>
       </c>
       <c r="D65" s="40" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -11126,7 +11316,7 @@
         <v>648</v>
       </c>
       <c r="D66" s="44" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -11216,7 +11406,7 @@
         <v>653</v>
       </c>
       <c r="D73" s="44" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -11278,7 +11468,7 @@
         <v>61</v>
       </c>
       <c r="D78" s="48" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
     </row>
     <row r="79" spans="1:4">
@@ -11318,7 +11508,7 @@
         <v>650</v>
       </c>
       <c r="D81" s="44" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
     </row>
     <row r="82" spans="1:4">
@@ -11332,7 +11522,7 @@
         <v>94</v>
       </c>
       <c r="D82" s="40" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
     </row>
     <row r="83" spans="1:4">
@@ -11370,7 +11560,7 @@
         <v>64</v>
       </c>
       <c r="D85" s="40" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
     </row>
     <row r="86" spans="1:4">
@@ -11384,7 +11574,7 @@
         <v>98</v>
       </c>
       <c r="D86" s="40" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
     </row>
     <row r="87" spans="1:4">
@@ -11486,7 +11676,7 @@
         <v>67</v>
       </c>
       <c r="D94" s="14" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
     </row>
     <row r="95" spans="1:4">
@@ -11500,7 +11690,7 @@
         <v>695</v>
       </c>
       <c r="D95" s="14" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
     </row>
     <row r="96" spans="1:4">
@@ -11597,10 +11787,10 @@
         <v>711</v>
       </c>
       <c r="C103" s="14" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="D103" s="14" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
     </row>
     <row r="104" spans="1:4">
@@ -11743,7 +11933,7 @@
         <v>768</v>
       </c>
       <c r="C115" s="14" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="D115" s="14" t="s">
         <v>776</v>
@@ -11757,7 +11947,7 @@
         <v>769</v>
       </c>
       <c r="C116" s="14" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="D116" s="14" t="s">
         <v>777</v>
@@ -11912,10 +12102,10 @@
         <v>160</v>
       </c>
       <c r="B129" s="13" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="C129" s="14" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="D129" s="14"/>
     </row>
@@ -11925,7 +12115,7 @@
       </c>
       <c r="B130" s="13"/>
       <c r="C130" s="14" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="D130" s="14"/>
     </row>
@@ -11935,7 +12125,7 @@
       </c>
       <c r="B131" s="13"/>
       <c r="C131" s="14" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="D131" s="14"/>
     </row>
@@ -11945,7 +12135,7 @@
       </c>
       <c r="B132" s="13"/>
       <c r="C132" s="14" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="D132" s="14"/>
     </row>
@@ -11955,53 +12145,114 @@
       </c>
       <c r="B133" s="13"/>
       <c r="C133" s="14" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="D133" s="14"/>
     </row>
     <row r="134" spans="1:4">
+      <c r="A134">
+        <v>165</v>
+      </c>
       <c r="B134" s="15"/>
-      <c r="C134" s="9"/>
+      <c r="C134" s="9" t="s">
+        <v>954</v>
+      </c>
       <c r="D134" s="9"/>
     </row>
     <row r="135" spans="1:4">
-      <c r="B135" s="67"/>
-      <c r="C135" s="68"/>
+      <c r="A135">
+        <v>166</v>
+      </c>
+      <c r="B135" s="56" t="s">
+        <v>105</v>
+      </c>
+      <c r="C135" s="57" t="s">
+        <v>585</v>
+      </c>
       <c r="D135" s="68"/>
     </row>
     <row r="136" spans="1:4">
-      <c r="B136" s="67"/>
-      <c r="C136" s="68"/>
+      <c r="A136">
+        <v>167</v>
+      </c>
+      <c r="B136" s="59" t="s">
+        <v>138</v>
+      </c>
+      <c r="C136" s="60" t="s">
+        <v>676</v>
+      </c>
       <c r="D136" s="68"/>
     </row>
     <row r="137" spans="1:4">
-      <c r="B137" s="67"/>
-      <c r="C137" s="68"/>
+      <c r="A137">
+        <v>168</v>
+      </c>
+      <c r="B137" s="61" t="s">
+        <v>140</v>
+      </c>
+      <c r="C137" s="62" t="s">
+        <v>683</v>
+      </c>
       <c r="D137" s="68"/>
     </row>
     <row r="138" spans="1:4">
-      <c r="B138" s="67"/>
-      <c r="C138" s="68"/>
+      <c r="A138">
+        <v>169</v>
+      </c>
+      <c r="B138" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="C138" s="4" t="s">
+        <v>701</v>
+      </c>
       <c r="D138" s="68"/>
     </row>
     <row r="139" spans="1:4">
-      <c r="B139" s="67"/>
-      <c r="C139" s="68"/>
+      <c r="A139">
+        <v>170</v>
+      </c>
+      <c r="B139" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="C139" s="4" t="s">
+        <v>825</v>
+      </c>
       <c r="D139" s="68"/>
     </row>
     <row r="140" spans="1:4">
-      <c r="B140" s="67"/>
-      <c r="C140" s="68"/>
+      <c r="A140">
+        <v>171</v>
+      </c>
+      <c r="B140" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="C140" s="4" t="s">
+        <v>859</v>
+      </c>
       <c r="D140" s="68"/>
     </row>
     <row r="141" spans="1:4">
-      <c r="B141" s="67"/>
-      <c r="C141" s="68"/>
+      <c r="A141">
+        <v>172</v>
+      </c>
+      <c r="B141" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="C141" s="4" t="s">
+        <v>869</v>
+      </c>
       <c r="D141" s="68"/>
     </row>
     <row r="142" spans="1:4">
-      <c r="B142" s="67"/>
-      <c r="C142" s="68"/>
+      <c r="A142">
+        <v>173</v>
+      </c>
+      <c r="B142" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="C142" s="4" t="s">
+        <v>871</v>
+      </c>
       <c r="D142" s="68"/>
     </row>
     <row r="143" spans="1:4">
@@ -13198,8 +13449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J129"/>
   <sheetViews>
-    <sheetView topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="C123" sqref="A3:C123"/>
+    <sheetView topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -13209,8 +13460,8 @@
     <col min="3" max="3" width="12.5" style="1" customWidth="1"/>
     <col min="4" max="4" width="12.125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="44.5" style="1" customWidth="1"/>
-    <col min="7" max="7" width="47.875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="41" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5" style="1" customWidth="1"/>
     <col min="8" max="8" width="10.75" style="1" customWidth="1"/>
     <col min="11" max="16384" width="9" style="1"/>
   </cols>
@@ -13280,7 +13531,7 @@
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" hidden="1">
       <c r="A4" s="4" t="s">
         <v>105</v>
       </c>
@@ -13295,7 +13546,9 @@
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="4"/>
-      <c r="G4" s="5"/>
+      <c r="G4" s="5">
+        <v>1</v>
+      </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
     </row>
@@ -13975,7 +14228,7 @@
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" hidden="1">
       <c r="A41" s="4" t="s">
         <v>138</v>
       </c>
@@ -13988,11 +14241,13 @@
       <c r="D41" s="5"/>
       <c r="E41" s="5"/>
       <c r="F41" s="4"/>
-      <c r="G41" s="5"/>
+      <c r="G41" s="5">
+        <v>1</v>
+      </c>
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" ht="12.75" customHeight="1">
       <c r="A42" s="4" t="s">
         <v>139</v>
       </c>
@@ -14011,7 +14266,7 @@
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" hidden="1">
       <c r="A43" s="4" t="s">
         <v>140</v>
       </c>
@@ -14026,7 +14281,9 @@
       <c r="F43" s="7" t="s">
         <v>684</v>
       </c>
-      <c r="G43" s="5"/>
+      <c r="G43" s="5">
+        <v>1</v>
+      </c>
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
     </row>
@@ -14047,7 +14304,7 @@
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" hidden="1">
       <c r="A45" s="4" t="s">
         <v>141</v>
       </c>
@@ -14062,7 +14319,9 @@
       <c r="F45" s="7" t="s">
         <v>702</v>
       </c>
-      <c r="G45" s="5"/>
+      <c r="G45" s="5">
+        <v>1</v>
+      </c>
       <c r="I45" s="1"/>
       <c r="J45" s="1"/>
     </row>
@@ -14404,7 +14663,7 @@
       <c r="I63" s="1"/>
       <c r="J63" s="1"/>
     </row>
-    <row r="64" spans="1:10">
+    <row r="64" spans="1:10" hidden="1">
       <c r="A64" s="4" t="s">
         <v>155</v>
       </c>
@@ -14419,7 +14678,9 @@
       <c r="F64" s="7" t="s">
         <v>824</v>
       </c>
-      <c r="G64" s="5"/>
+      <c r="G64" s="5">
+        <v>1</v>
+      </c>
       <c r="I64" s="1"/>
       <c r="J64" s="1"/>
     </row>
@@ -14775,7 +15036,7 @@
       <c r="I82" s="1"/>
       <c r="J82" s="1"/>
     </row>
-    <row r="83" spans="1:10">
+    <row r="83" spans="1:10" hidden="1">
       <c r="A83" s="4" t="s">
         <v>172</v>
       </c>
@@ -14790,7 +15051,9 @@
       <c r="F83" s="7" t="s">
         <v>860</v>
       </c>
-      <c r="G83" s="5"/>
+      <c r="G83" s="5">
+        <v>1</v>
+      </c>
       <c r="I83" s="1"/>
       <c r="J83" s="1"/>
     </row>
@@ -14893,7 +15156,7 @@
       <c r="I88" s="1"/>
       <c r="J88" s="1"/>
     </row>
-    <row r="89" spans="1:10">
+    <row r="89" spans="1:10" hidden="1">
       <c r="A89" s="4" t="s">
         <v>178</v>
       </c>
@@ -14908,7 +15171,9 @@
       <c r="F89" s="7" t="s">
         <v>870</v>
       </c>
-      <c r="G89" s="5"/>
+      <c r="G89" s="5">
+        <v>1</v>
+      </c>
       <c r="I89" s="1"/>
       <c r="J89" s="1"/>
     </row>
@@ -14986,7 +15251,7 @@
       <c r="I93" s="1"/>
       <c r="J93" s="1"/>
     </row>
-    <row r="94" spans="1:10">
+    <row r="94" spans="1:10" hidden="1">
       <c r="A94" s="4" t="s">
         <v>181</v>
       </c>
@@ -15001,7 +15266,9 @@
       <c r="F94" s="7" t="s">
         <v>873</v>
       </c>
-      <c r="G94" s="5"/>
+      <c r="G94" s="5">
+        <v>1</v>
+      </c>
       <c r="I94" s="1"/>
       <c r="J94" s="1"/>
     </row>

</xml_diff>

<commit_message>
qqq Signed-off-by: twtcom001 <twtcom001@sina.com>
</commit_message>
<xml_diff>
--- a/统计清单/2017国内编号清单.xlsx
+++ b/统计清单/2017国内编号清单.xlsx
@@ -2712,10 +2712,6 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>Trichocereus Indio Magic MEX33</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
     <t>Hildewintera Humkes Röschen</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
@@ -2809,10 +2805,6 @@
   </si>
   <si>
     <t>黄金荷花 火焰花色</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Lobivia bit</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
@@ -3582,6 +3574,14 @@
   </si>
   <si>
     <t>Echinopsis</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lobivia bit</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Trichocereus Indio Magic MEX33</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -3936,197 +3936,6 @@
   <dxfs count="18">
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="10"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="4"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -4324,6 +4133,197 @@
         <horizontal/>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="10"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="4"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
@@ -4343,14 +4343,14 @@
   <tableColumns count="12">
     <tableColumn id="1" name="145"/>
     <tableColumn id="2" name="属"/>
-    <tableColumn id="3" name="属内编号" dataDxfId="6"/>
-    <tableColumn id="4" name="拉丁名" dataDxfId="5"/>
-    <tableColumn id="5" name="中文" dataDxfId="4"/>
-    <tableColumn id="7" name="来源编号" dataDxfId="3"/>
+    <tableColumn id="3" name="属内编号" dataDxfId="17"/>
+    <tableColumn id="4" name="拉丁名" dataDxfId="16"/>
+    <tableColumn id="5" name="中文" dataDxfId="15"/>
+    <tableColumn id="7" name="来源编号" dataDxfId="14"/>
     <tableColumn id="12" name="引进价格"/>
-    <tableColumn id="6" name="来源" dataDxfId="2"/>
-    <tableColumn id="8" name="参考链接" dataDxfId="1" dataCellStyle="超链接"/>
-    <tableColumn id="10" name="引进尺寸2" dataDxfId="0"/>
+    <tableColumn id="6" name="来源" dataDxfId="13"/>
+    <tableColumn id="8" name="参考链接" dataDxfId="12" dataCellStyle="超链接"/>
+    <tableColumn id="10" name="引进尺寸2" dataDxfId="11"/>
     <tableColumn id="11" name="引进日期"/>
     <tableColumn id="13" name="备注"/>
   </tableColumns>
@@ -4363,9 +4363,9 @@
   <autoFilter ref="A1:E162"/>
   <tableColumns count="5">
     <tableColumn id="1" name="145"/>
-    <tableColumn id="3" name="编号" dataDxfId="17"/>
-    <tableColumn id="5" name="中文" dataDxfId="16"/>
-    <tableColumn id="7" name="来源编号" dataDxfId="15"/>
+    <tableColumn id="3" name="编号" dataDxfId="10"/>
+    <tableColumn id="5" name="中文" dataDxfId="9"/>
+    <tableColumn id="7" name="来源编号" dataDxfId="8"/>
     <tableColumn id="2" name="数量"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -4373,20 +4373,16 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A1:G129" totalsRowShown="0" dataDxfId="14">
-  <autoFilter ref="A1:G129">
-    <filterColumn colId="6">
-      <filters blank="1"/>
-    </filterColumn>
-  </autoFilter>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A1:G129" totalsRowShown="0" dataDxfId="7">
+  <autoFilter ref="A1:G129"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="本地编号" dataDxfId="13"/>
-    <tableColumn id="2" name="编号" dataDxfId="12"/>
-    <tableColumn id="5" name="中文名" dataDxfId="11"/>
-    <tableColumn id="6" name="购买目标" dataDxfId="10"/>
-    <tableColumn id="7" name="来源编号" dataDxfId="9"/>
-    <tableColumn id="4" name="链接" dataDxfId="8"/>
-    <tableColumn id="3" name="购买数量" dataDxfId="7"/>
+    <tableColumn id="1" name="本地编号" dataDxfId="6"/>
+    <tableColumn id="2" name="编号" dataDxfId="5"/>
+    <tableColumn id="5" name="中文名" dataDxfId="4"/>
+    <tableColumn id="6" name="购买目标" dataDxfId="3"/>
+    <tableColumn id="7" name="来源编号" dataDxfId="2"/>
+    <tableColumn id="4" name="链接" dataDxfId="1"/>
+    <tableColumn id="3" name="购买数量" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4681,8 +4677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L186"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C172" workbookViewId="0">
-      <selection activeCell="H179" sqref="H179:H186"/>
+    <sheetView tabSelected="1" topLeftCell="C64" workbookViewId="0">
+      <selection activeCell="E64" sqref="E64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -4703,7 +4699,7 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="3" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>733</v>
@@ -4721,7 +4717,7 @@
         <v>738</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>959</v>
+        <v>957</v>
       </c>
       <c r="H1" s="14" t="s">
         <v>737</v>
@@ -4730,13 +4726,13 @@
         <v>739</v>
       </c>
       <c r="J1" s="14" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="K1" s="27" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -4750,7 +4746,7 @@
         <v>500</v>
       </c>
       <c r="D2" s="40" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="E2" s="40" t="s">
         <v>330</v>
@@ -4780,10 +4776,10 @@
         <v>732</v>
       </c>
       <c r="C3" s="41" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="D3" s="40" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="E3" s="40" t="s">
         <v>468</v>
@@ -4816,7 +4812,7 @@
         <v>501</v>
       </c>
       <c r="D4" s="43" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="E4" s="40" t="s">
         <v>415</v>
@@ -4849,7 +4845,7 @@
         <v>502</v>
       </c>
       <c r="D5" s="40" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="E5" s="40" t="s">
         <v>1</v>
@@ -4884,7 +4880,7 @@
         <v>503</v>
       </c>
       <c r="D6" s="40" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="E6" s="40" t="s">
         <v>6</v>
@@ -4919,7 +4915,7 @@
         <v>504</v>
       </c>
       <c r="D7" s="40" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="E7" s="40" t="s">
         <v>9</v>
@@ -4954,7 +4950,7 @@
         <v>505</v>
       </c>
       <c r="D8" s="40" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="E8" s="40" t="s">
         <v>12</v>
@@ -4989,7 +4985,7 @@
         <v>506</v>
       </c>
       <c r="D9" s="40" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="E9" s="40" t="s">
         <v>15</v>
@@ -5024,7 +5020,7 @@
         <v>507</v>
       </c>
       <c r="D10" s="40" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="E10" s="40" t="s">
         <v>18</v>
@@ -5059,7 +5055,7 @@
         <v>103</v>
       </c>
       <c r="D11" s="43" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="E11" s="43" t="s">
         <v>584</v>
@@ -5849,7 +5845,7 @@
         <v>732</v>
       </c>
       <c r="C36" s="41" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="D36" s="40" t="s">
         <v>418</v>
@@ -7302,7 +7298,7 @@
         <v>568</v>
       </c>
       <c r="E81" s="43" t="s">
-        <v>851</v>
+        <v>849</v>
       </c>
       <c r="F81" s="44" t="s">
         <v>625</v>
@@ -7522,7 +7518,7 @@
         <v>86</v>
       </c>
       <c r="B88" s="38" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="C88" s="42" t="s">
         <v>203</v>
@@ -7751,7 +7747,7 @@
         <v>499</v>
       </c>
       <c r="D95" s="14" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="E95" s="9" t="s">
         <v>67</v>
@@ -8800,7 +8796,7 @@
         <v>320</v>
       </c>
       <c r="D128" s="14" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
       <c r="E128" s="14" t="s">
         <v>272</v>
@@ -9214,7 +9210,7 @@
         <v>741</v>
       </c>
       <c r="D141" s="14" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="E141" s="9"/>
       <c r="F141" s="9">
@@ -9268,7 +9264,7 @@
         <v>510</v>
       </c>
       <c r="D143" s="14" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="E143" s="9"/>
       <c r="F143" s="9">
@@ -9313,7 +9309,7 @@
         <v>132</v>
       </c>
       <c r="B145" s="38" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="C145" s="41" t="s">
         <v>699</v>
@@ -9336,16 +9332,16 @@
         <v>133</v>
       </c>
       <c r="B146" s="38" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="C146" s="50" t="s">
+        <v>793</v>
+      </c>
+      <c r="D146" s="51" t="s">
+        <v>749</v>
+      </c>
+      <c r="E146" s="51" t="s">
         <v>795</v>
-      </c>
-      <c r="D146" s="51" t="s">
-        <v>750</v>
-      </c>
-      <c r="E146" s="51" t="s">
-        <v>797</v>
       </c>
       <c r="F146" s="51"/>
       <c r="G146" s="17"/>
@@ -9395,7 +9391,7 @@
         <v>496</v>
       </c>
       <c r="D148" s="14" t="s">
-        <v>748</v>
+        <v>961</v>
       </c>
       <c r="E148" s="14" t="s">
         <v>488</v>
@@ -9503,7 +9499,7 @@
         <v>717</v>
       </c>
       <c r="D152" s="14" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="E152" s="14" t="s">
         <v>716</v>
@@ -9527,7 +9523,7 @@
         <v>719</v>
       </c>
       <c r="D153" s="14" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="E153" s="14" t="s">
         <v>721</v>
@@ -9551,7 +9547,7 @@
         <v>724</v>
       </c>
       <c r="D154" s="14" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="E154" s="14" t="s">
         <v>722</v>
@@ -9593,16 +9589,16 @@
         <v>143</v>
       </c>
       <c r="B156" s="52" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="C156" s="53" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="D156" s="54" t="s">
         <v>730</v>
       </c>
       <c r="E156" s="54" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="F156" s="9"/>
       <c r="G156" s="9"/>
@@ -9618,21 +9614,21 @@
         <v>743</v>
       </c>
       <c r="C157" s="13" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="D157" s="9" t="s">
+        <v>759</v>
+      </c>
+      <c r="E157" s="9" t="s">
         <v>760</v>
-      </c>
-      <c r="E157" s="9" t="s">
-        <v>761</v>
       </c>
       <c r="F157" s="9"/>
       <c r="G157" s="9"/>
       <c r="H157" s="9" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="I157" s="37" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="J157" s="9"/>
     </row>
@@ -9641,24 +9637,24 @@
         <v>145</v>
       </c>
       <c r="B158" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="C158" s="15" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="D158" s="9" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="E158" s="9" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="F158" s="9"/>
       <c r="G158" s="9"/>
       <c r="H158" s="9" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="I158" s="37" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="J158" s="9"/>
     </row>
@@ -9670,20 +9666,20 @@
         <v>742</v>
       </c>
       <c r="C159" s="15" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="D159" s="9" t="s">
+        <v>770</v>
+      </c>
+      <c r="E159" s="9" t="s">
         <v>771</v>
       </c>
-      <c r="E159" s="9" t="s">
-        <v>772</v>
-      </c>
       <c r="F159" s="9" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="G159" s="9"/>
       <c r="H159" s="9" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="I159" s="36"/>
       <c r="J159" s="9"/>
@@ -9696,20 +9692,20 @@
         <v>742</v>
       </c>
       <c r="C160" s="15" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="D160" s="9" t="s">
-        <v>773</v>
+        <v>960</v>
       </c>
       <c r="E160" s="9" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="F160" s="9" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="G160" s="9"/>
       <c r="H160" s="9" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="I160" s="36"/>
       <c r="J160" s="9"/>
@@ -9719,14 +9715,14 @@
         <v>148</v>
       </c>
       <c r="B161" s="38" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="C161" s="41" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="D161" s="40"/>
       <c r="E161" s="40" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="F161" s="14"/>
       <c r="G161" s="14"/>
@@ -9739,14 +9735,14 @@
         <v>149</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="C162" s="13" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="D162" s="14"/>
       <c r="E162" s="14" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="F162" s="14"/>
       <c r="G162" s="14"/>
@@ -9759,14 +9755,14 @@
         <v>150</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="C163" s="13" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="D163" s="14"/>
       <c r="E163" s="14" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -9779,14 +9775,14 @@
         <v>151</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="C164" s="13" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="D164" s="14"/>
       <c r="E164" s="14" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="F164" s="14"/>
       <c r="G164" s="14"/>
@@ -9799,14 +9795,14 @@
         <v>152</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="C165" s="13" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="D165" s="14"/>
       <c r="E165" s="14" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="F165" s="14"/>
       <c r="G165" s="14"/>
@@ -9819,14 +9815,14 @@
         <v>153</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="C166" s="13" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="D166" s="14"/>
       <c r="E166" s="14" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="F166" s="14"/>
       <c r="G166" s="14"/>
@@ -9839,14 +9835,14 @@
         <v>154</v>
       </c>
       <c r="B167" s="38" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="C167" s="41" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="D167" s="40"/>
       <c r="E167" s="40" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="F167" s="14"/>
       <c r="G167" s="14"/>
@@ -9859,7 +9855,7 @@
         <v>155</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="C168" s="56" t="s">
         <v>125</v>
@@ -9875,7 +9871,7 @@
         <v>50</v>
       </c>
       <c r="H168" s="9" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
       <c r="I168" s="58" t="s">
         <v>681</v>
@@ -9890,16 +9886,16 @@
         <v>156</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="C169" s="59" t="s">
         <v>175</v>
       </c>
       <c r="D169" s="60" t="s">
-        <v>862</v>
+        <v>860</v>
       </c>
       <c r="E169" s="60" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
       <c r="F169" s="14"/>
       <c r="G169" s="14">
@@ -9909,7 +9905,7 @@
         <v>482</v>
       </c>
       <c r="I169" s="55" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
       <c r="J169" s="14"/>
       <c r="K169" s="66">
@@ -9921,16 +9917,16 @@
         <v>157</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
       <c r="C170" s="59" t="s">
         <v>186</v>
       </c>
       <c r="D170" s="60" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
       <c r="E170" s="60" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14">
@@ -9940,7 +9936,7 @@
         <v>482</v>
       </c>
       <c r="I170" s="55" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
       <c r="J170" s="14"/>
       <c r="K170" s="66">
@@ -9952,7 +9948,7 @@
         <v>158</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="C171" s="61" t="s">
         <v>187</v>
@@ -9981,7 +9977,7 @@
         <v>159</v>
       </c>
       <c r="B172" s="3" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
       <c r="C172" s="59" t="s">
         <v>202</v>
@@ -10010,16 +10006,16 @@
         <v>160</v>
       </c>
       <c r="B173" s="3" t="s">
+        <v>904</v>
+      </c>
+      <c r="C173" s="13" t="s">
+        <v>903</v>
+      </c>
+      <c r="D173" s="14" t="s">
+        <v>905</v>
+      </c>
+      <c r="E173" s="14" t="s">
         <v>906</v>
-      </c>
-      <c r="C173" s="13" t="s">
-        <v>905</v>
-      </c>
-      <c r="D173" s="14" t="s">
-        <v>907</v>
-      </c>
-      <c r="E173" s="14" t="s">
-        <v>908</v>
       </c>
       <c r="F173" s="14"/>
       <c r="G173" s="14"/>
@@ -10034,14 +10030,14 @@
         <v>161</v>
       </c>
       <c r="B174" s="3" t="s">
-        <v>957</v>
+        <v>955</v>
       </c>
       <c r="C174" s="13"/>
       <c r="D174" s="14" t="s">
-        <v>958</v>
+        <v>956</v>
       </c>
       <c r="E174" s="14" t="s">
-        <v>909</v>
+        <v>907</v>
       </c>
       <c r="F174" s="14"/>
       <c r="G174" s="14"/>
@@ -10056,12 +10052,12 @@
         <v>162</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="C175" s="13"/>
       <c r="D175" s="14"/>
       <c r="E175" s="14" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="F175" s="14"/>
       <c r="G175" s="14"/>
@@ -10074,20 +10070,20 @@
         <v>163</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="C176" s="13"/>
       <c r="D176" s="14" t="s">
-        <v>956</v>
+        <v>954</v>
       </c>
       <c r="E176" s="14" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="F176" s="14"/>
       <c r="G176" s="14"/>
       <c r="H176" s="14"/>
       <c r="I176" s="37" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="J176" s="14"/>
     </row>
@@ -10096,14 +10092,14 @@
         <v>164</v>
       </c>
       <c r="B177" s="3" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
       <c r="C177" s="13"/>
       <c r="D177" s="14" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="E177" s="14" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="F177" s="14"/>
       <c r="G177" s="14"/>
@@ -10116,12 +10112,12 @@
         <v>165</v>
       </c>
       <c r="B178" s="3" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="C178" s="15"/>
       <c r="D178" s="9"/>
       <c r="E178" s="9" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
       <c r="F178" s="9"/>
       <c r="G178" s="9"/>
@@ -10134,7 +10130,7 @@
         <v>166</v>
       </c>
       <c r="B179" t="s">
-        <v>960</v>
+        <v>958</v>
       </c>
       <c r="C179" s="56" t="s">
         <v>105</v>
@@ -10160,7 +10156,7 @@
         <v>167</v>
       </c>
       <c r="B180" t="s">
-        <v>960</v>
+        <v>958</v>
       </c>
       <c r="C180" s="59" t="s">
         <v>138</v>
@@ -10186,7 +10182,7 @@
         <v>168</v>
       </c>
       <c r="B181" t="s">
-        <v>960</v>
+        <v>958</v>
       </c>
       <c r="C181" s="61" t="s">
         <v>140</v>
@@ -10212,7 +10208,7 @@
         <v>169</v>
       </c>
       <c r="B182" t="s">
-        <v>960</v>
+        <v>958</v>
       </c>
       <c r="C182" s="4" t="s">
         <v>141</v>
@@ -10238,16 +10234,16 @@
         <v>170</v>
       </c>
       <c r="B183" t="s">
-        <v>960</v>
+        <v>958</v>
       </c>
       <c r="C183" s="4" t="s">
         <v>155</v>
       </c>
       <c r="D183" s="4" t="s">
+        <v>821</v>
+      </c>
+      <c r="E183" s="4" t="s">
         <v>823</v>
-      </c>
-      <c r="E183" s="4" t="s">
-        <v>825</v>
       </c>
       <c r="F183" s="14"/>
       <c r="G183">
@@ -10264,7 +10260,7 @@
         <v>171</v>
       </c>
       <c r="B184" t="s">
-        <v>960</v>
+        <v>958</v>
       </c>
       <c r="C184" s="4" t="s">
         <v>172</v>
@@ -10273,7 +10269,7 @@
         <v>670</v>
       </c>
       <c r="E184" s="4" t="s">
-        <v>859</v>
+        <v>857</v>
       </c>
       <c r="F184" s="14"/>
       <c r="G184">
@@ -10290,16 +10286,16 @@
         <v>172</v>
       </c>
       <c r="B185" t="s">
-        <v>960</v>
+        <v>958</v>
       </c>
       <c r="C185" s="4" t="s">
         <v>178</v>
       </c>
       <c r="D185" s="4" t="s">
-        <v>868</v>
+        <v>866</v>
       </c>
       <c r="E185" s="4" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
       <c r="F185" s="14"/>
       <c r="G185">
@@ -10316,16 +10312,16 @@
         <v>173</v>
       </c>
       <c r="B186" t="s">
-        <v>960</v>
+        <v>958</v>
       </c>
       <c r="C186" s="4" t="s">
         <v>181</v>
       </c>
       <c r="D186" s="4" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
       <c r="E186" s="4" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
       <c r="F186" s="14"/>
       <c r="G186">
@@ -10450,10 +10446,10 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="3" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>952</v>
+        <v>950</v>
       </c>
       <c r="C1" s="14" t="s">
         <v>736</v>
@@ -10462,7 +10458,7 @@
         <v>645</v>
       </c>
       <c r="E1" t="s">
-        <v>953</v>
+        <v>951</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -10482,7 +10478,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="41" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="C3" s="40" t="s">
         <v>468</v>
@@ -10512,7 +10508,7 @@
         <v>1</v>
       </c>
       <c r="D5" s="40" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -10526,7 +10522,7 @@
         <v>6</v>
       </c>
       <c r="D6" s="40" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -10540,7 +10536,7 @@
         <v>9</v>
       </c>
       <c r="D7" s="40" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -10554,7 +10550,7 @@
         <v>12</v>
       </c>
       <c r="D8" s="40" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -10568,7 +10564,7 @@
         <v>15</v>
       </c>
       <c r="D9" s="40" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -10582,7 +10578,7 @@
         <v>18</v>
       </c>
       <c r="D10" s="40" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -10660,7 +10656,7 @@
         <v>23</v>
       </c>
       <c r="D16" s="40" t="s">
-        <v>949</v>
+        <v>947</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -10736,7 +10732,7 @@
         <v>643</v>
       </c>
       <c r="D22" s="44" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -10750,7 +10746,7 @@
         <v>28</v>
       </c>
       <c r="D23" s="40" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -10816,7 +10812,7 @@
         <v>74</v>
       </c>
       <c r="D28" s="40" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -10870,7 +10866,7 @@
         <v>32</v>
       </c>
       <c r="D32" s="40" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -10908,7 +10904,7 @@
         <v>646</v>
       </c>
       <c r="D35" s="44" t="s">
-        <v>944</v>
+        <v>942</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -10916,7 +10912,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="41" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="C36" s="40" t="s">
         <v>391</v>
@@ -10960,7 +10956,7 @@
         <v>79</v>
       </c>
       <c r="D39" s="40" t="s">
-        <v>943</v>
+        <v>941</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -10974,7 +10970,7 @@
         <v>37</v>
       </c>
       <c r="D40" s="40" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -11014,7 +11010,7 @@
         <v>42</v>
       </c>
       <c r="D43" s="40" t="s">
-        <v>941</v>
+        <v>939</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -11042,7 +11038,7 @@
         <v>47</v>
       </c>
       <c r="D45" s="40" t="s">
-        <v>940</v>
+        <v>938</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -11092,7 +11088,7 @@
         <v>52</v>
       </c>
       <c r="D49" s="40" t="s">
-        <v>939</v>
+        <v>937</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -11130,7 +11126,7 @@
         <v>654</v>
       </c>
       <c r="D52" s="44" t="s">
-        <v>938</v>
+        <v>936</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -11184,7 +11180,7 @@
         <v>84</v>
       </c>
       <c r="D56" s="40" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -11288,7 +11284,7 @@
         <v>89</v>
       </c>
       <c r="D64" s="40" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -11302,7 +11298,7 @@
         <v>57</v>
       </c>
       <c r="D65" s="40" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -11316,7 +11312,7 @@
         <v>648</v>
       </c>
       <c r="D66" s="44" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -11406,7 +11402,7 @@
         <v>653</v>
       </c>
       <c r="D73" s="44" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -11468,7 +11464,7 @@
         <v>61</v>
       </c>
       <c r="D78" s="48" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
     </row>
     <row r="79" spans="1:4">
@@ -11491,7 +11487,7 @@
         <v>198</v>
       </c>
       <c r="C80" s="43" t="s">
-        <v>851</v>
+        <v>849</v>
       </c>
       <c r="D80" s="44" t="s">
         <v>625</v>
@@ -11508,7 +11504,7 @@
         <v>650</v>
       </c>
       <c r="D81" s="44" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
     </row>
     <row r="82" spans="1:4">
@@ -11522,7 +11518,7 @@
         <v>94</v>
       </c>
       <c r="D82" s="40" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
     </row>
     <row r="83" spans="1:4">
@@ -11560,7 +11556,7 @@
         <v>64</v>
       </c>
       <c r="D85" s="40" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
     </row>
     <row r="86" spans="1:4">
@@ -11574,7 +11570,7 @@
         <v>98</v>
       </c>
       <c r="D86" s="40" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
     </row>
     <row r="87" spans="1:4">
@@ -11676,7 +11672,7 @@
         <v>67</v>
       </c>
       <c r="D94" s="14" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
     </row>
     <row r="95" spans="1:4">
@@ -11690,7 +11686,7 @@
         <v>695</v>
       </c>
       <c r="D95" s="14" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
     </row>
     <row r="96" spans="1:4">
@@ -11772,10 +11768,10 @@
         <v>133</v>
       </c>
       <c r="B102" s="50" t="s">
+        <v>793</v>
+      </c>
+      <c r="C102" s="51" t="s">
         <v>795</v>
-      </c>
-      <c r="C102" s="51" t="s">
-        <v>797</v>
       </c>
       <c r="D102" s="51"/>
     </row>
@@ -11787,10 +11783,10 @@
         <v>711</v>
       </c>
       <c r="C103" s="14" t="s">
-        <v>926</v>
+        <v>924</v>
       </c>
       <c r="D103" s="14" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
     </row>
     <row r="104" spans="1:4">
@@ -11894,10 +11890,10 @@
         <v>143</v>
       </c>
       <c r="B112" s="53" t="s">
+        <v>753</v>
+      </c>
+      <c r="C112" s="54" t="s">
         <v>754</v>
-      </c>
-      <c r="C112" s="54" t="s">
-        <v>755</v>
       </c>
       <c r="D112" s="9"/>
     </row>
@@ -11906,10 +11902,10 @@
         <v>144</v>
       </c>
       <c r="B113" s="13" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="C113" s="9" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="D113" s="9"/>
     </row>
@@ -11918,10 +11914,10 @@
         <v>145</v>
       </c>
       <c r="B114" s="15" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="C114" s="9" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="D114" s="9"/>
     </row>
@@ -11930,13 +11926,13 @@
         <v>146</v>
       </c>
       <c r="B115" s="15" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="C115" s="14" t="s">
-        <v>950</v>
+        <v>948</v>
       </c>
       <c r="D115" s="14" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
     </row>
     <row r="116" spans="1:4">
@@ -11944,13 +11940,13 @@
         <v>147</v>
       </c>
       <c r="B116" s="15" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="C116" s="14" t="s">
-        <v>951</v>
+        <v>949</v>
       </c>
       <c r="D116" s="14" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
     </row>
     <row r="117" spans="1:4">
@@ -11958,10 +11954,10 @@
         <v>148</v>
       </c>
       <c r="B117" s="41" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="C117" s="40" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="D117" s="14"/>
     </row>
@@ -11970,10 +11966,10 @@
         <v>149</v>
       </c>
       <c r="B118" s="13" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="C118" s="14" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="D118" s="14"/>
     </row>
@@ -11982,10 +11978,10 @@
         <v>150</v>
       </c>
       <c r="B119" s="13" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="C119" s="14" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="D119" s="14"/>
     </row>
@@ -11994,10 +11990,10 @@
         <v>151</v>
       </c>
       <c r="B120" s="13" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="C120" s="14" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="D120" s="14"/>
     </row>
@@ -12006,10 +12002,10 @@
         <v>152</v>
       </c>
       <c r="B121" s="13" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="C121" s="14" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="D121" s="14"/>
     </row>
@@ -12018,10 +12014,10 @@
         <v>153</v>
       </c>
       <c r="B122" s="13" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="C122" s="14" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="D122" s="14"/>
     </row>
@@ -12030,10 +12026,10 @@
         <v>154</v>
       </c>
       <c r="B123" s="41" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="C123" s="40" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="D123" s="14"/>
     </row>
@@ -12057,7 +12053,7 @@
         <v>175</v>
       </c>
       <c r="C125" s="60" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
       <c r="D125" s="14"/>
     </row>
@@ -12069,7 +12065,7 @@
         <v>186</v>
       </c>
       <c r="C126" s="60" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
       <c r="D126" s="14"/>
     </row>
@@ -12102,10 +12098,10 @@
         <v>160</v>
       </c>
       <c r="B129" s="13" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="C129" s="14" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
       <c r="D129" s="14"/>
     </row>
@@ -12115,7 +12111,7 @@
       </c>
       <c r="B130" s="13"/>
       <c r="C130" s="14" t="s">
-        <v>909</v>
+        <v>907</v>
       </c>
       <c r="D130" s="14"/>
     </row>
@@ -12125,7 +12121,7 @@
       </c>
       <c r="B131" s="13"/>
       <c r="C131" s="14" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="D131" s="14"/>
     </row>
@@ -12135,7 +12131,7 @@
       </c>
       <c r="B132" s="13"/>
       <c r="C132" s="14" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="D132" s="14"/>
     </row>
@@ -12145,7 +12141,7 @@
       </c>
       <c r="B133" s="13"/>
       <c r="C133" s="14" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="D133" s="14"/>
     </row>
@@ -12155,7 +12151,7 @@
       </c>
       <c r="B134" s="15"/>
       <c r="C134" s="9" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
       <c r="D134" s="9"/>
     </row>
@@ -12215,7 +12211,7 @@
         <v>155</v>
       </c>
       <c r="C139" s="4" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="D139" s="68"/>
     </row>
@@ -12227,7 +12223,7 @@
         <v>172</v>
       </c>
       <c r="C140" s="4" t="s">
-        <v>859</v>
+        <v>857</v>
       </c>
       <c r="D140" s="68"/>
     </row>
@@ -12239,7 +12235,7 @@
         <v>178</v>
       </c>
       <c r="C141" s="4" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
       <c r="D141" s="68"/>
     </row>
@@ -12251,7 +12247,7 @@
         <v>181</v>
       </c>
       <c r="C142" s="4" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
       <c r="D142" s="68"/>
     </row>
@@ -13449,8 +13445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J129"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A123"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -13491,7 +13487,7 @@
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:10" hidden="1">
+    <row r="2" spans="1:10">
       <c r="A2" s="4" t="s">
         <v>103</v>
       </c>
@@ -13531,7 +13527,7 @@
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:10" hidden="1">
+    <row r="4" spans="1:10">
       <c r="A4" s="4" t="s">
         <v>105</v>
       </c>
@@ -13552,7 +13548,7 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:10" hidden="1">
+    <row r="5" spans="1:10">
       <c r="A5" s="4" t="s">
         <v>106</v>
       </c>
@@ -13575,7 +13571,7 @@
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:10" hidden="1">
+    <row r="6" spans="1:10">
       <c r="A6" s="4" t="s">
         <v>107</v>
       </c>
@@ -13592,7 +13588,7 @@
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="1:10" hidden="1">
+    <row r="7" spans="1:10">
       <c r="A7" s="4" t="s">
         <v>108</v>
       </c>
@@ -13609,7 +13605,7 @@
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="1:10" hidden="1">
+    <row r="8" spans="1:10">
       <c r="A8" s="4" t="s">
         <v>109</v>
       </c>
@@ -13626,7 +13622,7 @@
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="1:10" hidden="1">
+    <row r="9" spans="1:10">
       <c r="A9" s="4" t="s">
         <v>21</v>
       </c>
@@ -13660,7 +13656,7 @@
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
     </row>
-    <row r="11" spans="1:10" hidden="1">
+    <row r="11" spans="1:10">
       <c r="A11" s="4" t="s">
         <v>111</v>
       </c>
@@ -13694,7 +13690,7 @@
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
     </row>
-    <row r="13" spans="1:10" hidden="1">
+    <row r="13" spans="1:10">
       <c r="A13" s="4" t="s">
         <v>113</v>
       </c>
@@ -13711,7 +13707,7 @@
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
     </row>
-    <row r="14" spans="1:10" hidden="1">
+    <row r="14" spans="1:10">
       <c r="A14" s="4" t="s">
         <v>114</v>
       </c>
@@ -13751,7 +13747,7 @@
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
     </row>
-    <row r="16" spans="1:10" hidden="1">
+    <row r="16" spans="1:10">
       <c r="A16" s="4" t="s">
         <v>116</v>
       </c>
@@ -13785,7 +13781,7 @@
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
     </row>
-    <row r="18" spans="1:10" hidden="1">
+    <row r="18" spans="1:10">
       <c r="A18" s="4" t="s">
         <v>118</v>
       </c>
@@ -13836,7 +13832,7 @@
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
     </row>
-    <row r="21" spans="1:10" hidden="1">
+    <row r="21" spans="1:10">
       <c r="A21" s="4" t="s">
         <v>121</v>
       </c>
@@ -13859,7 +13855,7 @@
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
     </row>
-    <row r="22" spans="1:10" hidden="1">
+    <row r="22" spans="1:10">
       <c r="A22" s="4" t="s">
         <v>26</v>
       </c>
@@ -13876,7 +13872,7 @@
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
     </row>
-    <row r="23" spans="1:10" hidden="1">
+    <row r="23" spans="1:10">
       <c r="A23" s="4" t="s">
         <v>122</v>
       </c>
@@ -13914,7 +13910,7 @@
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
     </row>
-    <row r="25" spans="1:10" hidden="1">
+    <row r="25" spans="1:10">
       <c r="A25" s="4" t="s">
         <v>124</v>
       </c>
@@ -13937,7 +13933,7 @@
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
     </row>
-    <row r="26" spans="1:10" hidden="1">
+    <row r="26" spans="1:10" ht="27">
       <c r="A26" s="4" t="s">
         <v>125</v>
       </c>
@@ -13948,7 +13944,7 @@
         <v>672</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
       <c r="E26" s="5"/>
       <c r="F26" s="7" t="s">
@@ -13960,7 +13956,7 @@
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
     </row>
-    <row r="27" spans="1:10" hidden="1">
+    <row r="27" spans="1:10">
       <c r="A27" s="4" t="s">
         <v>126</v>
       </c>
@@ -13983,7 +13979,7 @@
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
     </row>
-    <row r="28" spans="1:10" hidden="1">
+    <row r="28" spans="1:10">
       <c r="A28" s="4" t="s">
         <v>127</v>
       </c>
@@ -14000,7 +13996,7 @@
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
     </row>
-    <row r="29" spans="1:10" hidden="1">
+    <row r="29" spans="1:10">
       <c r="A29" s="4" t="s">
         <v>72</v>
       </c>
@@ -14017,7 +14013,7 @@
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
     </row>
-    <row r="30" spans="1:10" hidden="1">
+    <row r="30" spans="1:10">
       <c r="A30" s="4" t="s">
         <v>128</v>
       </c>
@@ -14057,7 +14053,7 @@
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
     </row>
-    <row r="32" spans="1:10" hidden="1">
+    <row r="32" spans="1:10">
       <c r="A32" s="4" t="s">
         <v>130</v>
       </c>
@@ -14080,7 +14076,7 @@
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
     </row>
-    <row r="33" spans="1:10" hidden="1">
+    <row r="33" spans="1:10">
       <c r="A33" s="4" t="s">
         <v>131</v>
       </c>
@@ -14097,7 +14093,7 @@
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
     </row>
-    <row r="34" spans="1:10" hidden="1">
+    <row r="34" spans="1:10">
       <c r="A34" s="4" t="s">
         <v>31</v>
       </c>
@@ -14114,7 +14110,7 @@
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
     </row>
-    <row r="35" spans="1:10" hidden="1">
+    <row r="35" spans="1:10">
       <c r="A35" s="4" t="s">
         <v>132</v>
       </c>
@@ -14131,7 +14127,7 @@
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
     </row>
-    <row r="36" spans="1:10" hidden="1">
+    <row r="36" spans="1:10">
       <c r="A36" s="4" t="s">
         <v>133</v>
       </c>
@@ -14148,7 +14144,7 @@
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
     </row>
-    <row r="37" spans="1:10" hidden="1">
+    <row r="37" spans="1:10">
       <c r="A37" s="4" t="s">
         <v>134</v>
       </c>
@@ -14171,7 +14167,7 @@
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
     </row>
-    <row r="38" spans="1:10" hidden="1">
+    <row r="38" spans="1:10">
       <c r="A38" s="4" t="s">
         <v>135</v>
       </c>
@@ -14188,7 +14184,7 @@
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
     </row>
-    <row r="39" spans="1:10" hidden="1">
+    <row r="39" spans="1:10">
       <c r="A39" s="4" t="s">
         <v>136</v>
       </c>
@@ -14211,7 +14207,7 @@
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
     </row>
-    <row r="40" spans="1:10" hidden="1">
+    <row r="40" spans="1:10">
       <c r="A40" s="4" t="s">
         <v>137</v>
       </c>
@@ -14228,7 +14224,7 @@
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
     </row>
-    <row r="41" spans="1:10" hidden="1">
+    <row r="41" spans="1:10">
       <c r="A41" s="4" t="s">
         <v>138</v>
       </c>
@@ -14266,7 +14262,7 @@
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
     </row>
-    <row r="43" spans="1:10" hidden="1">
+    <row r="43" spans="1:10" ht="27">
       <c r="A43" s="4" t="s">
         <v>140</v>
       </c>
@@ -14287,7 +14283,7 @@
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
     </row>
-    <row r="44" spans="1:10" hidden="1">
+    <row r="44" spans="1:10">
       <c r="A44" s="4" t="s">
         <v>77</v>
       </c>
@@ -14304,7 +14300,7 @@
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
     </row>
-    <row r="45" spans="1:10" hidden="1">
+    <row r="45" spans="1:10" ht="27">
       <c r="A45" s="4" t="s">
         <v>141</v>
       </c>
@@ -14325,7 +14321,7 @@
       <c r="I45" s="1"/>
       <c r="J45" s="1"/>
     </row>
-    <row r="46" spans="1:10" hidden="1">
+    <row r="46" spans="1:10">
       <c r="A46" s="4" t="s">
         <v>35</v>
       </c>
@@ -14342,7 +14338,7 @@
       <c r="I46" s="1"/>
       <c r="J46" s="1"/>
     </row>
-    <row r="47" spans="1:10" hidden="1">
+    <row r="47" spans="1:10">
       <c r="A47" s="4" t="s">
         <v>142</v>
       </c>
@@ -14365,7 +14361,7 @@
       <c r="I47" s="1"/>
       <c r="J47" s="1"/>
     </row>
-    <row r="48" spans="1:10" hidden="1">
+    <row r="48" spans="1:10">
       <c r="A48" s="4" t="s">
         <v>143</v>
       </c>
@@ -14382,7 +14378,7 @@
       <c r="I48" s="1"/>
       <c r="J48" s="1"/>
     </row>
-    <row r="49" spans="1:10" hidden="1">
+    <row r="49" spans="1:10">
       <c r="A49" s="4" t="s">
         <v>40</v>
       </c>
@@ -14399,7 +14395,7 @@
       <c r="I49" s="1"/>
       <c r="J49" s="1"/>
     </row>
-    <row r="50" spans="1:10" hidden="1">
+    <row r="50" spans="1:10">
       <c r="A50" s="4" t="s">
         <v>144</v>
       </c>
@@ -14422,7 +14418,7 @@
       <c r="I50" s="1"/>
       <c r="J50" s="1"/>
     </row>
-    <row r="51" spans="1:10" hidden="1">
+    <row r="51" spans="1:10">
       <c r="A51" s="4" t="s">
         <v>45</v>
       </c>
@@ -14439,7 +14435,7 @@
       <c r="I51" s="1"/>
       <c r="J51" s="1"/>
     </row>
-    <row r="52" spans="1:10" hidden="1">
+    <row r="52" spans="1:10">
       <c r="A52" s="4" t="s">
         <v>145</v>
       </c>
@@ -14456,7 +14452,7 @@
       <c r="I52" s="1"/>
       <c r="J52" s="1"/>
     </row>
-    <row r="53" spans="1:10" hidden="1">
+    <row r="53" spans="1:10">
       <c r="A53" s="4" t="s">
         <v>146</v>
       </c>
@@ -14473,7 +14469,7 @@
       <c r="I53" s="1"/>
       <c r="J53" s="1"/>
     </row>
-    <row r="54" spans="1:10" hidden="1">
+    <row r="54" spans="1:10">
       <c r="A54" s="4" t="s">
         <v>147</v>
       </c>
@@ -14490,26 +14486,26 @@
       <c r="I54" s="1"/>
       <c r="J54" s="1"/>
     </row>
-    <row r="55" spans="1:10">
+    <row r="55" spans="1:10" ht="27">
       <c r="A55" s="4" t="s">
         <v>148</v>
       </c>
       <c r="B55" s="4" t="s">
+        <v>809</v>
+      </c>
+      <c r="C55" s="4" t="s">
         <v>811</v>
-      </c>
-      <c r="C55" s="4" t="s">
-        <v>813</v>
       </c>
       <c r="D55" s="5"/>
       <c r="E55" s="5"/>
       <c r="F55" s="7" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="G55" s="5"/>
       <c r="I55" s="1"/>
       <c r="J55" s="1"/>
     </row>
-    <row r="56" spans="1:10" hidden="1">
+    <row r="56" spans="1:10">
       <c r="A56" s="4" t="s">
         <v>50</v>
       </c>
@@ -14526,45 +14522,45 @@
       <c r="I56" s="1"/>
       <c r="J56" s="1"/>
     </row>
-    <row r="57" spans="1:10">
+    <row r="57" spans="1:10" ht="27">
       <c r="A57" s="4" t="s">
         <v>149</v>
       </c>
       <c r="B57" s="4" t="s">
+        <v>812</v>
+      </c>
+      <c r="C57" s="4" t="s">
         <v>814</v>
-      </c>
-      <c r="C57" s="4" t="s">
-        <v>816</v>
       </c>
       <c r="D57" s="5"/>
       <c r="E57" s="5"/>
       <c r="F57" s="7" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="G57" s="5"/>
       <c r="I57" s="1"/>
       <c r="J57" s="1"/>
     </row>
-    <row r="58" spans="1:10">
+    <row r="58" spans="1:10" ht="27">
       <c r="A58" s="4" t="s">
         <v>150</v>
       </c>
       <c r="B58" s="4" t="s">
+        <v>815</v>
+      </c>
+      <c r="C58" s="4" t="s">
         <v>817</v>
-      </c>
-      <c r="C58" s="4" t="s">
-        <v>819</v>
       </c>
       <c r="D58" s="5"/>
       <c r="E58" s="5"/>
       <c r="F58" s="7" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="G58" s="5"/>
       <c r="I58" s="1"/>
       <c r="J58" s="1"/>
     </row>
-    <row r="59" spans="1:10" hidden="1">
+    <row r="59" spans="1:10">
       <c r="A59" s="4" t="s">
         <v>151</v>
       </c>
@@ -14581,7 +14577,7 @@
       <c r="I59" s="1"/>
       <c r="J59" s="1"/>
     </row>
-    <row r="60" spans="1:10" hidden="1">
+    <row r="60" spans="1:10">
       <c r="A60" s="4" t="s">
         <v>398</v>
       </c>
@@ -14598,7 +14594,7 @@
       <c r="I60" s="1"/>
       <c r="J60" s="1"/>
     </row>
-    <row r="61" spans="1:10" hidden="1">
+    <row r="61" spans="1:10">
       <c r="A61" s="4" t="s">
         <v>152</v>
       </c>
@@ -14621,26 +14617,26 @@
       <c r="I61" s="1"/>
       <c r="J61" s="1"/>
     </row>
-    <row r="62" spans="1:10">
+    <row r="62" spans="1:10" ht="27">
       <c r="A62" s="4" t="s">
         <v>153</v>
       </c>
       <c r="B62" s="4" t="s">
+        <v>818</v>
+      </c>
+      <c r="C62" s="4" t="s">
         <v>820</v>
-      </c>
-      <c r="C62" s="4" t="s">
-        <v>822</v>
       </c>
       <c r="D62" s="5"/>
       <c r="E62" s="5"/>
       <c r="F62" s="7" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="G62" s="5"/>
       <c r="I62" s="1"/>
       <c r="J62" s="1"/>
     </row>
-    <row r="63" spans="1:10" hidden="1">
+    <row r="63" spans="1:10">
       <c r="A63" s="4" t="s">
         <v>154</v>
       </c>
@@ -14663,20 +14659,20 @@
       <c r="I63" s="1"/>
       <c r="J63" s="1"/>
     </row>
-    <row r="64" spans="1:10" hidden="1">
+    <row r="64" spans="1:10" ht="27">
       <c r="A64" s="4" t="s">
         <v>155</v>
       </c>
       <c r="B64" s="4" t="s">
+        <v>821</v>
+      </c>
+      <c r="C64" s="4" t="s">
         <v>823</v>
-      </c>
-      <c r="C64" s="4" t="s">
-        <v>825</v>
       </c>
       <c r="D64" s="5"/>
       <c r="E64" s="5"/>
       <c r="F64" s="7" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="G64" s="5">
         <v>1</v>
@@ -14684,26 +14680,26 @@
       <c r="I64" s="1"/>
       <c r="J64" s="1"/>
     </row>
-    <row r="65" spans="1:10">
+    <row r="65" spans="1:10" ht="27">
       <c r="A65" s="4" t="s">
         <v>156</v>
       </c>
       <c r="B65" s="4" t="s">
+        <v>824</v>
+      </c>
+      <c r="C65" s="4" t="s">
         <v>826</v>
-      </c>
-      <c r="C65" s="4" t="s">
-        <v>828</v>
       </c>
       <c r="D65" s="5"/>
       <c r="E65" s="5"/>
       <c r="F65" s="7" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="G65" s="5"/>
       <c r="I65" s="1"/>
       <c r="J65" s="1"/>
     </row>
-    <row r="66" spans="1:10" hidden="1">
+    <row r="66" spans="1:10">
       <c r="A66" s="4" t="s">
         <v>336</v>
       </c>
@@ -14720,26 +14716,26 @@
       <c r="I66" s="1"/>
       <c r="J66" s="1"/>
     </row>
-    <row r="67" spans="1:10">
+    <row r="67" spans="1:10" ht="27">
       <c r="A67" s="4" t="s">
         <v>157</v>
       </c>
       <c r="B67" s="4" t="s">
+        <v>827</v>
+      </c>
+      <c r="C67" s="4" t="s">
         <v>829</v>
-      </c>
-      <c r="C67" s="4" t="s">
-        <v>831</v>
       </c>
       <c r="D67" s="5"/>
       <c r="E67" s="5"/>
       <c r="F67" s="7" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="G67" s="5"/>
       <c r="I67" s="1"/>
       <c r="J67" s="1"/>
     </row>
-    <row r="68" spans="1:10" hidden="1">
+    <row r="68" spans="1:10">
       <c r="A68" s="4" t="s">
         <v>158</v>
       </c>
@@ -14762,7 +14758,7 @@
       <c r="I68" s="1"/>
       <c r="J68" s="1"/>
     </row>
-    <row r="69" spans="1:10" hidden="1">
+    <row r="69" spans="1:10">
       <c r="A69" s="4" t="s">
         <v>82</v>
       </c>
@@ -14779,26 +14775,26 @@
       <c r="I69" s="1"/>
       <c r="J69" s="1"/>
     </row>
-    <row r="70" spans="1:10">
+    <row r="70" spans="1:10" ht="27">
       <c r="A70" s="4" t="s">
         <v>159</v>
       </c>
       <c r="B70" s="4" t="s">
+        <v>830</v>
+      </c>
+      <c r="C70" s="4" t="s">
         <v>832</v>
-      </c>
-      <c r="C70" s="4" t="s">
-        <v>834</v>
       </c>
       <c r="D70" s="5"/>
       <c r="E70" s="5"/>
       <c r="F70" s="4" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
       <c r="G70" s="5"/>
       <c r="I70" s="1"/>
       <c r="J70" s="1"/>
     </row>
-    <row r="71" spans="1:10" hidden="1">
+    <row r="71" spans="1:10">
       <c r="A71" s="4" t="s">
         <v>160</v>
       </c>
@@ -14821,7 +14817,7 @@
       <c r="I71" s="1"/>
       <c r="J71" s="1"/>
     </row>
-    <row r="72" spans="1:10" hidden="1">
+    <row r="72" spans="1:10">
       <c r="A72" s="4" t="s">
         <v>161</v>
       </c>
@@ -14844,123 +14840,123 @@
       <c r="I72" s="1"/>
       <c r="J72" s="1"/>
     </row>
-    <row r="73" spans="1:10">
+    <row r="73" spans="1:10" ht="27">
       <c r="A73" s="4" t="s">
         <v>162</v>
       </c>
       <c r="B73" s="4" t="s">
+        <v>833</v>
+      </c>
+      <c r="C73" s="4" t="s">
         <v>835</v>
       </c>
-      <c r="C73" s="4" t="s">
-        <v>837</v>
-      </c>
       <c r="D73" s="5" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="E73" s="5"/>
       <c r="F73" s="7" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
       <c r="G73" s="5"/>
       <c r="I73" s="1"/>
       <c r="J73" s="1"/>
     </row>
-    <row r="74" spans="1:10">
+    <row r="74" spans="1:10" ht="27">
       <c r="A74" s="4" t="s">
         <v>163</v>
       </c>
       <c r="B74" s="4" t="s">
+        <v>836</v>
+      </c>
+      <c r="C74" s="4" t="s">
         <v>838</v>
-      </c>
-      <c r="C74" s="4" t="s">
-        <v>840</v>
       </c>
       <c r="D74" s="5"/>
       <c r="E74" s="5"/>
       <c r="F74" s="7" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
       <c r="G74" s="5"/>
       <c r="I74" s="1"/>
       <c r="J74" s="1"/>
     </row>
-    <row r="75" spans="1:10">
+    <row r="75" spans="1:10" ht="27">
       <c r="A75" s="4" t="s">
         <v>164</v>
       </c>
       <c r="B75" s="4" t="s">
+        <v>839</v>
+      </c>
+      <c r="C75" s="4" t="s">
         <v>841</v>
-      </c>
-      <c r="C75" s="4" t="s">
-        <v>843</v>
       </c>
       <c r="D75" s="5"/>
       <c r="E75" s="5"/>
       <c r="F75" s="4" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
       <c r="G75" s="5"/>
       <c r="I75" s="1"/>
       <c r="J75" s="1"/>
     </row>
-    <row r="76" spans="1:10">
+    <row r="76" spans="1:10" ht="27">
       <c r="A76" s="4" t="s">
         <v>165</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
       <c r="D76" s="5"/>
       <c r="E76" s="5"/>
       <c r="F76" s="7" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="G76" s="5"/>
       <c r="I76" s="1"/>
       <c r="J76" s="1"/>
     </row>
-    <row r="77" spans="1:10">
+    <row r="77" spans="1:10" ht="27">
       <c r="A77" s="4" t="s">
         <v>166</v>
       </c>
       <c r="B77" s="4" t="s">
+        <v>845</v>
+      </c>
+      <c r="C77" s="4" t="s">
         <v>847</v>
-      </c>
-      <c r="C77" s="4" t="s">
-        <v>849</v>
       </c>
       <c r="D77" s="5"/>
       <c r="E77" s="5"/>
       <c r="F77" s="7" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="G77" s="5"/>
       <c r="I77" s="1"/>
       <c r="J77" s="1"/>
     </row>
-    <row r="78" spans="1:10">
+    <row r="78" spans="1:10" ht="27">
       <c r="A78" s="4" t="s">
         <v>167</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
       <c r="D78" s="5"/>
       <c r="E78" s="5"/>
       <c r="F78" s="7" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
       <c r="G78" s="5"/>
       <c r="I78" s="1"/>
       <c r="J78" s="1"/>
     </row>
-    <row r="79" spans="1:10" hidden="1">
+    <row r="79" spans="1:10">
       <c r="A79" s="4" t="s">
         <v>168</v>
       </c>
@@ -14977,31 +14973,31 @@
       <c r="I79" s="1"/>
       <c r="J79" s="1"/>
     </row>
-    <row r="80" spans="1:10">
+    <row r="80" spans="1:10" ht="27">
       <c r="A80" s="4" t="s">
         <v>169</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
       <c r="D80" s="5"/>
       <c r="E80" s="5"/>
       <c r="F80" s="7" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
       <c r="G80" s="5"/>
       <c r="I80" s="1"/>
       <c r="J80" s="1"/>
     </row>
-    <row r="81" spans="1:10">
+    <row r="81" spans="1:10" ht="27">
       <c r="A81" s="4" t="s">
         <v>170</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
       <c r="C81" s="4" t="s">
         <v>616</v>
@@ -15013,13 +15009,13 @@
         <v>617</v>
       </c>
       <c r="F81" s="7" t="s">
-        <v>861</v>
+        <v>859</v>
       </c>
       <c r="G81" s="5"/>
       <c r="I81" s="1"/>
       <c r="J81" s="1"/>
     </row>
-    <row r="82" spans="1:10" hidden="1">
+    <row r="82" spans="1:10">
       <c r="A82" s="4" t="s">
         <v>171</v>
       </c>
@@ -15036,7 +15032,7 @@
       <c r="I82" s="1"/>
       <c r="J82" s="1"/>
     </row>
-    <row r="83" spans="1:10" hidden="1">
+    <row r="83" spans="1:10" ht="27">
       <c r="A83" s="4" t="s">
         <v>172</v>
       </c>
@@ -15044,12 +15040,12 @@
         <v>670</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>859</v>
+        <v>857</v>
       </c>
       <c r="D83" s="5"/>
       <c r="E83" s="5"/>
       <c r="F83" s="7" t="s">
-        <v>860</v>
+        <v>858</v>
       </c>
       <c r="G83" s="5">
         <v>1</v>
@@ -15057,7 +15053,7 @@
       <c r="I83" s="1"/>
       <c r="J83" s="1"/>
     </row>
-    <row r="84" spans="1:10" hidden="1">
+    <row r="84" spans="1:10">
       <c r="A84" s="4" t="s">
         <v>173</v>
       </c>
@@ -15074,7 +15070,7 @@
       <c r="I84" s="1"/>
       <c r="J84" s="1"/>
     </row>
-    <row r="85" spans="1:10" hidden="1">
+    <row r="85" spans="1:10">
       <c r="A85" s="4" t="s">
         <v>174</v>
       </c>
@@ -15097,22 +15093,22 @@
       <c r="I85" s="1"/>
       <c r="J85" s="1"/>
     </row>
-    <row r="86" spans="1:10" hidden="1">
+    <row r="86" spans="1:10" ht="27">
       <c r="A86" s="4" t="s">
         <v>175</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>862</v>
+        <v>860</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
       <c r="D86" s="5" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
       <c r="E86" s="5"/>
       <c r="F86" s="7" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
       <c r="G86" s="5">
         <v>1</v>
@@ -15120,7 +15116,7 @@
       <c r="I86" s="1"/>
       <c r="J86" s="1"/>
     </row>
-    <row r="87" spans="1:10" hidden="1">
+    <row r="87" spans="1:10">
       <c r="A87" s="4" t="s">
         <v>176</v>
       </c>
@@ -15137,39 +15133,39 @@
       <c r="I87" s="1"/>
       <c r="J87" s="1"/>
     </row>
-    <row r="88" spans="1:10">
+    <row r="88" spans="1:10" ht="27">
       <c r="A88" s="4" t="s">
         <v>177</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>865</v>
+        <v>863</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
       <c r="D88" s="5"/>
       <c r="E88" s="5"/>
       <c r="F88" s="7" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
       <c r="G88" s="5"/>
       <c r="I88" s="1"/>
       <c r="J88" s="1"/>
     </row>
-    <row r="89" spans="1:10" hidden="1">
+    <row r="89" spans="1:10" ht="27">
       <c r="A89" s="4" t="s">
         <v>178</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>868</v>
+        <v>866</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
       <c r="D89" s="5"/>
       <c r="E89" s="5"/>
       <c r="F89" s="7" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
       <c r="G89" s="5">
         <v>1</v>
@@ -15177,7 +15173,7 @@
       <c r="I89" s="1"/>
       <c r="J89" s="1"/>
     </row>
-    <row r="90" spans="1:10" hidden="1">
+    <row r="90" spans="1:10">
       <c r="A90" s="4" t="s">
         <v>87</v>
       </c>
@@ -15194,7 +15190,7 @@
       <c r="I90" s="1"/>
       <c r="J90" s="1"/>
     </row>
-    <row r="91" spans="1:10" hidden="1">
+    <row r="91" spans="1:10">
       <c r="A91" s="4" t="s">
         <v>55</v>
       </c>
@@ -15211,7 +15207,7 @@
       <c r="I91" s="1"/>
       <c r="J91" s="1"/>
     </row>
-    <row r="92" spans="1:10" hidden="1">
+    <row r="92" spans="1:10">
       <c r="A92" s="4" t="s">
         <v>179</v>
       </c>
@@ -15234,7 +15230,7 @@
       <c r="I92" s="1"/>
       <c r="J92" s="1"/>
     </row>
-    <row r="93" spans="1:10" hidden="1">
+    <row r="93" spans="1:10">
       <c r="A93" s="4" t="s">
         <v>180</v>
       </c>
@@ -15251,20 +15247,20 @@
       <c r="I93" s="1"/>
       <c r="J93" s="1"/>
     </row>
-    <row r="94" spans="1:10" hidden="1">
+    <row r="94" spans="1:10" ht="27">
       <c r="A94" s="4" t="s">
         <v>181</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
       <c r="D94" s="5"/>
       <c r="E94" s="5"/>
       <c r="F94" s="7" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
       <c r="G94" s="5">
         <v>1</v>
@@ -15272,26 +15268,26 @@
       <c r="I94" s="1"/>
       <c r="J94" s="1"/>
     </row>
-    <row r="95" spans="1:10">
+    <row r="95" spans="1:10" ht="27">
       <c r="A95" s="4" t="s">
         <v>182</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="D95" s="5"/>
       <c r="E95" s="5"/>
       <c r="F95" s="7" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
       <c r="G95" s="5"/>
       <c r="I95" s="1"/>
       <c r="J95" s="1"/>
     </row>
-    <row r="96" spans="1:10" hidden="1">
+    <row r="96" spans="1:10">
       <c r="A96" s="4" t="s">
         <v>183</v>
       </c>
@@ -15314,7 +15310,7 @@
       <c r="I96" s="1"/>
       <c r="J96" s="1"/>
     </row>
-    <row r="97" spans="1:10" hidden="1">
+    <row r="97" spans="1:10">
       <c r="A97" s="4" t="s">
         <v>184</v>
       </c>
@@ -15331,7 +15327,7 @@
       <c r="I97" s="1"/>
       <c r="J97" s="1"/>
     </row>
-    <row r="98" spans="1:10" hidden="1">
+    <row r="98" spans="1:10">
       <c r="A98" s="4" t="s">
         <v>348</v>
       </c>
@@ -15348,41 +15344,41 @@
       <c r="I98" s="1"/>
       <c r="J98" s="1"/>
     </row>
-    <row r="99" spans="1:10">
+    <row r="99" spans="1:10" ht="27">
       <c r="A99" s="4" t="s">
         <v>185</v>
       </c>
       <c r="B99" s="4" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
       <c r="D99" s="5"/>
       <c r="E99" s="5"/>
       <c r="F99" s="7" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="G99" s="5"/>
       <c r="I99" s="1"/>
       <c r="J99" s="1"/>
     </row>
-    <row r="100" spans="1:10" ht="27" hidden="1">
+    <row r="100" spans="1:10" ht="27">
       <c r="A100" s="4" t="s">
         <v>186</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
       <c r="D100" s="5" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
       <c r="E100" s="5"/>
       <c r="F100" s="7" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
       <c r="G100" s="5">
         <v>1</v>
@@ -15390,7 +15386,7 @@
       <c r="I100" s="1"/>
       <c r="J100" s="1"/>
     </row>
-    <row r="101" spans="1:10" hidden="1">
+    <row r="101" spans="1:10">
       <c r="A101" s="4" t="s">
         <v>187</v>
       </c>
@@ -15411,7 +15407,7 @@
       <c r="I101" s="1"/>
       <c r="J101" s="1"/>
     </row>
-    <row r="102" spans="1:10" hidden="1">
+    <row r="102" spans="1:10">
       <c r="A102" s="4" t="s">
         <v>188</v>
       </c>
@@ -15434,7 +15430,7 @@
       <c r="I102" s="1"/>
       <c r="J102" s="1"/>
     </row>
-    <row r="103" spans="1:10" hidden="1">
+    <row r="103" spans="1:10">
       <c r="A103" s="4" t="s">
         <v>189</v>
       </c>
@@ -15451,26 +15447,26 @@
       <c r="I103" s="1"/>
       <c r="J103" s="1"/>
     </row>
-    <row r="104" spans="1:10">
+    <row r="104" spans="1:10" ht="27">
       <c r="A104" s="4" t="s">
         <v>190</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
       <c r="D104" s="5"/>
       <c r="E104" s="5"/>
       <c r="F104" s="7" t="s">
-        <v>885</v>
+        <v>883</v>
       </c>
       <c r="G104" s="5"/>
       <c r="I104" s="1"/>
       <c r="J104" s="1"/>
     </row>
-    <row r="105" spans="1:10" hidden="1">
+    <row r="105" spans="1:10">
       <c r="A105" s="4" t="s">
         <v>191</v>
       </c>
@@ -15493,7 +15489,7 @@
       <c r="I105" s="1"/>
       <c r="J105" s="1"/>
     </row>
-    <row r="106" spans="1:10" hidden="1">
+    <row r="106" spans="1:10">
       <c r="A106" s="4" t="s">
         <v>192</v>
       </c>
@@ -15510,7 +15506,7 @@
       <c r="I106" s="1"/>
       <c r="J106" s="1"/>
     </row>
-    <row r="107" spans="1:10" hidden="1">
+    <row r="107" spans="1:10">
       <c r="A107" s="4" t="s">
         <v>193</v>
       </c>
@@ -15527,7 +15523,7 @@
       <c r="I107" s="1"/>
       <c r="J107" s="1"/>
     </row>
-    <row r="108" spans="1:10" hidden="1">
+    <row r="108" spans="1:10">
       <c r="A108" s="4" t="s">
         <v>194</v>
       </c>
@@ -15544,7 +15540,7 @@
       <c r="I108" s="1"/>
       <c r="J108" s="1"/>
     </row>
-    <row r="109" spans="1:10" hidden="1">
+    <row r="109" spans="1:10">
       <c r="A109" s="4" t="s">
         <v>195</v>
       </c>
@@ -15561,7 +15557,7 @@
       <c r="I109" s="1"/>
       <c r="J109" s="1"/>
     </row>
-    <row r="110" spans="1:10" hidden="1">
+    <row r="110" spans="1:10">
       <c r="A110" s="4" t="s">
         <v>60</v>
       </c>
@@ -15578,26 +15574,26 @@
       <c r="I110" s="1"/>
       <c r="J110" s="1"/>
     </row>
-    <row r="111" spans="1:10">
+    <row r="111" spans="1:10" ht="27">
       <c r="A111" s="4" t="s">
         <v>196</v>
       </c>
       <c r="B111" s="4" t="s">
+        <v>884</v>
+      </c>
+      <c r="C111" s="4" t="s">
         <v>886</v>
-      </c>
-      <c r="C111" s="4" t="s">
-        <v>888</v>
       </c>
       <c r="D111" s="5"/>
       <c r="E111" s="5"/>
       <c r="F111" s="7" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
       <c r="G111" s="5"/>
       <c r="I111" s="1"/>
       <c r="J111" s="1"/>
     </row>
-    <row r="112" spans="1:10" hidden="1">
+    <row r="112" spans="1:10">
       <c r="A112" s="4" t="s">
         <v>197</v>
       </c>
@@ -15614,7 +15610,7 @@
       <c r="I112" s="1"/>
       <c r="J112" s="1"/>
     </row>
-    <row r="113" spans="1:10" hidden="1">
+    <row r="113" spans="1:10">
       <c r="A113" s="4" t="s">
         <v>198</v>
       </c>
@@ -15637,7 +15633,7 @@
       <c r="I113" s="1"/>
       <c r="J113" s="1"/>
     </row>
-    <row r="114" spans="1:10" hidden="1">
+    <row r="114" spans="1:10">
       <c r="A114" s="4" t="s">
         <v>199</v>
       </c>
@@ -15660,7 +15656,7 @@
       <c r="I114" s="1"/>
       <c r="J114" s="1"/>
     </row>
-    <row r="115" spans="1:10" hidden="1">
+    <row r="115" spans="1:10">
       <c r="A115" s="4" t="s">
         <v>92</v>
       </c>
@@ -15677,7 +15673,7 @@
       <c r="I115" s="1"/>
       <c r="J115" s="1"/>
     </row>
-    <row r="116" spans="1:10" hidden="1">
+    <row r="116" spans="1:10">
       <c r="A116" s="4" t="s">
         <v>200</v>
       </c>
@@ -15694,7 +15690,7 @@
       <c r="I116" s="1"/>
       <c r="J116" s="1"/>
     </row>
-    <row r="117" spans="1:10" hidden="1">
+    <row r="117" spans="1:10">
       <c r="A117" s="4" t="s">
         <v>201</v>
       </c>
@@ -15711,7 +15707,7 @@
       <c r="I117" s="1"/>
       <c r="J117" s="1"/>
     </row>
-    <row r="118" spans="1:10" hidden="1">
+    <row r="118" spans="1:10">
       <c r="A118" s="4" t="s">
         <v>63</v>
       </c>
@@ -15728,7 +15724,7 @@
       <c r="I118" s="1"/>
       <c r="J118" s="1"/>
     </row>
-    <row r="119" spans="1:10" hidden="1">
+    <row r="119" spans="1:10">
       <c r="A119" s="4" t="s">
         <v>97</v>
       </c>
@@ -15745,7 +15741,7 @@
       <c r="I119" s="1"/>
       <c r="J119" s="1"/>
     </row>
-    <row r="120" spans="1:10" hidden="1">
+    <row r="120" spans="1:10">
       <c r="A120" s="4" t="s">
         <v>202</v>
       </c>
@@ -15756,7 +15752,7 @@
         <v>608</v>
       </c>
       <c r="D120" s="5" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="E120" s="5" t="s">
         <v>610</v>
@@ -15768,7 +15764,7 @@
       <c r="I120" s="1"/>
       <c r="J120" s="1"/>
     </row>
-    <row r="121" spans="1:10" hidden="1">
+    <row r="121" spans="1:10">
       <c r="A121" s="4" t="s">
         <v>203</v>
       </c>
@@ -15785,45 +15781,45 @@
       <c r="I121" s="1"/>
       <c r="J121" s="1"/>
     </row>
-    <row r="122" spans="1:10">
+    <row r="122" spans="1:10" ht="27">
       <c r="A122" s="4" t="s">
         <v>204</v>
       </c>
       <c r="B122" s="4" t="s">
-        <v>889</v>
+        <v>887</v>
       </c>
       <c r="C122" s="4" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
       <c r="D122" s="5"/>
       <c r="E122" s="5"/>
       <c r="F122" s="7" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
       <c r="G122" s="5"/>
       <c r="I122" s="1"/>
       <c r="J122" s="1"/>
     </row>
-    <row r="123" spans="1:10">
+    <row r="123" spans="1:10" ht="27">
       <c r="A123" s="4" t="s">
         <v>205</v>
       </c>
       <c r="B123" s="4" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
       <c r="C123" s="4" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
       <c r="D123" s="5"/>
       <c r="E123" s="5"/>
       <c r="F123" s="7" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="G123" s="5"/>
       <c r="I123" s="1"/>
       <c r="J123" s="1"/>
     </row>
-    <row r="124" spans="1:10" hidden="1">
+    <row r="124" spans="1:10">
       <c r="A124" s="4" t="s">
         <v>206</v>
       </c>
@@ -15846,7 +15842,7 @@
       <c r="I124" s="1"/>
       <c r="J124" s="1"/>
     </row>
-    <row r="125" spans="1:10" hidden="1">
+    <row r="125" spans="1:10">
       <c r="A125" s="4" t="s">
         <v>207</v>
       </c>
@@ -15869,7 +15865,7 @@
       <c r="I125" s="1"/>
       <c r="J125" s="1"/>
     </row>
-    <row r="126" spans="1:10" hidden="1">
+    <row r="126" spans="1:10">
       <c r="A126" s="4" t="s">
         <v>208</v>
       </c>
@@ -15886,7 +15882,7 @@
       <c r="I126" s="1"/>
       <c r="J126" s="1"/>
     </row>
-    <row r="127" spans="1:10" hidden="1">
+    <row r="127" spans="1:10">
       <c r="A127" s="4" t="s">
         <v>209</v>
       </c>
@@ -15903,7 +15899,7 @@
       <c r="I127" s="1"/>
       <c r="J127" s="1"/>
     </row>
-    <row r="128" spans="1:10" hidden="1">
+    <row r="128" spans="1:10">
       <c r="A128" s="4" t="s">
         <v>210</v>
       </c>
@@ -15920,7 +15916,7 @@
       <c r="I128" s="1"/>
       <c r="J128" s="1"/>
     </row>
-    <row r="129" spans="1:10" hidden="1">
+    <row r="129" spans="1:10">
       <c r="A129" s="4" t="s">
         <v>211</v>
       </c>

</xml_diff>

<commit_message>
111 Signed-off-by: twtcom001 <twtcom001@sina.com>
</commit_message>
<xml_diff>
--- a/统计清单/2017国内编号清单.xlsx
+++ b/统计清单/2017国内编号清单.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1908" uniqueCount="965">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1919" uniqueCount="978">
   <si>
     <t>本地编号</t>
   </si>
@@ -3309,10 +3309,6 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>Chamaecereus</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
     <t>Chamaecereus Lincoln Gem</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
@@ -3557,6 +3553,61 @@
   </si>
   <si>
     <t>惜别</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Trichocereus</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Trichocereus</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>飞碟</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lobivia ochielen</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lobivia</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>乌艳丸、方便面</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Echinopsis</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Echinopsis</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Chamaecereus</t>
+  </si>
+  <si>
+    <t>Chamaecereus</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Echinopsis</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>斯特恩泰勒</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>彩草319</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>胭脂复色白檀</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -3793,7 +3844,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3918,6 +3969,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -4328,8 +4380,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:L186" totalsRowShown="0">
-  <autoFilter ref="A1:L186"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:L197" totalsRowShown="0">
+  <autoFilter ref="A1:L197"/>
   <tableColumns count="12">
     <tableColumn id="1" name="145"/>
     <tableColumn id="2" name="属"/>
@@ -4665,10 +4717,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L186"/>
+  <dimension ref="A1:L197"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A151" workbookViewId="0">
-      <selection activeCell="D176" sqref="D176"/>
+    <sheetView tabSelected="1" topLeftCell="A166" workbookViewId="0">
+      <selection activeCell="D191" sqref="D191"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -4707,7 +4759,7 @@
         <v>736</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="H1" s="14" t="s">
         <v>735</v>
@@ -8786,7 +8838,7 @@
         <v>320</v>
       </c>
       <c r="D128" s="14" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="E128" s="14" t="s">
         <v>272</v>
@@ -9381,7 +9433,7 @@
         <v>496</v>
       </c>
       <c r="D148" s="39" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="E148" s="39" t="s">
         <v>488</v>
@@ -9409,7 +9461,7 @@
         <v>497</v>
       </c>
       <c r="D149" s="39" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="E149" s="39" t="s">
         <v>333</v>
@@ -9465,7 +9517,7 @@
         <v>712</v>
       </c>
       <c r="D151" s="39" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="E151" s="39" t="s">
         <v>713</v>
@@ -9579,7 +9631,7 @@
         <v>143</v>
       </c>
       <c r="B156" s="51" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="C156" s="52" t="s">
         <v>751</v>
@@ -9601,7 +9653,7 @@
         <v>144</v>
       </c>
       <c r="B157" s="37" t="s">
-        <v>741</v>
+        <v>964</v>
       </c>
       <c r="C157" s="40" t="s">
         <v>755</v>
@@ -9685,7 +9737,7 @@
         <v>766</v>
       </c>
       <c r="D160" s="39" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="E160" s="39" t="s">
         <v>770</v>
@@ -9967,7 +10019,7 @@
         <v>159</v>
       </c>
       <c r="B172" s="37" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="C172" s="68" t="s">
         <v>202</v>
@@ -9996,16 +10048,16 @@
         <v>160</v>
       </c>
       <c r="B173" s="3" t="s">
-        <v>902</v>
+        <v>973</v>
       </c>
       <c r="C173" s="13" t="s">
         <v>901</v>
       </c>
       <c r="D173" s="14" t="s">
+        <v>902</v>
+      </c>
+      <c r="E173" s="14" t="s">
         <v>903</v>
-      </c>
-      <c r="E173" s="14" t="s">
-        <v>904</v>
       </c>
       <c r="F173" s="14"/>
       <c r="G173" s="14"/>
@@ -10020,14 +10072,14 @@
         <v>161</v>
       </c>
       <c r="B174" s="3" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="C174" s="13"/>
       <c r="D174" s="14" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="E174" s="14" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="F174" s="14"/>
       <c r="G174" s="14"/>
@@ -10042,12 +10094,12 @@
         <v>162</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="C175" s="13"/>
       <c r="D175" s="14"/>
       <c r="E175" s="14" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="F175" s="14"/>
       <c r="G175" s="14"/>
@@ -10060,20 +10112,20 @@
         <v>163</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="C176" s="13"/>
       <c r="D176" s="14" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="E176" s="14" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="F176" s="14"/>
       <c r="G176" s="14"/>
       <c r="H176" s="14"/>
       <c r="I176" s="36" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="J176" s="14"/>
     </row>
@@ -10082,14 +10134,14 @@
         <v>164</v>
       </c>
       <c r="B177" s="3" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="C177" s="13"/>
       <c r="D177" s="14" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="E177" s="14" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="F177" s="14"/>
       <c r="G177" s="14"/>
@@ -10107,7 +10159,7 @@
       <c r="C178" s="15"/>
       <c r="D178" s="9"/>
       <c r="E178" s="9" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="F178" s="9"/>
       <c r="G178" s="9"/>
@@ -10120,7 +10172,7 @@
         <v>166</v>
       </c>
       <c r="B179" s="37" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="C179" s="68" t="s">
         <v>105</v>
@@ -10129,7 +10181,7 @@
         <v>514</v>
       </c>
       <c r="E179" s="69" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="F179" s="39"/>
       <c r="G179" s="39">
@@ -10146,7 +10198,7 @@
         <v>167</v>
       </c>
       <c r="B180" s="37" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="C180" s="68" t="s">
         <v>138</v>
@@ -10155,7 +10207,7 @@
         <v>675</v>
       </c>
       <c r="E180" s="69" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="F180" s="39"/>
       <c r="G180" s="39">
@@ -10172,7 +10224,7 @@
         <v>168</v>
       </c>
       <c r="B181" s="37" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="C181" s="72" t="s">
         <v>140</v>
@@ -10181,7 +10233,7 @@
         <v>682</v>
       </c>
       <c r="E181" s="73" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="F181" s="74"/>
       <c r="G181" s="74">
@@ -10198,7 +10250,7 @@
         <v>169</v>
       </c>
       <c r="B182" s="37" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="C182" s="77" t="s">
         <v>141</v>
@@ -10224,7 +10276,7 @@
         <v>170</v>
       </c>
       <c r="B183" s="37" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="C183" s="77" t="s">
         <v>155</v>
@@ -10250,7 +10302,7 @@
         <v>171</v>
       </c>
       <c r="B184" s="37" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="C184" s="77" t="s">
         <v>172</v>
@@ -10276,7 +10328,7 @@
         <v>172</v>
       </c>
       <c r="B185" s="37" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="C185" s="77" t="s">
         <v>178</v>
@@ -10302,7 +10354,7 @@
         <v>173</v>
       </c>
       <c r="B186" s="37" t="s">
-        <v>956</v>
+        <v>970</v>
       </c>
       <c r="C186" s="77" t="s">
         <v>181</v>
@@ -10322,6 +10374,165 @@
       </c>
       <c r="I186" s="66"/>
       <c r="J186" s="39"/>
+    </row>
+    <row r="187" spans="1:10">
+      <c r="A187" s="37">
+        <v>174</v>
+      </c>
+      <c r="B187" s="37" t="s">
+        <v>965</v>
+      </c>
+      <c r="C187" s="40"/>
+      <c r="D187" s="39"/>
+      <c r="E187" s="39" t="s">
+        <v>966</v>
+      </c>
+      <c r="F187" s="9"/>
+      <c r="H187" s="9"/>
+      <c r="I187" s="64"/>
+      <c r="J187" s="9"/>
+    </row>
+    <row r="188" spans="1:10">
+      <c r="A188" s="37">
+        <v>175</v>
+      </c>
+      <c r="B188" s="37" t="s">
+        <v>968</v>
+      </c>
+      <c r="C188" s="40"/>
+      <c r="D188" s="39" t="s">
+        <v>967</v>
+      </c>
+      <c r="E188" s="39" t="s">
+        <v>969</v>
+      </c>
+      <c r="F188" s="9"/>
+      <c r="H188" s="9"/>
+      <c r="I188" s="64"/>
+      <c r="J188" s="9"/>
+    </row>
+    <row r="189" spans="1:10">
+      <c r="A189">
+        <v>176</v>
+      </c>
+      <c r="B189" s="3" t="s">
+        <v>971</v>
+      </c>
+      <c r="C189" s="15"/>
+      <c r="D189" s="9"/>
+      <c r="E189" s="14" t="s">
+        <v>976</v>
+      </c>
+      <c r="F189" s="9"/>
+      <c r="H189" s="9"/>
+      <c r="I189" s="64"/>
+      <c r="J189" s="9"/>
+    </row>
+    <row r="190" spans="1:10">
+      <c r="A190">
+        <v>177</v>
+      </c>
+      <c r="B190" s="3" t="s">
+        <v>974</v>
+      </c>
+      <c r="C190" s="62"/>
+      <c r="D190" s="63"/>
+      <c r="E190" s="60" t="s">
+        <v>975</v>
+      </c>
+      <c r="F190" s="63"/>
+      <c r="H190" s="63"/>
+      <c r="I190" s="78"/>
+      <c r="J190" s="63"/>
+    </row>
+    <row r="191" spans="1:10">
+      <c r="A191">
+        <v>178</v>
+      </c>
+      <c r="B191" t="s">
+        <v>972</v>
+      </c>
+      <c r="C191" s="62"/>
+      <c r="D191" s="63"/>
+      <c r="E191" s="60" t="s">
+        <v>977</v>
+      </c>
+      <c r="F191" s="63"/>
+      <c r="H191" s="63"/>
+      <c r="I191" s="78"/>
+      <c r="J191" s="63"/>
+    </row>
+    <row r="192" spans="1:10">
+      <c r="A192">
+        <v>179</v>
+      </c>
+      <c r="C192" s="62"/>
+      <c r="D192" s="63"/>
+      <c r="E192" s="63"/>
+      <c r="F192" s="63"/>
+      <c r="H192" s="63"/>
+      <c r="I192" s="78"/>
+      <c r="J192" s="63"/>
+    </row>
+    <row r="193" spans="1:10">
+      <c r="A193">
+        <v>180</v>
+      </c>
+      <c r="C193" s="62"/>
+      <c r="D193" s="63"/>
+      <c r="E193" s="63"/>
+      <c r="F193" s="63"/>
+      <c r="H193" s="63"/>
+      <c r="I193" s="78"/>
+      <c r="J193" s="63"/>
+    </row>
+    <row r="194" spans="1:10">
+      <c r="A194">
+        <v>181</v>
+      </c>
+      <c r="C194" s="62"/>
+      <c r="D194" s="63"/>
+      <c r="E194" s="63"/>
+      <c r="F194" s="63"/>
+      <c r="H194" s="63"/>
+      <c r="I194" s="78"/>
+      <c r="J194" s="63"/>
+    </row>
+    <row r="195" spans="1:10">
+      <c r="A195">
+        <v>182</v>
+      </c>
+      <c r="C195" s="62"/>
+      <c r="D195" s="63"/>
+      <c r="E195" s="63"/>
+      <c r="F195" s="63"/>
+      <c r="H195" s="63"/>
+      <c r="I195" s="78"/>
+      <c r="J195" s="63"/>
+    </row>
+    <row r="196" spans="1:10">
+      <c r="A196">
+        <v>183</v>
+      </c>
+      <c r="C196" s="62"/>
+      <c r="D196" s="63"/>
+      <c r="E196" s="63"/>
+      <c r="F196" s="63"/>
+      <c r="H196" s="63"/>
+      <c r="I196" s="78"/>
+      <c r="J196" s="63"/>
+    </row>
+    <row r="197" spans="1:10">
+      <c r="A197">
+        <v>184</v>
+      </c>
+      <c r="C197" s="62"/>
+      <c r="D197" s="63"/>
+      <c r="E197" s="63"/>
+      <c r="F197" s="63"/>
+      <c r="H197" s="63"/>
+      <c r="I197" s="78"/>
+      <c r="J197" s="63"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
@@ -10439,7 +10650,7 @@
         <v>764</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="C1" s="14" t="s">
         <v>734</v>
@@ -10448,7 +10659,7 @@
         <v>645</v>
       </c>
       <c r="E1" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -10498,7 +10709,7 @@
         <v>1</v>
       </c>
       <c r="D5" s="39" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -10512,7 +10723,7 @@
         <v>6</v>
       </c>
       <c r="D6" s="39" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -10526,7 +10737,7 @@
         <v>9</v>
       </c>
       <c r="D7" s="39" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -10540,7 +10751,7 @@
         <v>12</v>
       </c>
       <c r="D8" s="39" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -10554,7 +10765,7 @@
         <v>15</v>
       </c>
       <c r="D9" s="39" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -10568,7 +10779,7 @@
         <v>18</v>
       </c>
       <c r="D10" s="39" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -10646,7 +10857,7 @@
         <v>23</v>
       </c>
       <c r="D16" s="39" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -10722,7 +10933,7 @@
         <v>643</v>
       </c>
       <c r="D22" s="43" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -10736,7 +10947,7 @@
         <v>28</v>
       </c>
       <c r="D23" s="39" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -10802,7 +11013,7 @@
         <v>74</v>
       </c>
       <c r="D28" s="39" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -10856,7 +11067,7 @@
         <v>32</v>
       </c>
       <c r="D32" s="39" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -10894,7 +11105,7 @@
         <v>646</v>
       </c>
       <c r="D35" s="43" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -10946,7 +11157,7 @@
         <v>79</v>
       </c>
       <c r="D39" s="39" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -10960,7 +11171,7 @@
         <v>37</v>
       </c>
       <c r="D40" s="39" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -11000,7 +11211,7 @@
         <v>42</v>
       </c>
       <c r="D43" s="39" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -11028,7 +11239,7 @@
         <v>47</v>
       </c>
       <c r="D45" s="39" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -11078,7 +11289,7 @@
         <v>52</v>
       </c>
       <c r="D49" s="39" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -11116,7 +11327,7 @@
         <v>654</v>
       </c>
       <c r="D52" s="43" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -11170,7 +11381,7 @@
         <v>84</v>
       </c>
       <c r="D56" s="39" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -11274,7 +11485,7 @@
         <v>89</v>
       </c>
       <c r="D64" s="39" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -11288,7 +11499,7 @@
         <v>57</v>
       </c>
       <c r="D65" s="39" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -11302,7 +11513,7 @@
         <v>648</v>
       </c>
       <c r="D66" s="43" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -11392,7 +11603,7 @@
         <v>653</v>
       </c>
       <c r="D73" s="43" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -11454,7 +11665,7 @@
         <v>61</v>
       </c>
       <c r="D78" s="47" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
     </row>
     <row r="79" spans="1:4">
@@ -11494,7 +11705,7 @@
         <v>650</v>
       </c>
       <c r="D81" s="43" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
     </row>
     <row r="82" spans="1:4">
@@ -11508,7 +11719,7 @@
         <v>94</v>
       </c>
       <c r="D82" s="39" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
     </row>
     <row r="83" spans="1:4">
@@ -11546,7 +11757,7 @@
         <v>64</v>
       </c>
       <c r="D85" s="39" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
     </row>
     <row r="86" spans="1:4">
@@ -11560,7 +11771,7 @@
         <v>98</v>
       </c>
       <c r="D86" s="39" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
     </row>
     <row r="87" spans="1:4">
@@ -11662,7 +11873,7 @@
         <v>67</v>
       </c>
       <c r="D94" s="14" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
     </row>
     <row r="95" spans="1:4">
@@ -11676,7 +11887,7 @@
         <v>695</v>
       </c>
       <c r="D95" s="14" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
     </row>
     <row r="96" spans="1:4">
@@ -11773,10 +11984,10 @@
         <v>711</v>
       </c>
       <c r="C103" s="14" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D103" s="14" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
     </row>
     <row r="104" spans="1:4">
@@ -11919,7 +12130,7 @@
         <v>765</v>
       </c>
       <c r="C115" s="14" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="D115" s="14" t="s">
         <v>772</v>
@@ -11933,7 +12144,7 @@
         <v>766</v>
       </c>
       <c r="C116" s="14" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="D116" s="14" t="s">
         <v>773</v>
@@ -12091,7 +12302,7 @@
         <v>901</v>
       </c>
       <c r="C129" s="14" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="D129" s="14"/>
     </row>
@@ -12101,7 +12312,7 @@
       </c>
       <c r="B130" s="13"/>
       <c r="C130" s="14" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="D130" s="14"/>
     </row>
@@ -12111,7 +12322,7 @@
       </c>
       <c r="B131" s="13"/>
       <c r="C131" s="14" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="D131" s="14"/>
     </row>
@@ -12121,7 +12332,7 @@
       </c>
       <c r="B132" s="13"/>
       <c r="C132" s="14" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="D132" s="14"/>
     </row>
@@ -12131,7 +12342,7 @@
       </c>
       <c r="B133" s="13"/>
       <c r="C133" s="14" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="D133" s="14"/>
     </row>
@@ -12141,7 +12352,7 @@
       </c>
       <c r="B134" s="15"/>
       <c r="C134" s="9" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="D134" s="9"/>
     </row>

</xml_diff>

<commit_message>
6 jiangnan Signed-off-by: twtcom001 <twtcom001@sina.com>
</commit_message>
<xml_diff>
--- a/统计清单/2017国内编号清单.xlsx
+++ b/统计清单/2017国内编号清单.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1921" uniqueCount="981">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1953" uniqueCount="991">
   <si>
     <t>本地编号</t>
   </si>
@@ -3620,6 +3620,46 @@
   </si>
   <si>
     <t>对版</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Echinopsis</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Echinopsis</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">盖伯·弗兰茨 </t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Chamaecereus</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Chamaecereus</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Chamaecereus Gelber Franz</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>天骄风信子</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>天骄风信子</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>江南百草园</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>江南百草园</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -3856,7 +3896,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3982,29 +4022,14 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="19">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -4328,6 +4353,23 @@
         <name val="宋体"/>
         <scheme val="minor"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -4409,20 +4451,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:M197" totalsRowShown="0">
-  <autoFilter ref="A1:M197"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:M205" totalsRowShown="0">
+  <autoFilter ref="A1:M205"/>
   <tableColumns count="13">
     <tableColumn id="1" name="145"/>
     <tableColumn id="2" name="属"/>
     <tableColumn id="3" name="属内编号" dataDxfId="18"/>
     <tableColumn id="4" name="拉丁名" dataDxfId="17"/>
     <tableColumn id="5" name="中文" dataDxfId="16"/>
-    <tableColumn id="9" name="对版" dataDxfId="0"/>
-    <tableColumn id="7" name="来源编号" dataDxfId="15"/>
+    <tableColumn id="9" name="对版" dataDxfId="15"/>
+    <tableColumn id="7" name="来源编号" dataDxfId="14"/>
     <tableColumn id="12" name="引进价格"/>
-    <tableColumn id="6" name="来源" dataDxfId="14"/>
-    <tableColumn id="8" name="参考链接" dataDxfId="13" dataCellStyle="超链接"/>
-    <tableColumn id="10" name="引进尺寸2" dataDxfId="12"/>
+    <tableColumn id="6" name="来源" dataDxfId="13"/>
+    <tableColumn id="8" name="参考链接" dataDxfId="12" dataCellStyle="超链接"/>
+    <tableColumn id="10" name="引进尺寸2" dataDxfId="11"/>
     <tableColumn id="11" name="引进日期"/>
     <tableColumn id="13" name="备注"/>
   </tableColumns>
@@ -4435,9 +4477,9 @@
   <autoFilter ref="A1:E162"/>
   <tableColumns count="5">
     <tableColumn id="1" name="145"/>
-    <tableColumn id="3" name="编号" dataDxfId="11"/>
-    <tableColumn id="5" name="中文" dataDxfId="10"/>
-    <tableColumn id="7" name="来源编号" dataDxfId="9"/>
+    <tableColumn id="3" name="编号" dataDxfId="10"/>
+    <tableColumn id="5" name="中文" dataDxfId="9"/>
+    <tableColumn id="7" name="来源编号" dataDxfId="8"/>
     <tableColumn id="2" name="数量"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -4445,16 +4487,20 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A1:G129" totalsRowShown="0" dataDxfId="8">
-  <autoFilter ref="A1:G129"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A1:G129" totalsRowShown="0" dataDxfId="7">
+  <autoFilter ref="A1:G129">
+    <filterColumn colId="6">
+      <filters blank="1"/>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="7">
-    <tableColumn id="1" name="本地编号" dataDxfId="7"/>
-    <tableColumn id="2" name="编号" dataDxfId="6"/>
-    <tableColumn id="5" name="中文名" dataDxfId="5"/>
-    <tableColumn id="6" name="购买目标" dataDxfId="4"/>
-    <tableColumn id="7" name="来源编号" dataDxfId="3"/>
-    <tableColumn id="4" name="链接" dataDxfId="2"/>
-    <tableColumn id="3" name="购买数量" dataDxfId="1"/>
+    <tableColumn id="1" name="本地编号" dataDxfId="6"/>
+    <tableColumn id="2" name="编号" dataDxfId="5"/>
+    <tableColumn id="5" name="中文名" dataDxfId="4"/>
+    <tableColumn id="6" name="购买目标" dataDxfId="3"/>
+    <tableColumn id="7" name="来源编号" dataDxfId="2"/>
+    <tableColumn id="4" name="链接" dataDxfId="1"/>
+    <tableColumn id="3" name="购买数量" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4747,10 +4793,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M197"/>
+  <dimension ref="A1:M205"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="F72" sqref="F72"/>
+    <sheetView tabSelected="1" topLeftCell="A172" workbookViewId="0">
+      <selection activeCell="I192" sqref="I192:I197"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -10365,7 +10411,7 @@
         <v>165</v>
       </c>
       <c r="B178" s="3" t="s">
-        <v>787</v>
+        <v>984</v>
       </c>
       <c r="C178" s="15"/>
       <c r="D178" s="9"/>
@@ -10519,7 +10565,7 @@
         <v>171</v>
       </c>
       <c r="B184" s="37" t="s">
-        <v>955</v>
+        <v>981</v>
       </c>
       <c r="C184" s="77" t="s">
         <v>172</v>
@@ -10590,7 +10636,7 @@
         <v>30</v>
       </c>
       <c r="I186" s="39" t="s">
-        <v>482</v>
+        <v>989</v>
       </c>
       <c r="J186" s="66"/>
       <c r="K186" s="39"/>
@@ -10647,7 +10693,9 @@
       </c>
       <c r="F189" s="14"/>
       <c r="G189" s="9"/>
-      <c r="I189" s="9"/>
+      <c r="I189" s="14" t="s">
+        <v>987</v>
+      </c>
       <c r="J189" s="64"/>
       <c r="K189" s="9"/>
     </row>
@@ -10665,7 +10713,9 @@
       </c>
       <c r="F190" s="60"/>
       <c r="G190" s="63"/>
-      <c r="I190" s="63"/>
+      <c r="I190" s="60" t="s">
+        <v>988</v>
+      </c>
       <c r="J190" s="78"/>
       <c r="K190" s="63"/>
     </row>
@@ -10683,7 +10733,9 @@
       </c>
       <c r="F191" s="60"/>
       <c r="G191" s="63"/>
-      <c r="I191" s="63"/>
+      <c r="I191" s="60" t="s">
+        <v>987</v>
+      </c>
       <c r="J191" s="78"/>
       <c r="K191" s="63"/>
     </row>
@@ -10691,12 +10743,23 @@
       <c r="A192">
         <v>179</v>
       </c>
-      <c r="C192" s="62"/>
-      <c r="D192" s="63"/>
-      <c r="E192" s="63"/>
+      <c r="B192" s="3" t="s">
+        <v>982</v>
+      </c>
+      <c r="C192" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D192" s="4" t="s">
+        <v>660</v>
+      </c>
+      <c r="E192" s="4" t="s">
+        <v>618</v>
+      </c>
       <c r="F192" s="63"/>
       <c r="G192" s="63"/>
-      <c r="I192" s="63"/>
+      <c r="I192" s="60" t="s">
+        <v>990</v>
+      </c>
       <c r="J192" s="78"/>
       <c r="K192" s="63"/>
     </row>
@@ -10704,12 +10767,23 @@
       <c r="A193">
         <v>180</v>
       </c>
-      <c r="C193" s="62"/>
-      <c r="D193" s="63"/>
-      <c r="E193" s="63"/>
+      <c r="B193" s="3" t="s">
+        <v>982</v>
+      </c>
+      <c r="C193" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D193" s="4" t="s">
+        <v>662</v>
+      </c>
+      <c r="E193" s="4" t="s">
+        <v>663</v>
+      </c>
       <c r="F193" s="63"/>
       <c r="G193" s="63"/>
-      <c r="I193" s="63"/>
+      <c r="I193" s="60" t="s">
+        <v>990</v>
+      </c>
       <c r="J193" s="78"/>
       <c r="K193" s="63"/>
     </row>
@@ -10717,12 +10791,23 @@
       <c r="A194">
         <v>181</v>
       </c>
-      <c r="C194" s="62"/>
-      <c r="D194" s="63"/>
-      <c r="E194" s="63"/>
+      <c r="B194" s="3" t="s">
+        <v>982</v>
+      </c>
+      <c r="C194" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D194" s="4" t="s">
+        <v>668</v>
+      </c>
+      <c r="E194" s="4" t="s">
+        <v>669</v>
+      </c>
       <c r="F194" s="63"/>
       <c r="G194" s="63"/>
-      <c r="I194" s="63"/>
+      <c r="I194" s="60" t="s">
+        <v>990</v>
+      </c>
       <c r="J194" s="78"/>
       <c r="K194" s="63"/>
     </row>
@@ -10730,12 +10815,23 @@
       <c r="A195">
         <v>182</v>
       </c>
-      <c r="C195" s="62"/>
-      <c r="D195" s="63"/>
-      <c r="E195" s="63"/>
+      <c r="B195" s="3" t="s">
+        <v>982</v>
+      </c>
+      <c r="C195" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="D195" s="4" t="s">
+        <v>831</v>
+      </c>
+      <c r="E195" s="4" t="s">
+        <v>833</v>
+      </c>
       <c r="F195" s="63"/>
       <c r="G195" s="63"/>
-      <c r="I195" s="63"/>
+      <c r="I195" s="60" t="s">
+        <v>990</v>
+      </c>
       <c r="J195" s="78"/>
       <c r="K195" s="63"/>
     </row>
@@ -10743,12 +10839,23 @@
       <c r="A196">
         <v>183</v>
       </c>
-      <c r="C196" s="62"/>
-      <c r="D196" s="63"/>
-      <c r="E196" s="63"/>
+      <c r="B196" s="3" t="s">
+        <v>982</v>
+      </c>
+      <c r="C196" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="D196" s="4" t="s">
+        <v>834</v>
+      </c>
+      <c r="E196" s="4" t="s">
+        <v>836</v>
+      </c>
       <c r="F196" s="63"/>
       <c r="G196" s="63"/>
-      <c r="I196" s="63"/>
+      <c r="I196" s="60" t="s">
+        <v>990</v>
+      </c>
       <c r="J196" s="78"/>
       <c r="K196" s="63"/>
     </row>
@@ -10756,14 +10863,127 @@
       <c r="A197">
         <v>184</v>
       </c>
+      <c r="B197" s="3" t="s">
+        <v>985</v>
+      </c>
       <c r="C197" s="62"/>
-      <c r="D197" s="63"/>
-      <c r="E197" s="63"/>
+      <c r="D197" s="60" t="s">
+        <v>986</v>
+      </c>
+      <c r="E197" s="60" t="s">
+        <v>983</v>
+      </c>
       <c r="F197" s="63"/>
       <c r="G197" s="63"/>
-      <c r="I197" s="63"/>
+      <c r="I197" s="60" t="s">
+        <v>990</v>
+      </c>
       <c r="J197" s="78"/>
       <c r="K197" s="63"/>
+    </row>
+    <row r="198" spans="1:11">
+      <c r="A198">
+        <v>185</v>
+      </c>
+      <c r="C198" s="13"/>
+      <c r="D198" s="14"/>
+      <c r="E198" s="14"/>
+      <c r="F198" s="3"/>
+      <c r="G198" s="14"/>
+      <c r="I198" s="14"/>
+      <c r="J198" s="11"/>
+      <c r="K198" s="14"/>
+    </row>
+    <row r="199" spans="1:11">
+      <c r="A199">
+        <v>186</v>
+      </c>
+      <c r="C199" s="79"/>
+      <c r="D199" s="60"/>
+      <c r="E199" s="60"/>
+      <c r="F199" s="3"/>
+      <c r="G199" s="60"/>
+      <c r="I199" s="60"/>
+      <c r="J199" s="80"/>
+      <c r="K199" s="60"/>
+    </row>
+    <row r="200" spans="1:11">
+      <c r="A200">
+        <v>187</v>
+      </c>
+      <c r="C200" s="79"/>
+      <c r="D200" s="60"/>
+      <c r="E200" s="60"/>
+      <c r="F200" s="3"/>
+      <c r="G200" s="60"/>
+      <c r="I200" s="60"/>
+      <c r="J200" s="80"/>
+      <c r="K200" s="60"/>
+    </row>
+    <row r="201" spans="1:11">
+      <c r="A201">
+        <v>188</v>
+      </c>
+      <c r="C201" s="79"/>
+      <c r="D201" s="60"/>
+      <c r="E201" s="60"/>
+      <c r="F201" s="3"/>
+      <c r="G201" s="60"/>
+      <c r="I201" s="60"/>
+      <c r="J201" s="80"/>
+      <c r="K201" s="60"/>
+    </row>
+    <row r="202" spans="1:11">
+      <c r="A202">
+        <v>189</v>
+      </c>
+      <c r="C202" s="79"/>
+      <c r="D202" s="60"/>
+      <c r="E202" s="60"/>
+      <c r="F202" s="3"/>
+      <c r="G202" s="60"/>
+      <c r="I202" s="60"/>
+      <c r="J202" s="80"/>
+      <c r="K202" s="60"/>
+    </row>
+    <row r="203" spans="1:11">
+      <c r="A203">
+        <v>190</v>
+      </c>
+      <c r="C203" s="79"/>
+      <c r="D203" s="60"/>
+      <c r="E203" s="60"/>
+      <c r="F203" s="3"/>
+      <c r="G203" s="60"/>
+      <c r="I203" s="60"/>
+      <c r="J203" s="80"/>
+      <c r="K203" s="60"/>
+    </row>
+    <row r="204" spans="1:11">
+      <c r="A204">
+        <v>191</v>
+      </c>
+      <c r="C204" s="79"/>
+      <c r="D204" s="60"/>
+      <c r="E204" s="60"/>
+      <c r="F204" s="3"/>
+      <c r="G204" s="60"/>
+      <c r="I204" s="60"/>
+      <c r="J204" s="80"/>
+      <c r="K204" s="60"/>
+    </row>
+    <row r="205" spans="1:11">
+      <c r="A205">
+        <v>192</v>
+      </c>
+      <c r="C205" s="79"/>
+      <c r="D205" s="60"/>
+      <c r="E205" s="60"/>
+      <c r="F205" s="3"/>
+      <c r="G205" s="60"/>
+      <c r="I205" s="60"/>
+      <c r="J205" s="80"/>
+      <c r="K205" s="60"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
@@ -13877,8 +14097,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J129"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:B123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -13888,7 +14108,7 @@
     <col min="3" max="3" width="12.5" style="1" customWidth="1"/>
     <col min="4" max="4" width="12.125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="41" style="1" customWidth="1"/>
+    <col min="6" max="6" width="49.375" style="1" customWidth="1"/>
     <col min="7" max="7" width="10.5" style="1" customWidth="1"/>
     <col min="8" max="8" width="10.75" style="1" customWidth="1"/>
     <col min="11" max="16384" width="9" style="1"/>
@@ -13919,7 +14139,7 @@
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" hidden="1">
       <c r="A2" s="4" t="s">
         <v>103</v>
       </c>
@@ -13942,7 +14162,7 @@
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" hidden="1">
       <c r="A3" s="4" t="s">
         <v>104</v>
       </c>
@@ -13955,11 +14175,13 @@
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
       <c r="F3" s="4"/>
-      <c r="G3" s="5"/>
+      <c r="G3" s="5">
+        <v>1</v>
+      </c>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" hidden="1">
       <c r="A4" s="4" t="s">
         <v>105</v>
       </c>
@@ -13980,7 +14202,7 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" hidden="1">
       <c r="A5" s="4" t="s">
         <v>106</v>
       </c>
@@ -14003,7 +14225,7 @@
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" hidden="1">
       <c r="A6" s="4" t="s">
         <v>107</v>
       </c>
@@ -14020,7 +14242,7 @@
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" hidden="1">
       <c r="A7" s="4" t="s">
         <v>108</v>
       </c>
@@ -14037,7 +14259,7 @@
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" hidden="1">
       <c r="A8" s="4" t="s">
         <v>109</v>
       </c>
@@ -14054,7 +14276,7 @@
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" hidden="1">
       <c r="A9" s="4" t="s">
         <v>21</v>
       </c>
@@ -14088,7 +14310,7 @@
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" hidden="1">
       <c r="A11" s="4" t="s">
         <v>111</v>
       </c>
@@ -14122,7 +14344,7 @@
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" hidden="1">
       <c r="A13" s="4" t="s">
         <v>113</v>
       </c>
@@ -14139,7 +14361,7 @@
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" hidden="1">
       <c r="A14" s="4" t="s">
         <v>114</v>
       </c>
@@ -14162,7 +14384,7 @@
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" hidden="1">
       <c r="A15" s="4" t="s">
         <v>115</v>
       </c>
@@ -14175,11 +14397,13 @@
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
       <c r="F15" s="4"/>
-      <c r="G15" s="5"/>
+      <c r="G15" s="5">
+        <v>1</v>
+      </c>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" hidden="1">
       <c r="A16" s="4" t="s">
         <v>116</v>
       </c>
@@ -14213,7 +14437,7 @@
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" hidden="1">
       <c r="A18" s="4" t="s">
         <v>118</v>
       </c>
@@ -14247,7 +14471,7 @@
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" hidden="1">
       <c r="A20" s="4" t="s">
         <v>120</v>
       </c>
@@ -14260,11 +14484,13 @@
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="4"/>
-      <c r="G20" s="5"/>
+      <c r="G20" s="5">
+        <v>1</v>
+      </c>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" hidden="1">
       <c r="A21" s="4" t="s">
         <v>121</v>
       </c>
@@ -14287,7 +14513,7 @@
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" hidden="1">
       <c r="A22" s="4" t="s">
         <v>26</v>
       </c>
@@ -14304,7 +14530,7 @@
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" hidden="1">
       <c r="A23" s="4" t="s">
         <v>122</v>
       </c>
@@ -14342,7 +14568,7 @@
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" hidden="1">
       <c r="A25" s="4" t="s">
         <v>124</v>
       </c>
@@ -14365,7 +14591,7 @@
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
     </row>
-    <row r="26" spans="1:10" ht="27">
+    <row r="26" spans="1:10" ht="27" hidden="1">
       <c r="A26" s="4" t="s">
         <v>125</v>
       </c>
@@ -14388,7 +14614,7 @@
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" hidden="1">
       <c r="A27" s="4" t="s">
         <v>126</v>
       </c>
@@ -14411,7 +14637,7 @@
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" hidden="1">
       <c r="A28" s="4" t="s">
         <v>127</v>
       </c>
@@ -14428,7 +14654,7 @@
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" hidden="1">
       <c r="A29" s="4" t="s">
         <v>72</v>
       </c>
@@ -14445,7 +14671,7 @@
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" hidden="1">
       <c r="A30" s="4" t="s">
         <v>128</v>
       </c>
@@ -14485,7 +14711,7 @@
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" hidden="1">
       <c r="A32" s="4" t="s">
         <v>130</v>
       </c>
@@ -14508,7 +14734,7 @@
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" hidden="1">
       <c r="A33" s="4" t="s">
         <v>131</v>
       </c>
@@ -14525,7 +14751,7 @@
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" hidden="1">
       <c r="A34" s="4" t="s">
         <v>31</v>
       </c>
@@ -14542,7 +14768,7 @@
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" hidden="1">
       <c r="A35" s="4" t="s">
         <v>132</v>
       </c>
@@ -14559,7 +14785,7 @@
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" hidden="1">
       <c r="A36" s="4" t="s">
         <v>133</v>
       </c>
@@ -14576,7 +14802,7 @@
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" hidden="1">
       <c r="A37" s="4" t="s">
         <v>134</v>
       </c>
@@ -14599,7 +14825,7 @@
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" hidden="1">
       <c r="A38" s="4" t="s">
         <v>135</v>
       </c>
@@ -14616,7 +14842,7 @@
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" hidden="1">
       <c r="A39" s="4" t="s">
         <v>136</v>
       </c>
@@ -14639,7 +14865,7 @@
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" hidden="1">
       <c r="A40" s="4" t="s">
         <v>137</v>
       </c>
@@ -14656,7 +14882,7 @@
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" hidden="1">
       <c r="A41" s="4" t="s">
         <v>138</v>
       </c>
@@ -14694,7 +14920,7 @@
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
     </row>
-    <row r="43" spans="1:10" ht="27">
+    <row r="43" spans="1:10" ht="27" hidden="1">
       <c r="A43" s="4" t="s">
         <v>140</v>
       </c>
@@ -14715,7 +14941,7 @@
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" hidden="1">
       <c r="A44" s="4" t="s">
         <v>77</v>
       </c>
@@ -14732,7 +14958,7 @@
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
     </row>
-    <row r="45" spans="1:10" ht="27">
+    <row r="45" spans="1:10" ht="27" hidden="1">
       <c r="A45" s="4" t="s">
         <v>141</v>
       </c>
@@ -14753,7 +14979,7 @@
       <c r="I45" s="1"/>
       <c r="J45" s="1"/>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:10" hidden="1">
       <c r="A46" s="4" t="s">
         <v>35</v>
       </c>
@@ -14770,7 +14996,7 @@
       <c r="I46" s="1"/>
       <c r="J46" s="1"/>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" hidden="1">
       <c r="A47" s="4" t="s">
         <v>142</v>
       </c>
@@ -14793,7 +15019,7 @@
       <c r="I47" s="1"/>
       <c r="J47" s="1"/>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:10" hidden="1">
       <c r="A48" s="4" t="s">
         <v>143</v>
       </c>
@@ -14810,7 +15036,7 @@
       <c r="I48" s="1"/>
       <c r="J48" s="1"/>
     </row>
-    <row r="49" spans="1:10">
+    <row r="49" spans="1:10" hidden="1">
       <c r="A49" s="4" t="s">
         <v>40</v>
       </c>
@@ -14827,7 +15053,7 @@
       <c r="I49" s="1"/>
       <c r="J49" s="1"/>
     </row>
-    <row r="50" spans="1:10">
+    <row r="50" spans="1:10" hidden="1">
       <c r="A50" s="4" t="s">
         <v>144</v>
       </c>
@@ -14850,7 +15076,7 @@
       <c r="I50" s="1"/>
       <c r="J50" s="1"/>
     </row>
-    <row r="51" spans="1:10">
+    <row r="51" spans="1:10" hidden="1">
       <c r="A51" s="4" t="s">
         <v>45</v>
       </c>
@@ -14867,7 +15093,7 @@
       <c r="I51" s="1"/>
       <c r="J51" s="1"/>
     </row>
-    <row r="52" spans="1:10">
+    <row r="52" spans="1:10" hidden="1">
       <c r="A52" s="4" t="s">
         <v>145</v>
       </c>
@@ -14884,7 +15110,7 @@
       <c r="I52" s="1"/>
       <c r="J52" s="1"/>
     </row>
-    <row r="53" spans="1:10">
+    <row r="53" spans="1:10" hidden="1">
       <c r="A53" s="4" t="s">
         <v>146</v>
       </c>
@@ -14901,7 +15127,7 @@
       <c r="I53" s="1"/>
       <c r="J53" s="1"/>
     </row>
-    <row r="54" spans="1:10">
+    <row r="54" spans="1:10" hidden="1">
       <c r="A54" s="4" t="s">
         <v>147</v>
       </c>
@@ -14937,7 +15163,7 @@
       <c r="I55" s="1"/>
       <c r="J55" s="1"/>
     </row>
-    <row r="56" spans="1:10">
+    <row r="56" spans="1:10" hidden="1">
       <c r="A56" s="4" t="s">
         <v>50</v>
       </c>
@@ -14992,7 +15218,7 @@
       <c r="I58" s="1"/>
       <c r="J58" s="1"/>
     </row>
-    <row r="59" spans="1:10">
+    <row r="59" spans="1:10" hidden="1">
       <c r="A59" s="4" t="s">
         <v>151</v>
       </c>
@@ -15009,7 +15235,7 @@
       <c r="I59" s="1"/>
       <c r="J59" s="1"/>
     </row>
-    <row r="60" spans="1:10">
+    <row r="60" spans="1:10" hidden="1">
       <c r="A60" s="4" t="s">
         <v>398</v>
       </c>
@@ -15026,7 +15252,7 @@
       <c r="I60" s="1"/>
       <c r="J60" s="1"/>
     </row>
-    <row r="61" spans="1:10">
+    <row r="61" spans="1:10" hidden="1">
       <c r="A61" s="4" t="s">
         <v>152</v>
       </c>
@@ -15068,7 +15294,7 @@
       <c r="I62" s="1"/>
       <c r="J62" s="1"/>
     </row>
-    <row r="63" spans="1:10">
+    <row r="63" spans="1:10" hidden="1">
       <c r="A63" s="4" t="s">
         <v>154</v>
       </c>
@@ -15091,7 +15317,7 @@
       <c r="I63" s="1"/>
       <c r="J63" s="1"/>
     </row>
-    <row r="64" spans="1:10" ht="27">
+    <row r="64" spans="1:10" ht="27" hidden="1">
       <c r="A64" s="4" t="s">
         <v>155</v>
       </c>
@@ -15131,7 +15357,7 @@
       <c r="I65" s="1"/>
       <c r="J65" s="1"/>
     </row>
-    <row r="66" spans="1:10">
+    <row r="66" spans="1:10" hidden="1">
       <c r="A66" s="4" t="s">
         <v>336</v>
       </c>
@@ -15167,7 +15393,7 @@
       <c r="I67" s="1"/>
       <c r="J67" s="1"/>
     </row>
-    <row r="68" spans="1:10">
+    <row r="68" spans="1:10" hidden="1">
       <c r="A68" s="4" t="s">
         <v>158</v>
       </c>
@@ -15190,7 +15416,7 @@
       <c r="I68" s="1"/>
       <c r="J68" s="1"/>
     </row>
-    <row r="69" spans="1:10">
+    <row r="69" spans="1:10" hidden="1">
       <c r="A69" s="4" t="s">
         <v>82</v>
       </c>
@@ -15226,7 +15452,7 @@
       <c r="I70" s="1"/>
       <c r="J70" s="1"/>
     </row>
-    <row r="71" spans="1:10">
+    <row r="71" spans="1:10" hidden="1">
       <c r="A71" s="4" t="s">
         <v>160</v>
       </c>
@@ -15249,7 +15475,7 @@
       <c r="I71" s="1"/>
       <c r="J71" s="1"/>
     </row>
-    <row r="72" spans="1:10">
+    <row r="72" spans="1:10" hidden="1">
       <c r="A72" s="4" t="s">
         <v>161</v>
       </c>
@@ -15272,7 +15498,7 @@
       <c r="I72" s="1"/>
       <c r="J72" s="1"/>
     </row>
-    <row r="73" spans="1:10" ht="27">
+    <row r="73" spans="1:10" ht="27" hidden="1">
       <c r="A73" s="4" t="s">
         <v>162</v>
       </c>
@@ -15289,11 +15515,13 @@
       <c r="F73" s="7" t="s">
         <v>832</v>
       </c>
-      <c r="G73" s="5"/>
+      <c r="G73" s="5">
+        <v>1</v>
+      </c>
       <c r="I73" s="1"/>
       <c r="J73" s="1"/>
     </row>
-    <row r="74" spans="1:10" ht="27">
+    <row r="74" spans="1:10" ht="27" hidden="1">
       <c r="A74" s="4" t="s">
         <v>163</v>
       </c>
@@ -15308,7 +15536,9 @@
       <c r="F74" s="7" t="s">
         <v>835</v>
       </c>
-      <c r="G74" s="5"/>
+      <c r="G74" s="5">
+        <v>1</v>
+      </c>
       <c r="I74" s="1"/>
       <c r="J74" s="1"/>
     </row>
@@ -15388,7 +15618,7 @@
       <c r="I78" s="1"/>
       <c r="J78" s="1"/>
     </row>
-    <row r="79" spans="1:10">
+    <row r="79" spans="1:10" hidden="1">
       <c r="A79" s="4" t="s">
         <v>168</v>
       </c>
@@ -15447,7 +15677,7 @@
       <c r="I81" s="1"/>
       <c r="J81" s="1"/>
     </row>
-    <row r="82" spans="1:10">
+    <row r="82" spans="1:10" hidden="1">
       <c r="A82" s="4" t="s">
         <v>171</v>
       </c>
@@ -15464,7 +15694,7 @@
       <c r="I82" s="1"/>
       <c r="J82" s="1"/>
     </row>
-    <row r="83" spans="1:10" ht="27">
+    <row r="83" spans="1:10" ht="27" hidden="1">
       <c r="A83" s="4" t="s">
         <v>172</v>
       </c>
@@ -15485,7 +15715,7 @@
       <c r="I83" s="1"/>
       <c r="J83" s="1"/>
     </row>
-    <row r="84" spans="1:10">
+    <row r="84" spans="1:10" hidden="1">
       <c r="A84" s="4" t="s">
         <v>173</v>
       </c>
@@ -15502,7 +15732,7 @@
       <c r="I84" s="1"/>
       <c r="J84" s="1"/>
     </row>
-    <row r="85" spans="1:10">
+    <row r="85" spans="1:10" hidden="1">
       <c r="A85" s="4" t="s">
         <v>174</v>
       </c>
@@ -15525,7 +15755,7 @@
       <c r="I85" s="1"/>
       <c r="J85" s="1"/>
     </row>
-    <row r="86" spans="1:10" ht="27">
+    <row r="86" spans="1:10" ht="27" hidden="1">
       <c r="A86" s="4" t="s">
         <v>175</v>
       </c>
@@ -15548,7 +15778,7 @@
       <c r="I86" s="1"/>
       <c r="J86" s="1"/>
     </row>
-    <row r="87" spans="1:10">
+    <row r="87" spans="1:10" hidden="1">
       <c r="A87" s="4" t="s">
         <v>176</v>
       </c>
@@ -15584,7 +15814,7 @@
       <c r="I88" s="1"/>
       <c r="J88" s="1"/>
     </row>
-    <row r="89" spans="1:10" ht="27">
+    <row r="89" spans="1:10" ht="27" hidden="1">
       <c r="A89" s="4" t="s">
         <v>178</v>
       </c>
@@ -15605,7 +15835,7 @@
       <c r="I89" s="1"/>
       <c r="J89" s="1"/>
     </row>
-    <row r="90" spans="1:10">
+    <row r="90" spans="1:10" hidden="1">
       <c r="A90" s="4" t="s">
         <v>87</v>
       </c>
@@ -15622,7 +15852,7 @@
       <c r="I90" s="1"/>
       <c r="J90" s="1"/>
     </row>
-    <row r="91" spans="1:10">
+    <row r="91" spans="1:10" hidden="1">
       <c r="A91" s="4" t="s">
         <v>55</v>
       </c>
@@ -15639,7 +15869,7 @@
       <c r="I91" s="1"/>
       <c r="J91" s="1"/>
     </row>
-    <row r="92" spans="1:10">
+    <row r="92" spans="1:10" hidden="1">
       <c r="A92" s="4" t="s">
         <v>179</v>
       </c>
@@ -15662,7 +15892,7 @@
       <c r="I92" s="1"/>
       <c r="J92" s="1"/>
     </row>
-    <row r="93" spans="1:10">
+    <row r="93" spans="1:10" hidden="1">
       <c r="A93" s="4" t="s">
         <v>180</v>
       </c>
@@ -15679,7 +15909,7 @@
       <c r="I93" s="1"/>
       <c r="J93" s="1"/>
     </row>
-    <row r="94" spans="1:10" ht="27">
+    <row r="94" spans="1:10" ht="27" hidden="1">
       <c r="A94" s="4" t="s">
         <v>181</v>
       </c>
@@ -15719,7 +15949,7 @@
       <c r="I95" s="1"/>
       <c r="J95" s="1"/>
     </row>
-    <row r="96" spans="1:10">
+    <row r="96" spans="1:10" hidden="1">
       <c r="A96" s="4" t="s">
         <v>183</v>
       </c>
@@ -15742,7 +15972,7 @@
       <c r="I96" s="1"/>
       <c r="J96" s="1"/>
     </row>
-    <row r="97" spans="1:10">
+    <row r="97" spans="1:10" hidden="1">
       <c r="A97" s="4" t="s">
         <v>184</v>
       </c>
@@ -15759,7 +15989,7 @@
       <c r="I97" s="1"/>
       <c r="J97" s="1"/>
     </row>
-    <row r="98" spans="1:10">
+    <row r="98" spans="1:10" hidden="1">
       <c r="A98" s="4" t="s">
         <v>348</v>
       </c>
@@ -15795,7 +16025,7 @@
       <c r="I99" s="1"/>
       <c r="J99" s="1"/>
     </row>
-    <row r="100" spans="1:10" ht="27">
+    <row r="100" spans="1:10" ht="27" hidden="1">
       <c r="A100" s="4" t="s">
         <v>186</v>
       </c>
@@ -15818,7 +16048,7 @@
       <c r="I100" s="1"/>
       <c r="J100" s="1"/>
     </row>
-    <row r="101" spans="1:10">
+    <row r="101" spans="1:10" hidden="1">
       <c r="A101" s="4" t="s">
         <v>187</v>
       </c>
@@ -15839,7 +16069,7 @@
       <c r="I101" s="1"/>
       <c r="J101" s="1"/>
     </row>
-    <row r="102" spans="1:10">
+    <row r="102" spans="1:10" hidden="1">
       <c r="A102" s="4" t="s">
         <v>188</v>
       </c>
@@ -15862,7 +16092,7 @@
       <c r="I102" s="1"/>
       <c r="J102" s="1"/>
     </row>
-    <row r="103" spans="1:10">
+    <row r="103" spans="1:10" hidden="1">
       <c r="A103" s="4" t="s">
         <v>189</v>
       </c>
@@ -15898,7 +16128,7 @@
       <c r="I104" s="1"/>
       <c r="J104" s="1"/>
     </row>
-    <row r="105" spans="1:10">
+    <row r="105" spans="1:10" hidden="1">
       <c r="A105" s="4" t="s">
         <v>191</v>
       </c>
@@ -15921,7 +16151,7 @@
       <c r="I105" s="1"/>
       <c r="J105" s="1"/>
     </row>
-    <row r="106" spans="1:10">
+    <row r="106" spans="1:10" hidden="1">
       <c r="A106" s="4" t="s">
         <v>192</v>
       </c>
@@ -15938,7 +16168,7 @@
       <c r="I106" s="1"/>
       <c r="J106" s="1"/>
     </row>
-    <row r="107" spans="1:10">
+    <row r="107" spans="1:10" hidden="1">
       <c r="A107" s="4" t="s">
         <v>193</v>
       </c>
@@ -15955,7 +16185,7 @@
       <c r="I107" s="1"/>
       <c r="J107" s="1"/>
     </row>
-    <row r="108" spans="1:10">
+    <row r="108" spans="1:10" hidden="1">
       <c r="A108" s="4" t="s">
         <v>194</v>
       </c>
@@ -15972,7 +16202,7 @@
       <c r="I108" s="1"/>
       <c r="J108" s="1"/>
     </row>
-    <row r="109" spans="1:10">
+    <row r="109" spans="1:10" hidden="1">
       <c r="A109" s="4" t="s">
         <v>195</v>
       </c>
@@ -15989,7 +16219,7 @@
       <c r="I109" s="1"/>
       <c r="J109" s="1"/>
     </row>
-    <row r="110" spans="1:10">
+    <row r="110" spans="1:10" hidden="1">
       <c r="A110" s="4" t="s">
         <v>60</v>
       </c>
@@ -16025,7 +16255,7 @@
       <c r="I111" s="1"/>
       <c r="J111" s="1"/>
     </row>
-    <row r="112" spans="1:10">
+    <row r="112" spans="1:10" hidden="1">
       <c r="A112" s="4" t="s">
         <v>197</v>
       </c>
@@ -16042,7 +16272,7 @@
       <c r="I112" s="1"/>
       <c r="J112" s="1"/>
     </row>
-    <row r="113" spans="1:10">
+    <row r="113" spans="1:10" hidden="1">
       <c r="A113" s="4" t="s">
         <v>198</v>
       </c>
@@ -16065,7 +16295,7 @@
       <c r="I113" s="1"/>
       <c r="J113" s="1"/>
     </row>
-    <row r="114" spans="1:10">
+    <row r="114" spans="1:10" hidden="1">
       <c r="A114" s="4" t="s">
         <v>199</v>
       </c>
@@ -16088,7 +16318,7 @@
       <c r="I114" s="1"/>
       <c r="J114" s="1"/>
     </row>
-    <row r="115" spans="1:10">
+    <row r="115" spans="1:10" hidden="1">
       <c r="A115" s="4" t="s">
         <v>92</v>
       </c>
@@ -16105,7 +16335,7 @@
       <c r="I115" s="1"/>
       <c r="J115" s="1"/>
     </row>
-    <row r="116" spans="1:10">
+    <row r="116" spans="1:10" hidden="1">
       <c r="A116" s="4" t="s">
         <v>200</v>
       </c>
@@ -16122,7 +16352,7 @@
       <c r="I116" s="1"/>
       <c r="J116" s="1"/>
     </row>
-    <row r="117" spans="1:10">
+    <row r="117" spans="1:10" hidden="1">
       <c r="A117" s="4" t="s">
         <v>201</v>
       </c>
@@ -16139,7 +16369,7 @@
       <c r="I117" s="1"/>
       <c r="J117" s="1"/>
     </row>
-    <row r="118" spans="1:10">
+    <row r="118" spans="1:10" hidden="1">
       <c r="A118" s="4" t="s">
         <v>63</v>
       </c>
@@ -16156,7 +16386,7 @@
       <c r="I118" s="1"/>
       <c r="J118" s="1"/>
     </row>
-    <row r="119" spans="1:10">
+    <row r="119" spans="1:10" hidden="1">
       <c r="A119" s="4" t="s">
         <v>97</v>
       </c>
@@ -16173,7 +16403,7 @@
       <c r="I119" s="1"/>
       <c r="J119" s="1"/>
     </row>
-    <row r="120" spans="1:10">
+    <row r="120" spans="1:10" hidden="1">
       <c r="A120" s="4" t="s">
         <v>202</v>
       </c>
@@ -16196,7 +16426,7 @@
       <c r="I120" s="1"/>
       <c r="J120" s="1"/>
     </row>
-    <row r="121" spans="1:10">
+    <row r="121" spans="1:10" hidden="1">
       <c r="A121" s="4" t="s">
         <v>203</v>
       </c>
@@ -16251,7 +16481,7 @@
       <c r="I123" s="1"/>
       <c r="J123" s="1"/>
     </row>
-    <row r="124" spans="1:10">
+    <row r="124" spans="1:10" hidden="1">
       <c r="A124" s="4" t="s">
         <v>206</v>
       </c>
@@ -16274,7 +16504,7 @@
       <c r="I124" s="1"/>
       <c r="J124" s="1"/>
     </row>
-    <row r="125" spans="1:10">
+    <row r="125" spans="1:10" hidden="1">
       <c r="A125" s="4" t="s">
         <v>207</v>
       </c>
@@ -16297,7 +16527,7 @@
       <c r="I125" s="1"/>
       <c r="J125" s="1"/>
     </row>
-    <row r="126" spans="1:10">
+    <row r="126" spans="1:10" hidden="1">
       <c r="A126" s="4" t="s">
         <v>208</v>
       </c>
@@ -16314,7 +16544,7 @@
       <c r="I126" s="1"/>
       <c r="J126" s="1"/>
     </row>
-    <row r="127" spans="1:10">
+    <row r="127" spans="1:10" hidden="1">
       <c r="A127" s="4" t="s">
         <v>209</v>
       </c>
@@ -16331,7 +16561,7 @@
       <c r="I127" s="1"/>
       <c r="J127" s="1"/>
     </row>
-    <row r="128" spans="1:10">
+    <row r="128" spans="1:10" hidden="1">
       <c r="A128" s="4" t="s">
         <v>210</v>
       </c>
@@ -16348,7 +16578,7 @@
       <c r="I128" s="1"/>
       <c r="J128" s="1"/>
     </row>
-    <row r="129" spans="1:10">
+    <row r="129" spans="1:10" hidden="1">
       <c r="A129" s="4" t="s">
         <v>211</v>
       </c>

</xml_diff>